<commit_message>
Bij M16 is Jira ook van toepassing bij applicatiebeheer en niet alleen bij DevOps. Closes #687.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -595,8 +595,8 @@
 13. Toegankelijkheid: Axe,
 14. Software bill of materials: tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,
 15. Artifact repository: Nexus of Harbor,
-16. Bij een DevOps werkwijze: Uitrollen in de productieomgeving: Ansible, en
-17. Bij een DevOps werkwijze: Registratie van incidenten bij gebruik en beheer: Jira.
+16. Registratie van incidenten bij gebruik en beheer: Jira,
+17. Bij een DevOps werkwijze; uitrollen in de productieomgeving: Ansible.
 Rationale
 Projecten hebben een redelijke vrijheid bij het kiezen en gebruiken van tools, maar voor een aantal taken is het gebruik verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van de Kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren; daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af. Tot slot is het gebruik in een aantal gevallen, ten behoeve van informatiebeveiliging bij de overheid, verplicht.
 </t>
@@ -894,7 +894,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 3.0.1, 31-03-2023.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 3.0.1, 03-04-2023.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
@@ -1194,10 +1194,10 @@
     <t>15. Artifact repository: Nexus of Harbor,</t>
   </si>
   <si>
-    <t>16. Bij een DevOps werkwijze: Uitrollen in de productieomgeving: Ansible, en</t>
-  </si>
-  <si>
-    <t>17. Bij een DevOps werkwijze: Registratie van incidenten bij gebruik en beheer: Jira.</t>
+    <t>16. Registratie van incidenten bij gebruik en beheer: Jira,</t>
+  </si>
+  <si>
+    <t>17. Bij een DevOps werkwijze; uitrollen in de productieomgeving: Ansible.</t>
   </si>
   <si>
     <t>M28</t>

</xml_diff>

<commit_message>
De titel van M02 is veranderd van 'Het project zorgt dat het product continu aan de kwaliteitsnormen voldoet' in 'Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet'. Continue aan alle kwaliteitsnormen voldoen is in de praktijk onmogelijk (zie ook M08 'Het project maakt technische schuld inzichtelijk en lost deze planmatig op'). Hiermee is de overlap met M06 'Het project meet kwaliteitsnormen geautomatiseerd en frequent' zo groot dat deze laatste maatregel is komen te vervallen. Closes #688.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -230,10 +230,10 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M02: Het project zorgt dat het product continu aan de kwaliteitsnormen voldoet
-Producten voldoen zo snel mogelijk vanaf de start van een project aan de door het project en ICTU vastgestelde kwaliteitsnormen en blijven daar zo veel mogelijk aan voldoen. De kwaliteit van producten, die nog niet zijn afgerond of nog niet aan de normen voldoen, wordt door het project bewaakt. Het voldoen aan de kwaliteitsnormen is onderdeel van de Definition of Done en herstel van de kwaliteit wordt planmatig opgepakt.
+          <t xml:space="preserve">M02: Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet
+Projecten bewaken zo snel mogelijk vanaf de start de door het project en ICTU vastgestelde kwaliteitsnormen en voldoen daar zo snel en goed mogelijk aan. De kwaliteit van producten, die nog niet zijn afgerond of nog niet aan de normen voldoen, wordt door het project bewaakt. Het voldoen aan de kwaliteitsnormen is onderdeel van de Definition of Done en herstel van de kwaliteit wordt planmatig opgepakt.
 De kwaliteitsnormen voor het project zijn beschreven in de niet-functionele eisen, het informatiebeveiligingsplan, het kwaliteitsplan en deze Kwaliteitsaanpak, zie M01: Het project levert in elke fase vastgestelde producten en informatie op.
-Om te zorgen dat het product continu aan de kwaliteitsnormen voldoet, voert het project de volgende activiteiten uit:
+Om continu te bewaken dat het product aan de kwaliteitsnormen voldoet, voert het project de volgende activiteiten uit:
 1. Tijdens de voorfase: het project reviewt de deliverables periodiek.
 2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software.
 3. Bij toepassing van DevOps tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.
@@ -245,7 +245,7 @@
 Tijdens de voorfase wordt het voldoen aan de kwaliteitsnormen met behulp van reviews gecontroleerd, normaal gesproken elke sprint. Als onderdeel van het op te stellen kwaliteitsplan wordt tijdens de voorfase bepaald hoe het project de kwaliteit tijdens realisatie gaat controleren; voor producten die niet geautomatiseerd kunnen worden gecontroleerd, beschrijft het kwaliteitsplan een alternatieve aanpak. Als bijvoorbeeld door de gekozen technologie geen ondersteuning van het kwaliteitssysteem mogelijk is, kunnen periodieke, handmatige controles als alternatief ingezet worden.
 Realisatiefase: geautomatiseerde kwaliteitsmeting
 Tijdens de realisatiefase wordt de kwaliteit diverse malen per uur gemeten door Quality-time, een door ICTU ontwikkeld, open source, geautomatiseerd kwaliteitssysteem. De kwaliteitsmanager configureert de kwaliteitsrapportage in Quality-time en past waar nodig de normen aan, op basis van de projectspecifieke kwaliteitseisen.
-Het Scrumteam kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie, indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het Scrumteam.
+Het Scrumteam kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie, indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het Scrumteam tijdens de daily scrum en/of tijdens het projectoverleg.
 Realisatiefase DevOps: geautomatiseerde monitoring
 Bij een DevOps-werkwijze monitort en test het project continue het gedrag van de software in gebruik en beheer. Hiertoe gebruikt het project operationele monitoringsoftware, bijvoorbeeld Nagios en/of Zabbix.
 Realisatiefase: handmatige evaluatie
@@ -258,7 +258,7 @@
 - Indien dat niet tot resultaat leidt, escaleert de kwaliteitsmanager de situatie naar de projectleider.
 - Indien dat ook niet tot resultaat leidt, escaleert de kwaliteitsmanager de situatie naar het hoofd van de afdeling ICTU Software Expertise (ISE).
 Rationale
-Het zo snel mogelijk en continu voldoen aan de kwaliteitsnormen beperkt toekomstige hersteltijd. Het dwingt tevens een systematische kwaliteitscontrole af.
+Vaak de kwaliteitsnormen bewaken maakt een actueel inzicht mogelijk. Projectleden kunnen snel reageren op afwijkingen, die in de regel ook pas recent zijn ontstaan en dus meestal gerelateerd zijn aan huidige activiteiten. Met name afwijkingen van de normen op het vlak van informatiebeveiliging en onderhoudbaarheid komen zo snel aan het licht en kunnen dan ook snel worden beoordeeld en - indien nodig en mogelijk - opgelost.
 </t>
         </r>
       </text>
@@ -517,24 +517,6 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M06: Het project meet kwaliteitsnormen geautomatiseerd en frequent
-Het voldoen aan de kwaliteitsnormen die geautomatiseerd gemeten kunnen worden, wordt frequent en minimaal één keer per dag gemeten.
-ICTU faciliteert dit met mensen en middelen. Quality-time, het kwaliteitssysteem van ICTU meet het voldoen aan de normen meermaals per uur. De daaruit voortvloeiende kwaliteitsrapportage wordt besproken tijdens de daily scrum en/of tijdens het projectoverleg.
-Rationale
-Vaak meten maakt een vrijwel actueel inzicht op elk moment mogelijk. Projectleden kunnen snel reageren op afwijkingen, die in de regel ook pas recent zijn ontstaan en dus meestal gerelateerd zijn aan huidige activiteiten. Met name afwijkingen van de normen op het vlak van informatiebeveiliging en onderhoudbaarheid komen zo snel aan het licht en kunnen dan ook snel worden beoordeeld en - indien nodig en mogelijk - opgelost.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B64" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">M10: Het project kent een wekelijks projectoverleg
 De projectleider organiseert een periodiek projectoverleg. Dit overleg vindt wekelijks plaats en duurt niet langer dan een uur. Vereiste aanwezigen zijn de projectleider, de software delivery manager, de Scrummaster, een vertegenwoordiger uit elk van de Scrumteams en de kwaliteitsmanager van het project; andere aanwezigen kunnen zijn: de projectarchitect en de product owner. De agenda voor dit overleg bestaat ten minste uit de volgende onderwerpen: mededelingen, actie- en besluitenlijst, personele zaken, planning en voortgang, kwaliteit en architectuur, risico's en aandachtspunten.
 Het periodiek projectoverleg heet bij ICTU het "Intern Projectoverleg" of "IPO".
@@ -552,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B65" authorId="0">
+    <comment ref="B64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -603,7 +585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C65" authorId="0">
+    <comment ref="C64" authorId="0">
       <text>
         <r>
           <rPr>
@@ -616,7 +598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -643,7 +625,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -661,7 +643,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -693,7 +675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C85" authorId="0">
+    <comment ref="C84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -706,7 +688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0">
+    <comment ref="B99" authorId="0">
       <text>
         <r>
           <rPr>
@@ -726,7 +708,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B102" authorId="0">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -745,7 +727,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -764,7 +746,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -785,7 +767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -804,7 +786,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -822,7 +804,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -853,9 +835,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
-  <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 3.1.0-dev, 06-06-2023.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
+  <si>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 4.0.0-dev, 06-06-2023.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
@@ -966,7 +948,7 @@
     <t>M02</t>
   </si>
   <si>
-    <t>Het project zorgt dat het product continu aan de kwaliteitsnormen voldoet</t>
+    <t>Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet</t>
   </si>
   <si>
     <t>1. Tijdens de voorfase: het project reviewt de deliverables periodiek.</t>
@@ -1090,12 +1072,6 @@
   </si>
   <si>
     <t>4. Product backlog en sprint backlog.</t>
-  </si>
-  <si>
-    <t>M06</t>
-  </si>
-  <si>
-    <t>Het project meet kwaliteitsnormen geautomatiseerd en frequent</t>
   </si>
   <si>
     <t>M10</t>
@@ -1703,7 +1679,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2265,23 +2241,21 @@
       <c r="B64" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="7"/>
+      <c r="C64" s="3"/>
       <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="3" t="s">
+      <c r="A65" s="5"/>
+      <c r="B65" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C65" s="3"/>
+      <c r="C65" s="6"/>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="4"/>
@@ -2289,7 +2263,7 @@
     <row r="67" spans="1:4">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="4"/>
@@ -2297,7 +2271,7 @@
     <row r="68" spans="1:4">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="4"/>
@@ -2305,7 +2279,7 @@
     <row r="69" spans="1:4">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="4"/>
@@ -2313,7 +2287,7 @@
     <row r="70" spans="1:4">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" s="4"/>
@@ -2321,7 +2295,7 @@
     <row r="71" spans="1:4">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="4"/>
@@ -2329,7 +2303,7 @@
     <row r="72" spans="1:4">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="4"/>
@@ -2337,7 +2311,7 @@
     <row r="73" spans="1:4">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="4"/>
@@ -2345,7 +2319,7 @@
     <row r="74" spans="1:4">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="4"/>
@@ -2353,7 +2327,7 @@
     <row r="75" spans="1:4">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="4"/>
@@ -2361,7 +2335,7 @@
     <row r="76" spans="1:4">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="4"/>
@@ -2369,7 +2343,7 @@
     <row r="77" spans="1:4">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="4"/>
@@ -2377,7 +2351,7 @@
     <row r="78" spans="1:4">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="4"/>
@@ -2385,7 +2359,7 @@
     <row r="79" spans="1:4">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="4"/>
@@ -2393,7 +2367,7 @@
     <row r="80" spans="1:4">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="4"/>
@@ -2401,17 +2375,19 @@
     <row r="81" spans="1:4">
       <c r="A81" s="5"/>
       <c r="B81" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="5"/>
-      <c r="B82" s="5" t="s">
+      <c r="A82" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B82" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="C82" s="6"/>
+      <c r="C82" s="7"/>
       <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4">
@@ -2431,23 +2407,21 @@
       <c r="B84" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C84" s="7"/>
+      <c r="C84" s="3"/>
       <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="5"/>
+      <c r="B85" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B85" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="C85" s="3"/>
+      <c r="C85" s="6"/>
       <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="5"/>
       <c r="B86" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="4"/>
@@ -2455,7 +2429,7 @@
     <row r="87" spans="1:4">
       <c r="A87" s="5"/>
       <c r="B87" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="4"/>
@@ -2463,7 +2437,7 @@
     <row r="88" spans="1:4">
       <c r="A88" s="5"/>
       <c r="B88" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="4"/>
@@ -2471,7 +2445,7 @@
     <row r="89" spans="1:4">
       <c r="A89" s="5"/>
       <c r="B89" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="4"/>
@@ -2479,7 +2453,7 @@
     <row r="90" spans="1:4">
       <c r="A90" s="5"/>
       <c r="B90" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="4"/>
@@ -2487,7 +2461,7 @@
     <row r="91" spans="1:4">
       <c r="A91" s="5"/>
       <c r="B91" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="4"/>
@@ -2495,7 +2469,7 @@
     <row r="92" spans="1:4">
       <c r="A92" s="5"/>
       <c r="B92" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="4"/>
@@ -2503,7 +2477,7 @@
     <row r="93" spans="1:4">
       <c r="A93" s="5"/>
       <c r="B93" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="4"/>
@@ -2511,7 +2485,7 @@
     <row r="94" spans="1:4">
       <c r="A94" s="5"/>
       <c r="B94" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="4"/>
@@ -2519,7 +2493,7 @@
     <row r="95" spans="1:4">
       <c r="A95" s="5"/>
       <c r="B95" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95" s="4"/>
@@ -2527,7 +2501,7 @@
     <row r="96" spans="1:4">
       <c r="A96" s="5"/>
       <c r="B96" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C96" s="6"/>
       <c r="D96" s="4"/>
@@ -2535,7 +2509,7 @@
     <row r="97" spans="1:4">
       <c r="A97" s="5"/>
       <c r="B97" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C97" s="6"/>
       <c r="D97" s="4"/>
@@ -2543,36 +2517,38 @@
     <row r="98" spans="1:4">
       <c r="A98" s="5"/>
       <c r="B98" s="5" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C98" s="6"/>
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="5"/>
-      <c r="B99" s="5" t="s">
+      <c r="A99" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="6"/>
+      <c r="C99" s="7"/>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B100" s="3" t="s">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="4"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1" t="s">
+      <c r="B101" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="4"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
@@ -2623,16 +2599,6 @@
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="4"/>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B107" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C107" s="7"/>
-      <c r="D107" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2642,7 +2608,7 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A101:D101"/>
+    <mergeCell ref="A100:D100"/>
   </mergeCells>
   <conditionalFormatting sqref="C10">
     <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
@@ -2658,7 +2624,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
+  <conditionalFormatting sqref="C101">
     <cfRule type="cellIs" dxfId="0" priority="337" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2742,20 +2708,6 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="362" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="363" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="364" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C12">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3414,7 +3366,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
+  <conditionalFormatting sqref="C65">
     <cfRule type="cellIs" dxfId="0" priority="201" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3694,7 +3646,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="277" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3918,7 +3870,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="91">
+  <dataValidations count="90">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4069,7 +4021,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C63">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C65">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C66">
@@ -4126,7 +4078,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
@@ -4171,7 +4123,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C99">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
@@ -4187,9 +4139,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C106">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4214,7 +4163,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4222,10 +4171,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Maatregel M35 "Het project hanteert een agile architectuuraanpak" toegevoegd. Templates aangepast aan nieuwe maatregel. Closes #735.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -37,7 +37,7 @@
 3. Privacy impact assessment.
 Als de benodigde informatie niet gereed is bij de start van de voorfase dan maken opdrachtgever en ICTU nadere afspraken over de manier waarop de benodigde informatie nog tijdens de voorfase beschikbaar komt voor het project.
 Projectstartarchitectuur
-Een projectstartarchitectuur (PSA) is bedoeld om te borgen dat nieuwe ontwikkelingen en veranderingen in samenhang worden gerealiseerd en passen binnen de toekomstig gewenste informatievoorziening. Een PSA bevat in ieder geval de volgende onderwerpen:
+Een projectstartarchitectuur (PSA) is bedoeld om te borgen dat nieuwe ontwikkelingen en veranderingen in samenhang worden gerealiseerd en passen binnen de toekomstig gewenste informatievoorziening. De PSA is een concreet en doelgericht ICT-architectuurkader waarbinnen het project moet worden uitgevoerd. In de PSA zijn de architectuurvisie, enterprise-architectuur en overige architecturen van de opdrachtgever vertaald naar aan het product te stellen eisen. Een PSA bevat in ieder geval de volgende onderwerpen:
 - Een beschrijving van de doelen en ambities waaraan het project bijdraagt en invulling geeft. Dus niet de projectdoelen en -ambitie.
 - Een afbakening van het project en de context van de voorziening/oplossing die het project gaat realiseren. De PSA beschrijft niet de implementatie van de voorziening zelf (dit blijft een 'black box'), maar wel het gewenste gedrag in het grotere geheel. Denk o.a. ook aan relaties met andere projecten en generieke en specifieke diensten (services).
 - De belangrijkste functies van de door het project te realiseren voorziening, informatiestromen en koppelvlakken.
@@ -517,6 +517,27 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
+          <t xml:space="preserve">M35: Het project hanteert een agile architectuuraanpak
+Tijdens de voorfase verwerkt het project de door de opdrachtgever opgestelde projectstartarchitectuur (PSA) in een eerste versie van het softwarearchitectuurdocument (SAD). Tijdens de realisatiefase werkt het project het SAD bij op basis van nieuwe inzichten.
+Ten behoeve van de agile architectuuraanpak werkt het Scrumteam nauw samen met de architecten van de opdrachtgever en de beheerorganisatie, zowel in de voorfase als tijdens de realisatiefase.
+Tijdens de voorfase schrijft de softwarearchitect (het teamlid met de rol van architect) het SAD, inclusief genomen ontwerpbeslissingen.
+Tijdens de realisatiefase ondersteunt de softwareachitect het team bij het realiseren van de software conform het SAD. Daarbij kunnen nieuwe inzichten ontstaan die van invloed zijn op het SAD, bijvoorbeeld dat gekozen technologie niet voldoet of dat benodigde brondata niet eenvoudig ontsluitbaar is.
+De softwarearchitect informeert de opdrachtgever en de beheerorganisatie over deze nieuwe inzichten en stemt de gevolgen hiervan af. Deze nieuwe inzichten kunnen voor de opdrachtgever en de beheerorganisatie aanleiding zijn om hun architectuur aan te passen.
+Rationale
+Maatwerksoftwareontwikkeling is per definitie het ontwikkelen van een nieuw product. In de praktijk blijkt dat tijdens de ontwikkeling van het product altijd nog zaken ontdekt worden die bij aanvang niet bekend waren, of waarvan het belang eerder niet op waarde werd geschat. Het initiële SAD zal dus in de praktijk altijd moeten worden bijgewerkt op basis van die nieuwe inzichten.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B64" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Courier"/>
+            <family val="2"/>
+          </rPr>
           <t xml:space="preserve">M10: Het project kent een wekelijks projectoverleg
 De projectleider organiseert een periodiek projectoverleg. Dit overleg vindt wekelijks plaats en duurt niet langer dan een uur. Vereiste aanwezigen zijn de projectleider, de software delivery manager, de Scrummaster, een vertegenwoordiger uit elk van de Scrumteams en de kwaliteitsmanager van het project; andere aanwezigen kunnen zijn: de projectarchitect en de product owner. De agenda voor dit overleg bestaat ten minste uit de volgende onderwerpen: mededelingen, actie- en besluitenlijst, personele zaken, planning en voortgang, kwaliteit en architectuur, risico's en aandachtspunten.
 Het periodiek projectoverleg heet bij ICTU het "Intern Projectoverleg" of "IPO".
@@ -534,7 +555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B64" authorId="0">
+    <comment ref="B65" authorId="0">
       <text>
         <r>
           <rPr>
@@ -585,7 +606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C64" authorId="0">
+    <comment ref="C65" authorId="0">
       <text>
         <r>
           <rPr>
@@ -598,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -625,7 +646,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -643,7 +664,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -675,7 +696,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C84" authorId="0">
+    <comment ref="C85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -688,7 +709,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B99" authorId="0">
+    <comment ref="B100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -708,7 +729,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B101" authorId="0">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -727,7 +748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B102" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -746,7 +767,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +788,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -786,7 +807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -804,7 +825,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -835,7 +856,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 4.0.0-dev, 06-06-2023.</t>
   </si>
@@ -1072,6 +1093,12 @@
   </si>
   <si>
     <t>4. Product backlog en sprint backlog.</t>
+  </si>
+  <si>
+    <t>M35</t>
+  </si>
+  <si>
+    <t>Het project hanteert een agile architectuuraanpak</t>
   </si>
   <si>
     <t>M10</t>
@@ -1679,7 +1706,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2241,21 +2268,23 @@
       <c r="B64" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C64" s="3"/>
+      <c r="C64" s="7"/>
       <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="5"/>
-      <c r="B65" s="5" t="s">
+      <c r="A65" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C65" s="6"/>
+      <c r="B65" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C65" s="3"/>
       <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="5"/>
       <c r="B66" s="5" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="4"/>
@@ -2263,7 +2292,7 @@
     <row r="67" spans="1:4">
       <c r="A67" s="5"/>
       <c r="B67" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="4"/>
@@ -2271,7 +2300,7 @@
     <row r="68" spans="1:4">
       <c r="A68" s="5"/>
       <c r="B68" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="4"/>
@@ -2279,7 +2308,7 @@
     <row r="69" spans="1:4">
       <c r="A69" s="5"/>
       <c r="B69" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C69" s="6"/>
       <c r="D69" s="4"/>
@@ -2287,7 +2316,7 @@
     <row r="70" spans="1:4">
       <c r="A70" s="5"/>
       <c r="B70" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" s="4"/>
@@ -2295,7 +2324,7 @@
     <row r="71" spans="1:4">
       <c r="A71" s="5"/>
       <c r="B71" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="4"/>
@@ -2303,7 +2332,7 @@
     <row r="72" spans="1:4">
       <c r="A72" s="5"/>
       <c r="B72" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C72" s="6"/>
       <c r="D72" s="4"/>
@@ -2311,7 +2340,7 @@
     <row r="73" spans="1:4">
       <c r="A73" s="5"/>
       <c r="B73" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C73" s="6"/>
       <c r="D73" s="4"/>
@@ -2319,7 +2348,7 @@
     <row r="74" spans="1:4">
       <c r="A74" s="5"/>
       <c r="B74" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="4"/>
@@ -2327,7 +2356,7 @@
     <row r="75" spans="1:4">
       <c r="A75" s="5"/>
       <c r="B75" s="5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="4"/>
@@ -2335,7 +2364,7 @@
     <row r="76" spans="1:4">
       <c r="A76" s="5"/>
       <c r="B76" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="4"/>
@@ -2343,7 +2372,7 @@
     <row r="77" spans="1:4">
       <c r="A77" s="5"/>
       <c r="B77" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="4"/>
@@ -2351,7 +2380,7 @@
     <row r="78" spans="1:4">
       <c r="A78" s="5"/>
       <c r="B78" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="4"/>
@@ -2359,7 +2388,7 @@
     <row r="79" spans="1:4">
       <c r="A79" s="5"/>
       <c r="B79" s="5" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C79" s="6"/>
       <c r="D79" s="4"/>
@@ -2367,7 +2396,7 @@
     <row r="80" spans="1:4">
       <c r="A80" s="5"/>
       <c r="B80" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="4"/>
@@ -2375,19 +2404,17 @@
     <row r="81" spans="1:4">
       <c r="A81" s="5"/>
       <c r="B81" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C81" s="6"/>
       <c r="D81" s="4"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B82" s="3" t="s">
+      <c r="A82" s="5"/>
+      <c r="B82" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C82" s="7"/>
+      <c r="C82" s="6"/>
       <c r="D82" s="4"/>
     </row>
     <row r="83" spans="1:4">
@@ -2407,21 +2434,23 @@
       <c r="B84" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C84" s="3"/>
+      <c r="C84" s="7"/>
       <c r="D84" s="4"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="5"/>
-      <c r="B85" s="5" t="s">
+      <c r="A85" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="C85" s="6"/>
+      <c r="B85" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C85" s="3"/>
       <c r="D85" s="4"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="5"/>
       <c r="B86" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C86" s="6"/>
       <c r="D86" s="4"/>
@@ -2429,7 +2458,7 @@
     <row r="87" spans="1:4">
       <c r="A87" s="5"/>
       <c r="B87" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C87" s="6"/>
       <c r="D87" s="4"/>
@@ -2437,7 +2466,7 @@
     <row r="88" spans="1:4">
       <c r="A88" s="5"/>
       <c r="B88" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C88" s="6"/>
       <c r="D88" s="4"/>
@@ -2445,7 +2474,7 @@
     <row r="89" spans="1:4">
       <c r="A89" s="5"/>
       <c r="B89" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C89" s="6"/>
       <c r="D89" s="4"/>
@@ -2453,7 +2482,7 @@
     <row r="90" spans="1:4">
       <c r="A90" s="5"/>
       <c r="B90" s="5" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C90" s="6"/>
       <c r="D90" s="4"/>
@@ -2461,7 +2490,7 @@
     <row r="91" spans="1:4">
       <c r="A91" s="5"/>
       <c r="B91" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C91" s="6"/>
       <c r="D91" s="4"/>
@@ -2469,7 +2498,7 @@
     <row r="92" spans="1:4">
       <c r="A92" s="5"/>
       <c r="B92" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C92" s="6"/>
       <c r="D92" s="4"/>
@@ -2477,7 +2506,7 @@
     <row r="93" spans="1:4">
       <c r="A93" s="5"/>
       <c r="B93" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C93" s="6"/>
       <c r="D93" s="4"/>
@@ -2485,7 +2514,7 @@
     <row r="94" spans="1:4">
       <c r="A94" s="5"/>
       <c r="B94" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="4"/>
@@ -2493,7 +2522,7 @@
     <row r="95" spans="1:4">
       <c r="A95" s="5"/>
       <c r="B95" s="5" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C95" s="6"/>
       <c r="D95" s="4"/>
@@ -2501,7 +2530,7 @@
     <row r="96" spans="1:4">
       <c r="A96" s="5"/>
       <c r="B96" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C96" s="6"/>
       <c r="D96" s="4"/>
@@ -2509,7 +2538,7 @@
     <row r="97" spans="1:4">
       <c r="A97" s="5"/>
       <c r="B97" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C97" s="6"/>
       <c r="D97" s="4"/>
@@ -2517,38 +2546,36 @@
     <row r="98" spans="1:4">
       <c r="A98" s="5"/>
       <c r="B98" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C98" s="6"/>
       <c r="D98" s="4"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B99" s="3" t="s">
+      <c r="A99" s="5"/>
+      <c r="B99" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="7"/>
+      <c r="C99" s="6"/>
       <c r="D99" s="4"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="1" t="s">
+      <c r="A100" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B100" s="1"/>
-      <c r="C100" s="1"/>
-      <c r="D100" s="1"/>
+      <c r="B100" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C100" s="7"/>
+      <c r="D100" s="4"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B101" s="3" t="s">
+      <c r="A101" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C101" s="7"/>
-      <c r="D101" s="4"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
@@ -2599,6 +2626,16 @@
       </c>
       <c r="C106" s="7"/>
       <c r="D106" s="4"/>
+    </row>
+    <row r="107" spans="1:4">
+      <c r="A107" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B107" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C107" s="7"/>
+      <c r="D107" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2608,7 +2645,7 @@
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="A6:D6"/>
     <mergeCell ref="A54:D54"/>
-    <mergeCell ref="A100:D100"/>
+    <mergeCell ref="A101:D101"/>
   </mergeCells>
   <conditionalFormatting sqref="C10">
     <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
@@ -2624,7 +2661,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
+  <conditionalFormatting sqref="C100">
     <cfRule type="cellIs" dxfId="0" priority="337" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2708,6 +2745,20 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C107">
+    <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="362" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="363" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="364" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C12">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3366,7 +3417,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
+  <conditionalFormatting sqref="C64">
     <cfRule type="cellIs" dxfId="0" priority="201" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3646,7 +3697,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C84">
     <cfRule type="cellIs" dxfId="0" priority="277" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3870,7 +3921,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="90">
+  <dataValidations count="91">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4021,7 +4072,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C63">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C65">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C64">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C66">
@@ -4078,7 +4129,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
@@ -4123,7 +4174,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C99">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
@@ -4139,6 +4190,9 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C106">
+      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4163,7 +4217,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4171,10 +4225,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
De scope van maatregel M29 "ICTU zorgt dat een project verantwoord kan starten" gereduceerd tot het organiseren van de interne dienstverlening voor aanvang van een project en de titel hieraan aangepast: "ICTU organiseert voor aanvang van een project de interne dienstverlening". Closes #734.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -84,7 +84,7 @@
           </rPr>
           <t xml:space="preserve">M01: Het project levert in elke fase vastgestelde producten en informatie op
 Iedere projectfase levert specifieke informatie op. De voorfase levert inzicht in de functionele en niet-functionele eisen, ontwerp en architectuur, testplannen, operationele risico's, en benodigde kwaliteitsmaatregelen. Deze informatie wordt tijdens de realisatiefase waar nodig bijgewerkt. De realisatiefase levert één of meerdere werkende versies van de software met regressietests, aangevuld met een vrijgaveadvies, release notes en installatiedocumentatie.
-Opdrachtgever, ICTU, beheerpartij en andere meewerkende partijen leveren de onderstaande informatie op. Voor een aantal documenten zijn als onderdeel van de Kwaliteitsaanpak templates beschikbaar. Ook kan gebruik worden gemaakt van bestaande templates uit bijvoorbeeld de NORA. Zie M29: ICTU zorgt dat een project verantwoord kan starten.
+Opdrachtgever, ICTU, beheerpartij en andere meewerkende partijen leveren de onderstaande informatie op. Voor een aantal documenten zijn als onderdeel van de Kwaliteitsaanpak templates beschikbaar. Ook kan gebruik worden gemaakt van bestaande templates uit bijvoorbeeld de NORA. Zie M29: ICTU organiseert voor aanvang van een project de interne dienstverlening.
 De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het ✔ geeft aan in welke fase ze worden opgeleverd.
 Product                                                                     Voor start Voorfase Realisatiefase 
 Plan van aanpak: voorfase                                                   x                                  
@@ -735,51 +735,12 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M29: ICTU zorgt dat een project verantwoord kan starten
-Voordat een softwareontwikkelproject, dat conform de Kwaliteitsaanpak gaat werken, start, toetst ICTU of het project gebaseerd is op een adequaat projectvoorstel en of zij beschikt over de benodigde kennis, diensten en hulpmiddelen om het project te ondersteunen. Zo niet, dan voert de organisatie ofwel het project niet uit, ofwel past zij het projectvoorstel aan en/of organiseert zij de benodigde kennis, diensten en hulpmiddelen.
-Voordat ICTU een project verantwoord kan starten en het door de afdeling ICTU Software Diensten (ISD) ondersteund kan worden, moet aan een aantal randvoorwaarden zijn voldaan:
-1. Het project ontwikkelt en/of onderhoudt maatwerksoftware volgens deze Kwaliteitsaanpak.
-2. De opdrachtgever heeft kennisgenomen van en committeert zich aan de Kwaliteitsaanpak.
-3. Er is adequaat projectmanagement en -governance ingericht, zowel aan opdrachtgeverszijde als aan ICTU-zijde.
-4. De omvang, de snelheid van opschaling, en de behoefte aan ondersteuning van het project is zodanig dat dit samengaat met ongestoorde dienstverlening aan de lopende projecten.
-5. Er is een ICTU-projectleider verantwoordelijk voor projectuitvoering, projectresultaat en de geleverde kwaliteit.
-6. De projectleider en andere projectmedewerkers met projectmanagementverantwoordelijkheid hebben kennis van en ervaring met de Kwaliteitsaanpak en het ecosysteem.
-7. Het project zet een kwaliteitsmanager in met kennis van en ervaring met de Kwaliteitsaanpak en het ecosysteem.
-8. Het project doorloopt voorfase en realisatiefase volgens de Kwaliteitsaanpak.
-9. De dienstverlening met betrekking tot het ecosysteem is afgestemd tussen project en de afdeling ISD en is onderdeel van het aanbod van ICTU aan de opdrachtgever.
-Voorafgaand aan de start van een project organiseert ICTU in de regel een "Doordacht-van-Start-sessie", waarin aandacht besteed wordt aan de bovengenoemde punten.
-Projectvoorstellen van ICTU voor projecten die door ISD worden ondersteund, hebben ten minste de onderstaande stappen doorlopen. N.B: Input voor een projectvoorstel bestaat niet alleen uit schriftelijke communicatie, maar ook uit gesprekken met opdrachtgever en andere belanghebbenden.
-1. De verwachtingen van de opdrachtgever met betrekking tot omvang, doorlooptijd en kosten zijn geïdentificeerd voordat het projectvoorstel wordt geschreven.
-2. De schattingen voor doorlooptijd en teambezetting zijn gebaseerd op een expertschatting en optioneel een functiepuntentelling.
-3. Zowel de afdeling Relatiemanagement als de afdeling ISD reviewen het projectvoorstel. ISD gebruikt hiervoor de onderstaande checklist.
-4. De relatiemanager en de beoogd projectleider en/of software delivery manager nemen het projectvoorstel mondeling door met de opdrachtgever.
-Een projectvoorstel bevat ten minste de volgende onderdelen:
-- een beknopte en heldere omschrijving van het doel van het project: welk probleem van de opdrachtgever lost het project op;
-- een beschrijving van het beoogde resultaat van het project;
-- een beschrijving van de deliverables van het project;
-- een beschrijving van de aanpak van het project;
-- een beschrijving van de planning van het project, inclusief doorlooptijd, aantal sprints, lengte van sprints, eventuele voorbereidingstijd, sprint 0, overdrachtsfase, en nazorg;
-- een beschrijving van de rollen in het project, door welke organisatie deze rollen worden ingevuld, hoeveel tijd dat kost en welke eisen aan competenties en/of ervaring worden gesteld;
-- een beschrijving van het projectmanagement en de governance op het project, inclusief opdrachtgever (organisatie, naam en functie) en product owner (organisatie, naam en functie) en overzicht rapportages;
-- een beschrijving van het kwaliteitsmanagement op het project;
-- een beschrijving van het risicomanagement op het project;
-- een schatting van de kosten van het project;
-- een beschrijving van de randvoorwaarden en aannames die onder het plan liggen;
-- een beschrijving van de belangrijkste risico's voor het projectresultaat;
-- een beschrijving van relaties en/of afhankelijkheden met andere projecten door ICTU voor deze opdrachtgever, dan wel voor andere opdrachtgevers, dan wel andere projecten bij de opdrachtgever die niet door ICTU worden uitgevoerd;
-- een beschrijving van de belanghebbenden en hun belangen bij het project. Mogelijke belanghebbenden zijn bijvoorbeeld eindgebruikers, burgers, afdelingen bij de opdrachtgever, ketenpartners, en beheerorganisaties;
-- relevante referenties;
-- een distributielijst;
-- een versienummer, datum, auteur, status;
-- een algemene beschrijving van ICTU.
-In het geval van een voorstel voor een voorfase, zijn de volgende aanvullende onderdelen opgenomen:
-- hoe, door wie, en wanneer wordt besloten over het vervolg op de voorfase,
-- of er mensen beschikbaar worden gehouden, en, zo ja, hoe lang, tussen voorfase en eventuele realisatiefase.
-In het geval van een voorstel voor een realisatiefase, zijn de volgende aanvullende onderdelen opgenomen:
-- een releaseplanning;
-- de data waarop de software voor het eerst naar een acceptatieomgeving wordt opgeleverd en het moment dat de software voor het eerst in productie gaat.
+          <t xml:space="preserve">M29: ICTU organiseert voor aanvang van een project de interne dienstverlening
+Voordat ICTU een softwareontwikkelproject start, dat gaat werken conform de Kwaliteitsaanpak, maakt de beoogde projectleider afspraken met de afdelingen ICTU Software Diensten (ISD) en ICTU Software Expertise (ISE) over de af te nemen dienstverlening.
+Voordat ICTU een project start en een overeenkomst sluit met de opdrachtgever maakt de beoogde projectleider afspraken met de afdeling ISD over de door ISD geleverde voorzieningen die het project gaat afnemen en met de afdeling ISE over de medewerkers van de afdeling ISE die het project gaat inzetten.
+Hierbij bewaken ISD en ISE dat de omvang, de snelheid van opschaling, en de behoefte aan ondersteuning van het project zodanig is dat dit samengaat met ongestoorde dienstverlening aan de lopende projecten.
 Rationale
-Om de Kwaliteitsaanpak succesvol in te zetten, is ondersteuning van het project nodig. Het vooraf toetsen of deze ondersteuning in de juiste mate beschikbaar is, voorkomt dat projecten niet of niet goed volgens de Kwaliteitsaanpak kunnen werken.
+Door tijdig de interne dienstverlening aan projecten te organiseren helpt ICTU startende projecten de Kwaliteitsaanpak succesvol in te zetten, zonder de dienstverlening aan bestaande projecten te hinderen.
 </t>
         </r>
       </text>
@@ -894,7 +855,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 3.1.0-dev, 04-04-2023.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 3.1.0-dev, 06-06-2023.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
@@ -1272,7 +1233,7 @@
     <t>M29</t>
   </si>
   <si>
-    <t>ICTU zorgt dat een project verantwoord kan starten</t>
+    <t>ICTU organiseert voor aanvang van een project de interne dienstverlening</t>
   </si>
   <si>
     <t>M19</t>

</xml_diff>

<commit_message>
De term "DevOps-werkwijze" vervangen door "operationeel beheer" of door "operationeel en/of applicatiebeheer" op de plekken waar het gaat over de dienstverlening en niet zozeer over de aanpak. Closes #718.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -104,7 +104,7 @@
 Vrijgaveadvies                                                                                  x              
 Plan van aanpak
 Het plan van aanpak voor de voorfase en het plan van aanpak voor de realisatiefase beschrijven de in deze fasen te realiseren producten en diensten, en de planning, werkwijze en verantwoordelijkheden voor de totstandkoming van die producten en diensten.
-Bij een DevOps-werkwijze is de te leveren dienstverlening onderdeel van het plan van aanpak voor de realisatiefase. Het plan van aanpak voor de realisatiefase bevat dan de operationele beheerafspraken met de opdrachtgever en de beheerorganisatie. De afspraken omvatten zowel de te behalen kwaliteitsniveaus van de dienstverlening als de uit te voeren operationele beheertaken. Daarnaast beschrijft het plan hoe informatie zal worden verzameld over de software tijdens het gebruik en over de uitgevoerde beheeractiviteiten. En hoe hierover zal worden gerapporteerd. Ook worden de criteria voor het beëindigen van de dienstverlening vastgelegd. De te leveren dienstverlening is afgestemd op het beheerplan van de beheerorganisatie.
+Als operationeel en/of applicatiebeheer onderdeel is van de te leveren dienstverlening tijdens de realisatiefase bevat het plan van aanpak voor de realisatiefase de hiervoor noodzakelijke afspraken met de opdrachtgever en de beheerorganisatie. De afspraken omvatten zowel de te behalen kwaliteitsniveaus van de dienstverlening als de uit te voeren operationele en applicatiebeheertaken. Daarnaast beschrijft het plan hoe informatie zal worden verzameld over de software tijdens het gebruik en over de uitgevoerde beheeractiviteiten. En hoe hierover zal worden gerapporteerd. Ook worden de criteria voor het beëindigen van de dienstverlening vastgelegd. De te leveren dienstverlening is afgestemd op het beheerplan van de beheerorganisatie.
 Beschrijving van functionele eisen
 De beschrijving van functionele eisen bestaat uit epics en/of user stories, eventueel aangevuld met use cases. De beschrijving bevat tevens eisen voor ondersteuning van beheerfuncties, die door de beoogd beheerder gesteld worden, en voor logging, inclusief de globale inhoud van te loggen business events (gebeurtenissen op procesniveau) en de daarvoor geldende bewaartermijnen.
 Bronnen van de opdrachtgever zoals de projectstartarchitectuur, een programma van eisen en procesbeschrijvingen vormen het startpunt voor de functionele eisen. Tijdens het project worden use cases in samenwerking met de product owner vertaald naar epics en user stories.
@@ -236,7 +236,7 @@
 Om continu te bewaken dat het product aan de kwaliteitsnormen voldoet, voert het project de volgende activiteiten uit:
 1. Tijdens de voorfase: het project reviewt de deliverables periodiek.
 2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software.
-3. Bij toepassing van DevOps tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.
+3. Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.
 4. Tijdens de realisatiefase: het project evalueert periodiek en handmatig de kwaliteitseigenschappen van de software die niet geautomatiseerd kunnen worden gemeten.
 5. Tijdens de realisatiefase: het project actualiseert en reviewt periodiek de documentatie.
 6. Indien nodig: de kwaliteitsmanager escaleert het langdurig niet halen van de kwaliteitsnormen.
@@ -246,8 +246,8 @@
 Realisatiefase: geautomatiseerde kwaliteitsmeting
 Tijdens de realisatiefase wordt de kwaliteit diverse malen per uur gemeten door Quality-time, een door ICTU ontwikkeld, open source, geautomatiseerd kwaliteitssysteem. De kwaliteitsmanager configureert de kwaliteitsrapportage in Quality-time en past waar nodig de normen aan, op basis van de projectspecifieke kwaliteitseisen.
 Het Scrumteam kijkt dagelijks of er afwijkingen van de normen zijn en onderneemt actie, indien nodig. Ook de kwaliteitsmanager signaleert afwijkingen en meldt deze bij het Scrumteam tijdens de daily scrum en/of tijdens het projectoverleg.
-Realisatiefase DevOps: geautomatiseerde monitoring
-Bij een DevOps-werkwijze monitort en test het project continue het gedrag van de software in gebruik en beheer. Hiertoe gebruikt het project operationele monitoringsoftware, bijvoorbeeld Nagios en/of Zabbix.
+Realisatiefase operationeel beheer: geautomatiseerde monitoring
+Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase monitort en test het project continue het gedrag van de software in gebruik en beheer. Hiertoe gebruikt het project operationele monitoringsoftware, bijvoorbeeld Nagios en/of Zabbix.
 Realisatiefase: handmatige evaluatie
 Kwaliteitseigenschappen van de software die niet (volledig) geautomatiseerd kunnen worden gemeten, worden tijdens de realisatiefase periodiek handmatig geëvalueerd. Minimaal betreft dit de beveiliging van de software, zie M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen. Ook zorgt het project dat de performance van de software regelmatig wordt getest. Voor kwaliteitsaspecten als toegankelijkheid en gebruikskwaliteit organiseert het project handmatige testen en/of evaluaties in een vorm en met een frequentie die aansluit bij de aard van de applicatie en de door de opdrachtgever gestelde eisen. De kwaliteitsmanager houdt in Quality-time bij wanneer de laatste test of evaluatie is uitgevoerd en wanneer het tijd is voor de volgende.
 Realisatiefase: actualisering en review documentatie
@@ -488,7 +488,7 @@
 2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement,
 3. Definition of Ready en Definition of Done,
 4. Product backlog en sprint backlog.
-Bij een DevOps-werkwijze zijn deployment en operationeel beheer geïntegreerd in de Scrum-processen van het DevOps-team.
+Als operationeel beheer onderdeel is van de dienstverlening, past ICTU de DevOps-werkwijze toe door operationeel beheeractiviteiten te integreren in de Scrum-processen van het Scrumteam.
 Rationale
 De incrementele oplevering levert vrijwel iedere iteratie toegevoegde waarde en stelt opdrachtgevers, gebruikers en anderen in staat om gaandeweg ervaring op te doen en bij te sturen. Verder dwingt het vroegtijdige tests en kwaliteitscontroles af, die daarmee verankerd worden in het ontwikkel- en onderhoudsproces. Door naast de software telkens ook alle andere producten bij te werken en op te leveren, wordt bereikt dat het product als geheel consistent blijft en dat er geen achterstallig onderhoud ontstaat. Dit leidt tot een zich continu verbeterend proces.
 </t>
@@ -578,7 +578,7 @@
 14. Software bill of materials: tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,
 15. Artifact repository: Nexus of Harbor,
 16. Registratie van incidenten bij gebruik en beheer: Jira,
-17. Bij een DevOps werkwijze; uitrollen in de productieomgeving: Ansible.
+17. Bij het uitvoeren van operationeel beheer; uitrollen in de productieomgeving: Ansible.
 Rationale
 Projecten hebben een redelijke vrijheid bij het kiezen en gebruiken van tools, maar voor een aantal taken is het gebruik verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van de Kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren; daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af. Tot slot is het gebruik in een aantal gevallen, ten behoeve van informatiebeveiliging bij de overheid, verplicht.
 </t>
@@ -658,7 +658,7 @@
 Het project zorgt, bij voorkeur altijd maar in ieder geval bij de overdracht, dat de software, documentatie en testmiddelen aantoonbaar voldoen aan onderstaande criteria. Waar nodig scherpt het project, in afstemming met opdrachtgever en ontvangende partij, de criteria aan.
 1. De documentatie beschrijft de ontwikkel- en testomgeving die is toegepast (5.1),
 2. De functionele documentatie beschrijft gegevensmodellen, functionele indeling, koppelingen, berichtdefinities en workflows/processen (5.2),
-3. In het geval van DevOps: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),
+3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),
 4. De productbacklog bevat de bekende bugs en wensen (5.4),
 5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling (6.1),
 6. De broncode heeft een beperkte mate van duplicatie (6.2),
@@ -957,7 +957,7 @@
     <t>2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software.</t>
   </si>
   <si>
-    <t>3. Bij toepassing van DevOps tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.</t>
+    <t>3. Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.</t>
   </si>
   <si>
     <t>4. Tijdens de realisatiefase: het project evalueert periodiek en handmatig de kwaliteitseigenschappen van de software die niet geautomatiseerd kunnen worden gemeten.</t>
@@ -1134,7 +1134,7 @@
     <t>16. Registratie van incidenten bij gebruik en beheer: Jira,</t>
   </si>
   <si>
-    <t>17. Bij een DevOps werkwijze; uitrollen in de productieomgeving: Ansible.</t>
+    <t>17. Bij het uitvoeren van operationeel beheer; uitrollen in de productieomgeving: Ansible.</t>
   </si>
   <si>
     <t>M28</t>
@@ -1161,7 +1161,7 @@
     <t>2. De functionele documentatie beschrijft gegevensmodellen, functionele indeling, koppelingen, berichtdefinities en workflows/processen (5.2),</t>
   </si>
   <si>
-    <t>3. In het geval van DevOps: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),</t>
+    <t>3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),</t>
   </si>
   <si>
     <t>4. De productbacklog bevat de bekende bugs en wensen (5.4),</t>

</xml_diff>

<commit_message>
'Beheerorganisatie' en 'beheerpartij' werden door elkaar gebruikt. Alle voorkomens van beheerpartij vervangen door beheerorganisatie. Fixes #732.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -84,7 +84,7 @@
           </rPr>
           <t xml:space="preserve">M01: Het project levert in elke fase vastgestelde producten en informatie op
 Iedere projectfase levert specifieke informatie op. De voorfase levert inzicht in de functionele en niet-functionele eisen, ontwerp en architectuur, testplannen, operationele risico's, en benodigde kwaliteitsmaatregelen. Deze informatie wordt tijdens de realisatiefase waar nodig bijgewerkt. De realisatiefase levert één of meerdere werkende versies van de software met regressietests, aangevuld met een vrijgaveadvies, release notes en installatiedocumentatie.
-Opdrachtgever, ICTU, beheerpartij en andere meewerkende partijen leveren de onderstaande informatie op. Voor een aantal documenten zijn als onderdeel van de Kwaliteitsaanpak templates beschikbaar. Ook kan gebruik worden gemaakt van bestaande templates uit bijvoorbeeld de NORA. Zie M29: ICTU organiseert voor aanvang van een project de interne dienstverlening.
+Opdrachtgever, ICTU, beheerorganisatie en andere meewerkende partijen leveren de onderstaande informatie op. Voor een aantal documenten zijn als onderdeel van de Kwaliteitsaanpak templates beschikbaar. Ook kan gebruik worden gemaakt van bestaande templates uit bijvoorbeeld de NORA. Zie M29: ICTU organiseert voor aanvang van een project de interne dienstverlening.
 De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het ✔ geeft aan in welke fase ze worden opgeleverd.
 Product                                                                     Voor start Voorfase Realisatiefase 
 Plan van aanpak: voorfase                                                   x                                  
@@ -146,27 +146,27 @@
 Als er bijzondere of hoge niet-functionele eisen zijn, beschrijft het ICTU-kwaliteitsplan ook de extra projectspecifieke kwaliteitsmaatregelen die het project treft om deze eisen te realiseren.
 Als de opdrachtgever een overkoepelend kwaliteitsplan heeft zorgt het project dat het ICTU-kwaliteitsplan aansluit op het overkoepelende kwaliteitsplan.
 Deploybare versie van de software
-Het project levert deploybare versies van de software in een formaat dat is afgestemd met de beheerpartij.
+Het project levert deploybare versies van de software in een formaat dat is afgestemd met de beheerorganisatie.
 Documentatie voor deployment en operationeel beheer
 De deploymentdocumentatie bevat informatie over de eisen die een applicatie stelt aan een omgeving en de stappen die nodig zijn om de applicatie in die omgeving veilig te installeren en configureren. De documentatie bevat daartoe onder meer aanwijzingen voor de HTTP-header en -request-configuratie van de webserver en voor het verwijderen van overbodige header-informatie zoals de 'Server'-header. Ook zijn er aanwijzingen voor veilige configuratie(s) van (externe) toegang tot de beheerinterface. De documentatie bevat daarnaast in ieder geval een beschrijving van de protocollen en services die de applicatie aanbiedt, de protocollen, services en accounts die het product gebruikt en de protocollen, services en accounts die de applicatie gebruikt voor beheer.
 De documentatie voor operationeel beheer bevat tenminste informatie over: back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten, opstart- en afsluitprocedures.
 Software bill of materials
-Voor elke release stelt het project een "software bill of materials" op: een overzicht van de gebruikte libraries, frameworks, componenten en andere software(deel)producten in de release. Software draagt inherent het risico in zich van verborgen fouten. Deze fouten kunnen mogelijk misbruikt worden, waardoor (beveiligings)problemen ontstaan. Met dit overzicht heeft de opdrachtgever of diens beheerpartij informatie over de gebruikte software(deel)producten, die geraadpleegd kan worden wanneer fouten in software bekend wordt, zodat een risico-inschatting gemaakt kan worden en eventueel actie kan worden ondernomen.
+Voor elke release stelt het project een "software bill of materials" op: een overzicht van de gebruikte libraries, frameworks, componenten en andere software(deel)producten in de release. Software draagt inherent het risico in zich van verborgen fouten. Deze fouten kunnen mogelijk misbruikt worden, waardoor (beveiligings)problemen ontstaan. Met dit overzicht heeft de opdrachtgever of diens beheerorganisatie informatie over de gebruikte software(deel)producten, die geraadpleegd kan worden wanneer fouten in software bekend wordt, zodat een risico-inschatting gemaakt kan worden en eventueel actie kan worden ondernomen.
 Release notes
 Voor elke release stelt het project release notes op: een overzicht van de wijzigingen in de release. Software delivery manager en opdrachtgever maken afspraken over de opzet van de release notes.
 Vrijgaveadvies
 Voor elke release stelt het project een vrijgaveadvies op. Het vrijgaveadvies bevat tenminste alle nog openstaande testbevindingen en geconstateerde beveiligingsbevindingen; zie ook M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen en M16: Het project gebruikt tools voor vastgestelde taken. Als er issues zijn, bijvoorbeeld rondom kwaliteit of beveiliging, zijn deze voorzien van een beschrijving van de voorziene impact.
-Software delivery manager en opdrachtgever maken afspraken over de opzet van het vrijgaveadvies en de verantwoordelijkheden van betrokken partijen bij de totstandkoming ervan, waaronder ook de beheerpartij.
+Software delivery manager en opdrachtgever maken afspraken over de opzet van het vrijgaveadvies en de verantwoordelijkheden van betrokken partijen bij de totstandkoming ervan, waaronder ook de beheerorganisatie.
 Samenhang voorfaseproducten
 Bovenstaande figuur laat de belangrijkste relaties zien tussen de verschillende producten die de input en output van de voorfase vormen. Naast de informatiestromen zoals door de pijlen weergegeven zijn er in de praktijk nog meer verbanden tussen de producten. Zo kan de gekozen oplossing in de architectuur van invloed zijn op de maatregelen in het informatiebeveiligingsplan of leiden niet-functionele eisen tot extra functionele eisen.
 Verantwoordelijkheden
 De opdrachtgever is primair verantwoordelijk voor het beschrijven van de functionele en niet-functionele eisen, de geprioriteerde backlog, het mastertestplan en het informatiebeveiligingsplan.
 ICTU is primair verantwoordelijk voor plan van aanpak, softwarearchitectuurdocumentatie, globaal functioneel ontwerp, prototype, detailtestplannen en testrapportages voor bouwtesten, kwaliteitsplan, deploybare versie van de software, documentatie voor deployment en operationeel beheer, release notes en vrijgaveadvies.
 Als tijdens een project bestaande software dient te worden afgebouwd, onderhouden en/of herbouwd, vindt een onderzoek plaats naar de kwaliteit van deze software, zie M32: Het project onderzoekt de kwaliteit van over te nemen software. In dat geval levert het project ook de onderzoeksresultaten daarvan en maakt een transitieplan, en indien van toepassing, een plan voor het aflossen van technische schuld.
-De beheerpartij is primair verantwoordelijk voor de infrastructuurarchitectuur en -ontwerp en detailtestplannen en testrapportages voor infrastructuurtesten.
+De beheerorganisatie is primair verantwoordelijk voor de infrastructuurarchitectuur en -ontwerp en detailtestplannen en testrapportages voor infrastructuurtesten.
 Rationale
 Het uniformeren van op te leveren producten biedt voordelen voor planning (het is bekend welke producten gemaakt moeten worden), voor bemensing (het is bekend welke expertise nodig is) en voor het uitwisselen van medewerkers.
-De voorgeschreven producten stellen de beheerpartij in staat om de opgeleverde software uit te rollen, te beheren en eventueel te onderhouden. Daarnaast is duidelijk welke eventueel openstaande punten er nog zijn. De voorgeschreven producten bieden voldoende verantwoording richting de ontvanger voor uitgevoerde werkzaamheden.
+De voorgeschreven producten stellen de beheerorganisatie in staat om de opgeleverde software uit te rollen, te beheren en eventueel te onderhouden. Daarnaast is duidelijk welke eventueel openstaande punten er nog zijn. De voorgeschreven producten bieden voldoende verantwoording richting de ontvanger voor uitgevoerde werkzaamheden.
 De genoemde producten uit de voorfase hebben tot doel om enerzijds de omvang, kosten en doorlooptijd van de realisatiefase te kunnen schatten en anderzijds om de kaders voor de realisatiefase te bepalen, zodat de scope, aanpak en oplossingsrichting in grote lijnen bekend zijn.
 </t>
         </r>
@@ -356,7 +356,7 @@
 Performance- en beveiligingstests zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats.
 Niet alle testen en controles kunnen altijd geautomatiseerd worden uitgevoerd. Denk aan kwaliteitscontroles op architectuurbeslissingen of het testen van toegankelijkheidseisen. Waar mogelijk wordt wel een zo groot mogelijk deel van de testen en controles geautomatiseerd en als onderdeel van de pipeline uitgevoerd.
 De afdeling ICTU Software Diensten (ISD) voorziet in tools en ondersteuning, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
-ICTU gebruikt Jenkins, GitLab CI of Azure DevOps als tool voor de implementatie van de continuous delivery pipeline. ISD biedt de projecten een voorziening om releases van het totale product veilig op te leveren aan opdrachtgevers en beheerpartijen.
+ICTU gebruikt Jenkins, GitLab CI of Azure DevOps als tool voor de implementatie van de continuous delivery pipeline. ISD biedt de projecten een voorziening om releases van het totale product veilig op te leveren aan opdrachtgevers en beheerorganisaties.
 Rationale
 Software incrementeel opleveren vereist dat de software frequent gebouwd, getest en opgeleverd kan worden. Om dit efficiënt en foutvrij te doen, dient het proces van bouwen, testen en opleveren geautomatiseerd te zijn; een continuous delivery pipeline faciliteert dit.
 </t>
@@ -428,7 +428,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">M14: Het project bereidt samen met opdrachtgever en belanghebbenden de realisatie voor
-Projecten hebben een voorbereidingsfase, "voorfase" genoemd, voorafgaand aan de realisatiefase. Voor het uitvoeren van de voorfase zijn vertegenwoordigers van de opdrachtgever, de beoogde beheerpartij en andere belanghebbenden betrokken die meewerken aan het realiseren van een deel van de op te leveren producten. Het doel van de voorfase is beeld krijgen van de te realiseren oplossing, van de risico's die zich tijdens realisatie kunnen voordoen en van de kaders waarbinnen de oplossing moet passen; tijdens de realisatiefase vinden bouw en onderhoud van de software en actualiseren en afronden van documentatie plaats.
+Projecten hebben een voorbereidingsfase, "voorfase" genoemd, voorafgaand aan de realisatiefase. Voor het uitvoeren van de voorfase zijn vertegenwoordigers van de opdrachtgever, de beoogde beheerorganisatie en andere belanghebbenden betrokken die meewerken aan het realiseren van een deel van de op te leveren producten. Het doel van de voorfase is beeld krijgen van de te realiseren oplossing, van de risico's die zich tijdens realisatie kunnen voordoen en van de kaders waarbinnen de oplossing moet passen; tijdens de realisatiefase vinden bouw en onderhoud van de software en actualiseren en afronden van documentatie plaats.
 Bij voorkeur zijn dezelfde deskundigen in zowel de voorfase als in de realisatiefase betrokken.
 In de realisatiefase wordt de prioriteit van werk van het Scrumteam bepaald door een product owner van de opdrachtgever. Bij aanvang van de voorfase is deze beoogde product owner bekend en werkt deze ook mee in de voorfase.
 Rationale

</xml_diff>

<commit_message>
Add links to templates and other documents. Closes #745.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -111,6 +111,9 @@
 Plan van aanpak
 Het plan van aanpak voor de voorfase en het plan van aanpak voor de realisatiefase beschrijven de in deze fasen te realiseren producten en diensten, en de planning, werkwijze en verantwoordelijkheden voor de totstandkoming van die producten en diensten.
 Als operationeel en/of applicatiebeheer onderdeel is van de te leveren dienstverlening tijdens de realisatiefase bevat het plan van aanpak voor de realisatiefase de hiervoor noodzakelijke afspraken met de opdrachtgever en de beheerorganisatie. De afspraken omvatten zowel de te behalen kwaliteitsniveaus van de dienstverlening als de uit te voeren operationele en applicatiebeheertaken. Daarnaast beschrijft het plan hoe informatie zal worden verzameld over de software tijdens het gebruik en over de uitgevoerde beheeractiviteiten. En hoe hierover zal worden gerapporteerd. Ook worden de criteria voor het beëindigen van de dienstverlening vastgelegd. De te leveren dienstverlening is afgestemd op het beheerplan van de beheerorganisatie.
+Beschikbare templates:
+- Template plan van aanpak voorfase.
+- Template plan van aanpak realisatiefase.
 Beschrijving van functionele eisen
 De beschrijving van functionele eisen bestaat uit epics en/of user stories, eventueel aangevuld met use cases. De beschrijving bevat tevens eisen voor ondersteuning van beheerfuncties, die door de beoogd beheerder gesteld worden, en voor logging, inclusief de globale inhoud van te loggen business events (gebeurtenissen op procesniveau) en de daarvoor geldende bewaartermijnen.
 Bronnen van de opdrachtgever zoals de projectstartarchitectuur, een programma van eisen en procesbeschrijvingen vormen het startpunt voor de functionele eisen. Tijdens het project worden use cases in samenwerking met de product owner vertaald naar epics en user stories.
@@ -126,6 +129,8 @@
 De beschrijving van niet-functionele eisen moet expliciet aandacht besteden aan de door de beoogd beheerder gewenste ondersteuning van beheerfuncties. Bepaalde niet-functionele eisen kunnen aanleiding zijn tot het treffen van beveiligingsmaatregelen. Door deze eisen expliciet in de voorfase te benoemen, wordt voorkomen dat de bijbehorende beveiligingsmaatregelen achteraf moeten worden toegevoegd.
 Overheidsorganisaties moeten een toegankelijkheidsverklaring op hun websites plaatsen. Indien gewenst ondersteunt ICTU bij het opstellen van de toegankelijkheidsverklaring.
 Bronnen van de opdrachtgever zoals procesbeschrijvingen, privacy impact assessment (PIA), beheeracceptatiecriteria, beveiligingsbeleid en projectstartarchitectuur vormen het startpunt voor de niet-functionele eisen.
+Beschikbare templates:
+- Template niet-functionele eisen.
 Product backlog
 De product backlog is een geprioriteerd overzicht van alle nog te realiseren functionele en niet-functionele eigenschappen van de software. Al het werk dat het Scrumteam doet loopt via de backlog, niet alleen werk aan de broncode zelf maar bijvoorbeeld ook het schrijven van beheerdocumentatie. De product owner is de eigenaar van de product backlog. De zaken op de lijst zijn normaal gesproken in de vorm van een epic of user story. Hierin staat:
 - Wat er gemaakt moet worden,
@@ -139,10 +144,16 @@
 Het softwarearchitectuurdocument verschaft een compleet overzicht van de architectuur van de te ontwikkelen software, en de rationale hiervoor, waarbij diverse relevante views diverse aspecten van de software belichten. Zie bijvoorbeeld https://www.win.tue.nl/~wstomv/edu/2ip30/references/Kruchten-4+1-view.pdf; andere manieren van architectuurbeschrijving zijn ook toegestaan.
 De infrastructuurarchitectuur beschrijft de topologie van de implementatie-omgeving waaronder protocollen, beveiligingsniveaus en services. Deze architectuur biedt een logische afbeelding van de eisen naar de implementatie-omgeving en geeft onderbouwing voor de gemaakte keuzes.
 Een prototype is een eerste, ruwe versie van de applicatie. Het prototype illustreert waar men uiteindelijk met de toepassing naar toe wil. Het maakt ideeën tastbaar en creëert een eerste indruk van structuur, ontwerp en functionaliteit.
+Beschikbare templates:
+- Template globaal functioneel ontwerp.
+- Template softwarearchitectuurdocument.
+- Template infrastructuurarchitectuur.
 Testplannen en -rapportages
 De testplannen bestaan uit een mastertestplan (MTP), gemaakt op basis van een productrisicoanalyse (PRA), en detailtestplannen. Het doel van een mastertestplan is om betrokkenen bij het testproces te informeren over de strategie, aanpak, activiteiten, inclusief de onderlinge relaties en afhankelijkheden, en de op te leveren producten met betrekking tot het testtraject. Het mastertestplan beschrijft deze strategie, aanpak, activiteiten en eindproducten, die in de detailtestplannen verder worden gedetailleerd.
 Opdrachtgever is verantwoordelijk voor het mastertestplan. Het project maakt een detailtestplan voor de testsoorten die tijdens de realisatiefase door het project worden uitgevoerd. Voor testen die onder verantwoordelijkheid van het project door een derde partij worden uitgevoerd, denk aan penetratietesten en evaluaties van gebruikskwaliteit, worden aparte detailtestplannen gemaakt.
 Logische testgevallen worden vastgelegd en gekoppeld met use cases en user stories. Fysieke testgevallen worden vastgelegd in het formaat van de gebruikte tooling en gekoppeld met de logische testgevallen. Op basis hiervan worden testrapportages gegenereerd die laten zien dat alle use cases en user stories zijn getest en dat die tests zijn geslaagd.
+Beschikbare templates:
+- Template detailtestplan.
 Informatiebeveiligingsplan
 Het informatiebeveiligingsplan vormt een praktisch toepasbaar document dat uitlegt binnen welke kaders bescherming geleverd wordt tegen welke dreigingen en met welke maatregelen die bescherming vorm krijgt. Mogelijke bronnen voor het informatiebeveiligingsplan zijn de business impact analysis (BIA), privacy impact assessment (PIA) en de threat and vulnerability assessment (TVA).
 Het Besluit Voorschrift Informatiebeveiliging Rijksdienst 2007 (VIR 2007) bevat een methode om te komen tot een systematische aanpak van informatiebeveiliging. Eén van de vereisten van het VIR 2007 is dat voor elk informatiesysteem en voor elk verantwoordelijkheidsgebied een afhankelijkheids- en kwetsbaarheidsanalyse (A&amp;K-analyse) wordt uitgevoerd.
@@ -151,6 +162,8 @@
 Het ICTU-kwaliteitsplan beschrijft de standaard kwaliteitsmaatregelen die ICTU-projecten treffen om software te realiseren die voldoet aan de kwaliteitseisen van de opdrachtgever en andere belanghebbenden en aan de kwaliteitsnormen van ICTU.
 Als er bijzondere of hoge niet-functionele eisen zijn, beschrijft het ICTU-kwaliteitsplan ook de extra projectspecifieke kwaliteitsmaatregelen die het project treft om deze eisen te realiseren.
 Als de opdrachtgever een overkoepelend kwaliteitsplan heeft zorgt het project dat het ICTU-kwaliteitsplan aansluit op het overkoepelende kwaliteitsplan.
+Beschikbare templates:
+- Template kwaliteitsplan.
 Deploybare versie van de software
 Het project levert deploybare versies van de software in een formaat dat is afgestemd met de beheerorganisatie.
 Documentatie voor deployment en operationeel beheer
@@ -238,7 +251,7 @@
           </rPr>
           <t xml:space="preserve">M02: Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet
 Projecten bewaken zo snel mogelijk vanaf de start de door het project en ICTU vastgestelde kwaliteitsnormen en voldoen daar zo snel en goed mogelijk aan. De kwaliteit van producten, die nog niet zijn afgerond of nog niet aan de normen voldoen, wordt door het project bewaakt. Het voldoen aan de kwaliteitsnormen is onderdeel van de Definition of Done en herstel van de kwaliteit wordt planmatig opgepakt.
-De kwaliteitsnormen voor het project zijn beschreven in de niet-functionele eisen, het informatiebeveiligingsplan, het kwaliteitsplan en deze Kwaliteitsaanpak, zie M01: Het project levert in elke fase vastgestelde producten en informatie op.
+De kwaliteitsnormen voor het product zijn beschreven in de niet-functionele eisen, het informatiebeveiligingsplan, het kwaliteitsplan en deze Kwaliteitsaanpak, zie M01: Het project levert in elke fase vastgestelde producten en informatie op.
 Om continu te bewaken dat het product aan de kwaliteitsnormen voldoet, voert het project de volgende activiteiten uit:
 1. Tijdens de voorfase: het project reviewt de deliverables periodiek.
 2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software.
@@ -649,7 +662,7 @@
 - in geval van acceptatie; waarom het verschil geaccepteerd wordt,
 - in geval van verbeteractie; planning om het verschil weg te werken.
 De projectleider is verantwoordelijk voor het doen van de self-assessment, die in de regel door de software delivery manager wordt uitgevoerd. De kwaliteitsmanager reviewt de self-assessment, of de software delivery manager en kwaliteitsmanager voeren de self-assessment samen uit.
-De self-assessment is een intern product, maar kan gedeeld worden met opdrachtgevers en andere betrokkenen. Voor het doen van de self-assessment stelt ICTU een ondersteunend formulier beschikbaar.
+De self-assessment is een intern product, maar kan gedeeld worden met opdrachtgevers en andere betrokkenen. Voor het uitvoeren en vastleggen van de self-assessment stelt ICTU een self-assessment formulier beschikbaar.
 Rationale
 Net als bij technische producten is het periodiek meten van de kwaliteit van belang om in controle te blijven. Aangezien veel maatregelen uit de Kwaliteitsaanpak zich niet geautomatiseerd laten meten, is menselijke inbreng nodig.
 Omdat implementatie van maatregelen in een project tijd kost is de self-assessment gericht op het in kaart brengen van de belangrijkste verschillen tussen de Kwaliteitsaanpak en de in het project toegepaste werkwijze, maar niet op het uitputtend inventariseren van alle verschillen.
@@ -869,7 +882,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="143">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie 4.0.0-dev, 27-11-2023.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 30-11-2023.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>

</xml_diff>

<commit_message>
In maatregel M01 "Het project levert in elke fase vastgestelde producten en informatie op" verduidelijkt dat de aparte detailtestplannen die onder verantwoordelijkheid van het project door een derde partij worden uitgevoerd doorgaans de vorm hebben van een offerteaanvraag gemaakt door ICTU en een offerte met plan van aanpak gemaakt door de leverancier.
Closes #953.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -157,7 +157,7 @@
 - Template infrastructuurarchitectuur.
 Testplannen en -rapportages
 De testplannen bestaan uit een mastertestplan (MTP), gemaakt op basis van een productrisicoanalyse (PRA), en detailtestplannen. Het doel van een mastertestplan is om betrokkenen bij het testproces te informeren over de strategie, aanpak, activiteiten, inclusief de onderlinge relaties en afhankelijkheden, en de op te leveren producten met betrekking tot het testtraject. Het mastertestplan beschrijft deze strategie, aanpak, activiteiten en eindproducten, die in de detailtestplannen verder worden gedetailleerd.
-De opdrachtgevende organisatie is verantwoordelijk voor het mastertestplan. Het project maakt een detailtestplan voor de testsoorten die tijdens de realisatiefase door het project worden uitgevoerd. Voor testen die onder verantwoordelijkheid van het project door een derde partij worden uitgevoerd, denk aan penetratietesten en evaluaties van gebruikskwaliteit, worden aparte detailtestplannen gemaakt.
+De opdrachtgevende organisatie is verantwoordelijk voor het mastertestplan. Het project maakt een detailtestplan voor de testsoorten die tijdens de realisatiefase door het project worden uitgevoerd. Voor testen die onder verantwoordelijkheid van het project door een derde partij worden uitgevoerd, denk aan penetratietesten en evaluaties van gebruikskwaliteit, worden aparte detailtestplannen gemaakt. Deze hebben doorgaans de vorm van een offerteaanvraag gemaakt door ICTU en een offerte met plan van aanpak gemaakt door de leverancier.
 Logische testgevallen worden vastgelegd en gekoppeld met use cases en user stories. Fysieke testgevallen worden vastgelegd in het formaat van de gebruikte tooling en gekoppeld met de logische testgevallen. Op basis hiervan worden testrapportages gegenereerd die laten zien dat alle use cases en user stories zijn getest en dat die tests zijn geslaagd.
 Beschikbare templates:
 - Template detailtestplan softwarerealisatie.
@@ -884,7 +884,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 02-08-2024.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 22-10-2024.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>

</xml_diff>

<commit_message>
"OWASP ZAP" hernoemd naar "ZAP by Checkmarx" in alle documenten.
Closes #945.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -439,7 +439,7 @@
 8. controleren van de configuratie op aanwezigheid van bekende kwetsbaarheden in configuratie: OpenVAS (Vulnerability Assessment System),
 9. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,
 10. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,
-11. dynamische controle van de software op aanwezigheid van kwetsbare constructies: OWASP ZAP (Zed Attack Proxy),
+11. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,
 12. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,
 13. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,
 14. testen op toegankelijkheid van de applicatie: Axe,
@@ -1122,7 +1122,7 @@
     <t>10. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,</t>
   </si>
   <si>
-    <t>11. dynamische controle van de software op aanwezigheid van kwetsbare constructies: OWASP ZAP (Zed Attack Proxy),</t>
+    <t>11. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,</t>
   </si>
   <si>
     <t>12. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,</t>

</xml_diff>

<commit_message>
Voeg template voor voortgang voorfase producten toe.
Closes #760.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -30,10 +30,10 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">M31: Het project beschikt over actuele vastgestelde informatie
-Voor een goede uitvoering van het project is specifieke informatie nodig. De opdrachtgevende organisatie zorgt dat het project bij de start van de voorfase inzicht heeft in de informatie die typisch wordt vastgelegd in een projectstartarchitectuur, business impact analysis en privacy impact assessment. Waar nodig werkt de opdrachtgevende organisatie de informatie bij tijdens de voorfase en realisatiefase.
+Voor een goede uitvoering van het project is specifieke informatie nodig. De opdrachtgevende organisatie zorgt dat het project bij de start van de voorfase inzicht heeft in de informatie die typisch wordt vastgelegd in een projectstartarchitectuur, business impact analyse en privacy impact assessment. Waar nodig werkt de opdrachtgevende organisatie de informatie bij tijdens de voorfase en realisatiefase.
 De opdrachtgevende organisatie zorgt dat het project vanaf de start van de voorfase beschikt over:
 1. Projectstartarchitectuur,
-2. Business impact analysis,
+2. Business impact analyse,
 3. Privacy impact assessment,
 4. Afspraken tussen opdrachtgevende organisatie en beheerorganisatie.
 Als de benodigde informatie niet gereed is bij de start van de voorfase dan maken opdrachtgevende organisatie en ICTU nadere afspraken over de manier waarop de benodigde informatie nog tijdens de voorfase beschikbaar komt voor het project.
@@ -49,8 +49,8 @@
 Zie https://www.noraonline.nl/wiki/PSA.
 Conform NORA werkt de opdrachtgevende organisatie na de start van het project de PSA uit in een solution architectuur (SA).
 Zie https://www.noraonline.nl/wiki/Solution-architectuur.
-Business impact analysis
-In een business impact analysis (BIA) legt de opdrachtgevende organisatie vast hoe belangrijk informatiebeveiliging is voor de eigen bedrijfsvoering/processen. Naast de gevoeligheid voor incidenten komt hierin ook de 'risk appetite' van de organisatie tot uiting: de risico’s die een organisatie bereid is te accepteren. Alleen de opdrachtgevende organisatie zelf kan hierover een uitspraak doen.
+Business impact analyse
+In een business impact analyse (BIA) legt de opdrachtgevende organisatie vast hoe belangrijk informatiebeveiliging is voor de eigen bedrijfsvoering/processen. Naast de gevoeligheid voor incidenten komt hierin ook de 'risk appetite' van de organisatie tot uiting: de risico’s die een organisatie bereid is te accepteren. Alleen de opdrachtgevende organisatie zelf kan hierover een uitspraak doen.
 Privacy impact assessment
 In een privacy impact assessment (PIA) legt de opdrachtgevende organisatie vast wat de privacy-gevoeligheid is van de gegevens die in een proces of informatiesysteem worden verzameld en verwerkt. De rechtmatigheid van de verwerking wordt beoordeeld. En de PIA stelt grenzen aan de gegevens die mogen worden verzameld en verwerkt. Zicht op privacygevoelige gegevens en het (laten) treffen van adequate en afdoende beschermingsmaatregelen is een wettelijke plicht die een organisatie niet aan een andere partij kan overdragen.
 Als een PIA niet nodig is, dan is een verklaring daaromtrent vereist.
@@ -94,7 +94,7 @@
 De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het ✔ geeft aan in welke fase ze worden opgeleverd.
 Product                                             Voor start Voorfase Realisatiefase Verantwoordelijke organisatie 
 Projectstartarchitectuur                            x                                  opdrachtgever                 
-Business impact analysis                            x                                  opdrachtgever                 
+Business impact analyse                             x                                  opdrachtgever                 
 Privacy impact assessment                           x                                  opdrachtgever                 
 Plan van aanpak: voorfase                           x                                  ICTU                          
 Beschrijving van functionele eisen                             x        x              opdrachtgever                 
@@ -112,8 +112,8 @@
 Software bill of materials                                              x              ICTU                          
 Release notes                                                           x              ICTU                          
 Vrijgaveadvies                                                          x              opdrachtgever                 
-Projectstartarchitectuur, business impact analysis en privacy impact assessment
-De opdrachtgevende organisatie zorgt dat het project bij de start van de voorfase inzicht heeft in de informatie die typisch wordt vastgelegd in een projectstartarchitectuur, business impact analysis en privacy impact assessment. Zie M31: Het project beschikt over actuele vastgestelde informatie.
+Projectstartarchitectuur, business impact analyse en privacy impact assessment
+De opdrachtgevende organisatie zorgt dat het project bij de start van de voorfase inzicht heeft in de informatie die typisch wordt vastgelegd in een projectstartarchitectuur, business impact analyse en privacy impact assessment. Zie M31: Het project beschikt over actuele vastgestelde informatie.
 Plan van aanpak
 Het plan van aanpak voor de voorfase en het plan van aanpak voor de realisatiefase beschrijven de in deze fasen te realiseren producten en diensten, en de planning, werkwijze en verantwoordelijkheden voor de totstandkoming van die producten en diensten.
 Als tijdens de realisatiefase van het project bestaande software dient te worden afgebouwd, onderhouden en/of herbouwd, bevat het plan van aanpak voor de voorfase een onderzoek naar de kwaliteit van deze software, zie M32: Het project onderzoekt de kwaliteit van over te nemen software.
@@ -163,7 +163,7 @@
 - Template mastertestplan.
 - Template detailtestplan softwarerealisatie.
 Informatiebeveiligingsplan
-Het informatiebeveiligingsplan vormt een praktisch toepasbaar document dat uitlegt binnen welke kaders bescherming geleverd wordt tegen welke dreigingen en met welke maatregelen die bescherming vorm krijgt. Mogelijke bronnen voor het informatiebeveiligingsplan zijn de business impact analysis (BIA), privacy impact assessment (PIA) en de threat and vulnerability assessment (TVA).
+Het informatiebeveiligingsplan vormt een praktisch toepasbaar document dat uitlegt binnen welke kaders bescherming geleverd wordt tegen welke dreigingen en met welke maatregelen die bescherming vorm krijgt. Mogelijke bronnen voor het informatiebeveiligingsplan zijn de business impact analyse (BIA), privacy impact assessment (PIA) en de threat and vulnerability assessment (TVA).
 Het Besluit Voorschrift Informatiebeveiliging Rijksdienst 2007 (VIR 2007) bevat een methode om te komen tot een systematische aanpak van informatiebeveiliging. Eén van de vereisten van het VIR 2007 is dat voor elk informatiesysteem en voor elk verantwoordelijkheidsgebied een afhankelijkheids- en kwetsbaarheidsanalyse (A&amp;K-analyse) wordt uitgevoerd.
 Bij ICTU wordt daarvoor een TVA gebruikt. Hierin worden de betrouwbaarheidseisen, die aan de bedrijfsprocessen en dientengevolge aan het informatiesysteem of verantwoordelijkheidsgebied worden gesteld, tijdens een afhankelijkheidsanalyse geïnventariseerd. Vervolgens worden de bedreigingen geïdentificeerd en geanalyseerd. De TVA levert zodoende een deel van een traceerbare onderbouwing voor de te treffen beveiligingsmaatregelen. De TVA wordt tijdens de voorfase opgesteld op basis van de resultaten van de BIA, de eventuele PIA en de inhoud van de ontwerp- en architectuurdocumentatie.
 Kwaliteitsplan
@@ -885,7 +885,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 06-12-2024.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 16-12-2024.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
@@ -921,7 +921,7 @@
     <t>1. Projectstartarchitectuur,</t>
   </si>
   <si>
-    <t>2. Business impact analysis,</t>
+    <t>2. Business impact analyse,</t>
   </si>
   <si>
     <t>3. Privacy impact assessment,</t>
@@ -939,7 +939,7 @@
     <t>1. Projectstartarchitectuur</t>
   </si>
   <si>
-    <t>2. Business impact analysis</t>
+    <t>2. Business impact analyse</t>
   </si>
   <si>
     <t>3. Privacy impact assessment</t>
@@ -1404,7 +1404,7 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>

</xml_diff>

<commit_message>
Voeg template voor voortgang voorfase producten toe. (#986)
Closes #760.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -76,7 +76,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -204,7 +204,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -240,7 +240,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -295,7 +295,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -395,7 +395,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -596,7 +596,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -732,7 +732,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Bepaal a.u.b. de status per submaatregel.</t>
+          <t>Bepaal de status per submaatregel.</t>
         </r>
       </text>
     </comment>

</xml_diff>

<commit_message>
Product en sprint backlog consistent geschreven, conform de Scrumgids (behalve hoofdletters).
Closes #994.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -139,7 +139,7 @@
 Beschikbare templates:
 - Template niet-functionele eisen.
 Product backlog
-De product backlog is een geprioriteerd overzicht van alle nog te realiseren functionele en niet-functionele eigenschappen van de software. Al het werk dat het Scrumteam doet loopt via de backlog, niet alleen werk aan de broncode zelf maar bijvoorbeeld ook het schrijven van beheerdocumentatie. De product owner is de eigenaar van de product backlog. De zaken op de lijst zijn normaal gesproken in de vorm van een epic of user story. Hierin staat:
+De product backlog is een geprioriteerd overzicht van alle nog te realiseren functionele en niet-functionele eigenschappen van de software. Al het werk dat het Scrumteam doet loopt via de product backlog, niet alleen werk aan de broncode zelf maar bijvoorbeeld ook het schrijven van beheerdocumentatie. De product owner is de eigenaar van de product backlog. De zaken op de lijst zijn normaal gesproken in de vorm van een epic of user story. Hierin staat:
 - Wat er gemaakt moet worden,
 - Waarom,
 - en voor wie.
@@ -409,7 +409,7 @@
           </rPr>
           <t xml:space="preserve">M16: Het project gebruikt tools voor vastgestelde taken
 ICTU stelt het gebruik van tools verplicht voor de volgende taken:
-1. backlog management en agile werken,
+1. product en sprint backlog management en agile werken,
 2. inrichten en uitvoeren van een continuous delivery pipeline,
 3. monitoren van de kwaliteit van broncode,
 4. versiebeheer van op te leveren producten,
@@ -427,9 +427,9 @@
 16. opslaan van artifacten,
 17. registratie van incidenten bij gebruik en beheer, en
 18. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving.
-Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog en de iteraties als sprints.
+Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
 ICTU adviseert en ondersteunt voor de genoemde taken onderstaande tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven:
-1. backlog management en agile werken: Azure DevOps of Jira,
+1. product en sprint backlog management en agile werken: Azure DevOps of Jira,
 2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,
 3. monitoren van de kwaliteit van broncode: SonarQube,
 4. versiebeheer van op te leveren producten: GitLab of Azure DevOps,
@@ -500,7 +500,7 @@
 Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top-10 genoemd) vermeden zijn en of voldoende invulling gegeven is aan de normen die vanuit BIO en SSD gelden.
 ICTU zorgt ervoor dat de benodigde expertise op afroep beschikbaar gesteld kan worden aan projecten.
 De opdrachtgevende organisatie kan een derde partij opdracht geven beveiligingstesten uit te voeren in een daarvoor door de opdrachtgevende organisatie beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Als de opdrachtgevende organisatie dit structureel inricht en als deze beveiligingstesten voldoen aan de eisen die het project zou stellen, dan kunnen de opdrachtgevende organisatie en het project besluiten dat het project zelf geen beveiligingstesten laat uitvoeren. Afspraken hierover worden bij voorkeur al in de voorfase gemaakt, inclusief een controle dat de opdrachtgevende organisatie de benodigde contractuele mogelijkheden heeft beveiligingstesten uit te besteden. Het project ontvangt in dat geval de beveiligingstestrapportages van de opdrachtgevende organisatie.
-De beveiligingstesten vinden altijd plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software. Bevindingen uit beveiligingstesten en de continue analyse die niet direct worden opgelost, worden in Jira als issue vastgelegd op de backlog van het project.
+De beveiligingstesten vinden altijd plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software. Bevindingen uit beveiligingstesten en de continue analyse die niet direct worden opgelost, worden in Jira als issue vastgelegd op de product backlog.
 De kwaliteitsmanager van het project bewaakt de opvolging van de kritische beveiligingsissues. De kwaliteitsmanager bewaakt tevens of de beveiligingstesten voldoende frequent plaatsvinden, bij voorkeur door Quality-time te laten waarschuwen als het tijd is voor de volgende beveiligingstest.
 Rationale
 Het inschakelen van actuele, specifieke expertise vergroot de kans dat eventuele kwetsbaarheden in de gerealiseerde software tijdig herkend worden.
@@ -706,7 +706,7 @@
 1. De documentatie beschrijft de ontwikkel- en testomgeving die is toegepast (5.1),
 2. De functionele documentatie beschrijft gegevensmodellen, functionele indeling, koppelingen, berichtdefinities en workflows/processen (5.2),
 3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),
-4. De productbacklog bevat de bekende bugs en wensen (5.4),
+4. De product backlog bevat de bekende bugs en wensen (5.4),
 5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling (6.1),
 6. De broncode heeft een beperkte mate van duplicatie (6.2),
 7. De broncode heeft een beperkte mate van complexiteit (6.3),
@@ -870,7 +870,7 @@
 - Opvallende overeenkomsten en verschillen met eerdere gezamenlijke self-assessments,
 - Opvallende maatregelen, bijvoorbeeld maatregelen die veel projecten niet of deels toepassen, en
 - Gemaakte opmerkingen door de deelnemende projecten.
-ICTU organiseert een bespreking van de analyse met de deelnemende projecten. Hieruit vloeiende verbeteracties voor de Kwaliteitsaanpak worden door ICTU geprioriteerd en via de backlog voor de Kwaliteitsaanpak afgehandeld. Bij grotere verbeteracties betrekt ICTU de kwaliteitsmanagers van de belanghebbende projecten.
+ICTU organiseert een bespreking van de analyse met de deelnemende projecten. Hieruit vloeiende verbeteracties voor de Kwaliteitsaanpak worden door ICTU geprioriteerd en via de product backlog voor de Kwaliteitsaanpak afgehandeld. Bij grotere verbeteracties betrekt ICTU de kwaliteitsmanagers van de belanghebbende projecten.
 De gezamenlijke self-assessment is een intern product en de niet-geanonimiseerde resultaten worden alleen gedeeld met de deelnemende projecten. De geanonimiseerde resultaten kunnen worden gedeeld met belanghebbenden en belangstellenden binnen en buiten ICTU.
 Rationale
 Door een gezamenlijke self-assessment te doen met meerdere projecten tegelijkertijd onstaat er inzicht in de mate waarin maatregelen van de Kwaliteitsaanpak toegepast worden en zinvol zijn. Het gesprek over de uitkomsten van de gezamenlijke self-assessment levert input voor verbetering van de Kwaliteitsaanpak zelf.
@@ -1092,7 +1092,7 @@
     <t>Het project gebruikt tools voor vastgestelde taken</t>
   </si>
   <si>
-    <t>1. backlog management en agile werken: Azure DevOps of Jira,</t>
+    <t>1. product en sprint backlog management en agile werken: Azure DevOps of Jira,</t>
   </si>
   <si>
     <t>2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,</t>
@@ -1236,7 +1236,7 @@
     <t>3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),</t>
   </si>
   <si>
-    <t>4. De productbacklog bevat de bekende bugs en wensen (5.4),</t>
+    <t>4. De product backlog bevat de bekende bugs en wensen (5.4),</t>
   </si>
   <si>
     <t>5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling (6.1),</t>

</xml_diff>

<commit_message>
Update ISO 25010. (#983)
Update ISO 25010.

- Referenties naar NEN-ISO/IEC 25010:2011 vervangen door NEN-ISO/IEC 25010:2023.
- NEN-ISO/IEC 25010:2023 verwerkt in NFE-template.

Closes #874.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -126,7 +126,7 @@
 Bronnen van de opdrachtgevende organisatie zoals de projectstartarchitectuur, een programma van eisen en procesbeschrijvingen vormen het startpunt voor de functionele eisen. Tijdens het project worden use cases in samenwerking met de product owner vertaald naar epics en user stories.
 Beschrijving van niet-functionele eisen
 Niet-functionele eisen specificeren criteria om het functioneren van de software te beoordelen, maar beschrijven niet het specifieke gedrag zelf. Voor de beschrijving en onderverdeling van niet-functionele eisen maakt het project gebruik van:
-- NEN-ISO/IEC 25010,
+- NEN-ISO/IEC 25010:2023,
 - Wet beveiliging netwerk- en informatiesystemen (Wbni),
 - Baseline Informatiebeveiliging Overheid (BIO),
 - methode Grip op SDD (Secure Software Development) van het Centrum Informatiebeveiliging en Privacybescherming (CIP),
@@ -327,10 +327,10 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">M13: Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen
-Voor specificatie en documentatie van vereiste en gewenste kwaliteitseigenschappen, de niet-functionele eisen, maken projecten gebruik van de terminologie en categorisering uit NEN-ISO/IEC 25010. Projecten gebruiken NEN-ISO/IEC 25010 om te controleren of alle relevante kwaliteitseigenschappen van het op te leveren eindproduct worden meegenomen in de ontwikkeling en/of onderhoud van het product.
-De standaard NEN-ISO/IEC 25010:2011, kortweg "ISO-25010", biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. ISO-25010 dekt een breed spectrum van kwaliteitseigenschappen af.
+Voor specificatie en documentatie van vereiste en gewenste kwaliteitseigenschappen, de niet-functionele eisen, maken projecten gebruik van de terminologie en categorisering uit NEN-ISO/IEC 25010:2023. Projecten gebruiken NEN-ISO/IEC 25010:2023 om te controleren of alle relevante kwaliteitseigenschappen van het op te leveren eindproduct worden meegenomen in de ontwikkeling en/of onderhoud van het product.
+De standaard NEN-ISO/IEC 25010:2023 biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. NEN-ISO/IEC 25010:2023 dekt een breed spectrum van kwaliteitseigenschappen af.
 Rationale
-ISO-25010 biedt een model voor productkwaliteit. De standaard biedt geen concrete maatregelen, maar biedt wel een begrippenkader en dekt het volledige spectrum van mogelijk relevante kwaliteitseigenschappen af. Het gebruiken van een standaard voor specificatie van kwaliteit voorkomt miscommunicatie over kwaliteitseigenschappen en de breedte van de standaard zorgt ervoor dat alle relevante aspecten aan bod komen.
+NEN-ISO/IEC 25010:2023 biedt een model voor productkwaliteit. De standaard biedt geen concrete maatregelen, maar biedt wel een begrippenkader en dekt het volledige spectrum van mogelijk relevante kwaliteitseigenschappen af. Het gebruiken van een standaard voor specificatie van kwaliteit voorkomt miscommunicatie over kwaliteitseigenschappen en de breedte van de standaard zorgt ervoor dat alle relevante aspecten aan bod komen.
 </t>
         </r>
       </text>
@@ -519,7 +519,7 @@
           </rPr>
           <t xml:space="preserve">M14: Het project bereidt samen met opdrachtgevende organisatie en betrokken partijen de realisatie voor
 Projecten hebben een voorbereidingsfase, "voorfase" genoemd, voorafgaand aan de realisatiefase. Voor het uitvoeren van de voorfase zijn vertegenwoordigers van de opdrachtgevende organisatie, de beoogde beheerorganisatie en andere partijen betrokken die meewerken aan het realiseren van een deel van de op te leveren producten. Het doel van de voorfase is beeld krijgen van de te realiseren oplossing, van de risico's die zich tijdens realisatie kunnen voordoen en van de kaders waarbinnen de oplossing moet passen; tijdens de realisatiefase vinden bouw en onderhoud van de software en actualiseren en afronden van documentatie plaats.
-Bij voorkeur zijn dezelfde deskundigen in zowel de voorfase als in de realisatiefase betrokken.
+De opdrachtgever organiseert de betrokkenheid van vertegenwoordigers en zorgt dat zij voldoende tijd en mandaat hebben om hun rol goed in te vullen. Bij voorkeur zijn dezelfde vertegenwoordigers in zowel de voorfase als in de realisatiefase betrokken.
 In de realisatiefase wordt de prioriteit van werk van het Scrumteam bepaald door een product owner van de opdrachtgevende organisatie. Bij aanvang van de voorfase is deze beoogde product owner bekend en werkt deze ook mee in de voorfase.
 Als tijdens de realisatiefase blijkt dat de kaders van het project significant wijzigen, dan stemmen opdrachtgevende organisatie, ICTU en andere betrokken partijen af welke onderdelen van de voorfase opnieuw moeten worden uitgevoerd. Denk bij significante wijzigingen aan grote aanpassingen aan de scope, het budget, de belanghebbenden en/of de planning van het project.
 Rationale
@@ -885,7 +885,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 20-12-2024.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 28-02-2025.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>

</xml_diff>

<commit_message>
Product en sprint backlog consistent geschreven, conform de Scrumgids (behalve hoofdletters). (#1006)
Closes #994.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -139,7 +139,7 @@
 Beschikbare templates:
 - Template niet-functionele eisen.
 Product backlog
-De product backlog is een geprioriteerd overzicht van alle nog te realiseren functionele en niet-functionele eigenschappen van de software. Al het werk dat het Scrumteam doet loopt via de backlog, niet alleen werk aan de broncode zelf maar bijvoorbeeld ook het schrijven van beheerdocumentatie. De product owner is de eigenaar van de product backlog. De zaken op de lijst zijn normaal gesproken in de vorm van een epic of user story. Hierin staat:
+De product backlog is een geprioriteerd overzicht van alle nog te realiseren functionele en niet-functionele eigenschappen van de software. Al het werk dat het Scrumteam doet loopt via de product backlog, niet alleen werk aan de broncode zelf maar bijvoorbeeld ook het schrijven van beheerdocumentatie. De product owner is de eigenaar van de product backlog. De zaken op de lijst zijn normaal gesproken in de vorm van een epic of user story. Hierin staat:
 - Wat er gemaakt moet worden,
 - Waarom,
 - en voor wie.
@@ -409,7 +409,7 @@
           </rPr>
           <t xml:space="preserve">M16: Het project gebruikt tools voor vastgestelde taken
 ICTU stelt het gebruik van tools verplicht voor de volgende taken:
-1. backlog management en agile werken,
+1. product en sprint backlog management en agile werken,
 2. inrichten en uitvoeren van een continuous delivery pipeline,
 3. monitoren van de kwaliteit van broncode,
 4. versiebeheer van op te leveren producten,
@@ -427,9 +427,9 @@
 16. opslaan van artifacten,
 17. registratie van incidenten bij gebruik en beheer, en
 18. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving.
-Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als backlog en de iteraties als sprints.
+Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
 ICTU adviseert en ondersteunt voor de genoemde taken onderstaande tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven:
-1. backlog management en agile werken: Azure DevOps of Jira,
+1. product en sprint backlog management en agile werken: Azure DevOps of Jira,
 2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,
 3. monitoren van de kwaliteit van broncode: SonarQube,
 4. versiebeheer van op te leveren producten: GitLab of Azure DevOps,
@@ -500,7 +500,7 @@
 Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top-10 genoemd) vermeden zijn en of voldoende invulling gegeven is aan de normen die vanuit BIO en SSD gelden.
 ICTU zorgt ervoor dat de benodigde expertise op afroep beschikbaar gesteld kan worden aan projecten.
 De opdrachtgevende organisatie kan een derde partij opdracht geven beveiligingstesten uit te voeren in een daarvoor door de opdrachtgevende organisatie beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Als de opdrachtgevende organisatie dit structureel inricht en als deze beveiligingstesten voldoen aan de eisen die het project zou stellen, dan kunnen de opdrachtgevende organisatie en het project besluiten dat het project zelf geen beveiligingstesten laat uitvoeren. Afspraken hierover worden bij voorkeur al in de voorfase gemaakt, inclusief een controle dat de opdrachtgevende organisatie de benodigde contractuele mogelijkheden heeft beveiligingstesten uit te besteden. Het project ontvangt in dat geval de beveiligingstestrapportages van de opdrachtgevende organisatie.
-De beveiligingstesten vinden altijd plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software. Bevindingen uit beveiligingstesten en de continue analyse die niet direct worden opgelost, worden in Jira als issue vastgelegd op de backlog van het project.
+De beveiligingstesten vinden altijd plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software. Bevindingen uit beveiligingstesten en de continue analyse die niet direct worden opgelost, worden in Jira als issue vastgelegd op de product backlog.
 De kwaliteitsmanager van het project bewaakt de opvolging van de kritische beveiligingsissues. De kwaliteitsmanager bewaakt tevens of de beveiligingstesten voldoende frequent plaatsvinden, bij voorkeur door Quality-time te laten waarschuwen als het tijd is voor de volgende beveiligingstest.
 Rationale
 Het inschakelen van actuele, specifieke expertise vergroot de kans dat eventuele kwetsbaarheden in de gerealiseerde software tijdig herkend worden.
@@ -706,7 +706,7 @@
 1. De documentatie beschrijft de ontwikkel- en testomgeving die is toegepast (5.1),
 2. De functionele documentatie beschrijft gegevensmodellen, functionele indeling, koppelingen, berichtdefinities en workflows/processen (5.2),
 3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),
-4. De productbacklog bevat de bekende bugs en wensen (5.4),
+4. De product backlog bevat de bekende bugs en wensen (5.4),
 5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling (6.1),
 6. De broncode heeft een beperkte mate van duplicatie (6.2),
 7. De broncode heeft een beperkte mate van complexiteit (6.3),
@@ -870,7 +870,7 @@
 - Opvallende overeenkomsten en verschillen met eerdere gezamenlijke self-assessments,
 - Opvallende maatregelen, bijvoorbeeld maatregelen die veel projecten niet of deels toepassen, en
 - Gemaakte opmerkingen door de deelnemende projecten.
-ICTU organiseert een bespreking van de analyse met de deelnemende projecten. Hieruit vloeiende verbeteracties voor de Kwaliteitsaanpak worden door ICTU geprioriteerd en via de backlog voor de Kwaliteitsaanpak afgehandeld. Bij grotere verbeteracties betrekt ICTU de kwaliteitsmanagers van de belanghebbende projecten.
+ICTU organiseert een bespreking van de analyse met de deelnemende projecten. Hieruit vloeiende verbeteracties voor de Kwaliteitsaanpak worden door ICTU geprioriteerd en via de product backlog voor de Kwaliteitsaanpak afgehandeld. Bij grotere verbeteracties betrekt ICTU de kwaliteitsmanagers van de belanghebbende projecten.
 De gezamenlijke self-assessment is een intern product en de niet-geanonimiseerde resultaten worden alleen gedeeld met de deelnemende projecten. De geanonimiseerde resultaten kunnen worden gedeeld met belanghebbenden en belangstellenden binnen en buiten ICTU.
 Rationale
 Door een gezamenlijke self-assessment te doen met meerdere projecten tegelijkertijd onstaat er inzicht in de mate waarin maatregelen van de Kwaliteitsaanpak toegepast worden en zinvol zijn. Het gesprek over de uitkomsten van de gezamenlijke self-assessment levert input voor verbetering van de Kwaliteitsaanpak zelf.
@@ -1092,7 +1092,7 @@
     <t>Het project gebruikt tools voor vastgestelde taken</t>
   </si>
   <si>
-    <t>1. backlog management en agile werken: Azure DevOps of Jira,</t>
+    <t>1. product en sprint backlog management en agile werken: Azure DevOps of Jira,</t>
   </si>
   <si>
     <t>2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,</t>
@@ -1236,7 +1236,7 @@
     <t>3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),</t>
   </si>
   <si>
-    <t>4. De productbacklog bevat de bekende bugs en wensen (5.4),</t>
+    <t>4. De product backlog bevat de bekende bugs en wensen (5.4),</t>
   </si>
   <si>
     <t>5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling (6.1),</t>

</xml_diff>

<commit_message>
Informatie over testomgevingen toegevoegd.
- In M02 "Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet" bij het kopje "Realisatiefase: handmatige evaluatie" weggehaald dat de performance handmatig wordt getest; dit gebeurt in de praktijk altijd geautomatiseerd.
- In M07 "Het project gebruikt een continuous delivery pipeline om het product te bouwen, testen en op te leveren" toegevoegd in welke omgeving(en) performance- en beveiligingstests plaatsvinden.
- In M26 "Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen" toegevoegd in welke omgeving(en) penetratietesten plaatsvinden.

Closes #678.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -271,7 +271,7 @@
 Realisatiefase operationeel beheer: geautomatiseerde monitoring
 Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase monitort en test het project continue het gedrag van de software in gebruik en beheer. Hiertoe gebruikt het project operationele monitoringsoftware, bijvoorbeeld Nagios en/of Zabbix.
 Realisatiefase: handmatige evaluatie
-Kwaliteitseigenschappen van de software die niet (volledig) geautomatiseerd kunnen worden gemeten, worden tijdens de realisatiefase periodiek handmatig geëvalueerd. Minimaal betreft dit de beveiliging van de software, zie M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen. Ook zorgt het project dat de performance van de software regelmatig wordt getest. Voor kwaliteitsaspecten als toegankelijkheid en gebruikskwaliteit organiseert het project handmatige testen en/of evaluaties in een vorm en met een frequentie die aansluit bij de aard van de applicatie en de door de opdrachtgevende organisatie gestelde eisen. De kwaliteitsmanager houdt in Quality-time bij wanneer de laatste test of evaluatie is uitgevoerd en wanneer het tijd is voor de volgende.
+Kwaliteitseigenschappen van de software die niet (volledig) geautomatiseerd kunnen worden gemeten, worden tijdens de realisatiefase periodiek handmatig geëvalueerd. Minimaal betreft dit de beveiliging van de software, zie M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen. Voor kwaliteitsaspecten als toegankelijkheid en gebruikskwaliteit organiseert het project handmatige testen en/of evaluaties in een vorm en met een frequentie die aansluit bij de aard van de applicatie en de door de opdrachtgevende organisatie gestelde eisen. De kwaliteitsmanager houdt in Quality-time bij wanneer de laatste test of evaluatie is uitgevoerd en wanneer het tijd is voor de volgende.
 Realisatiefase: actualisering en review documentatie
 Documenten, die onderdeel uitmaken van het op te leveren projectresultaat, zijn zo veel mogelijk geactualiseerd; eventuele achterstand wordt planmatig weggewerkt. De kwaliteitscontrole van documenten gebeurt op basis van reviews. De auteur van een document en de software delivery manager zorgen dat de juiste reviewers benoemd zijn; hiertoe behoort in ieder geval de kwaliteitsmanager. De auteur van het document zorgt voor een correct versiebeheer van het document. De auteur koppelt aan de reviewers terug of en hoe het ontvangen commentaar is verwerkt in de volgende versie van het betreffende document.
 Escalatie
@@ -375,7 +375,7 @@
 8. Installatie van de software in test, acceptatie en/of productieomgevingen,
 9. Produceren van een "software bill of materials" (SBoM),
 10. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.
-Performance- en beveiligingstests zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats.
+Performance- en beveiligingstests op de software zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats. Performance- en beveiligingstests op de software vinden plaats in de testomgeving van het project. Als ICTU verantwoordelijk is voor het operationeel beheer laat ICTU de performance- en beveiligingstesten op de software (ook) uitvoeren in een productie-like omgeving.
 Niet alle testen en controles kunnen altijd geautomatiseerd worden uitgevoerd. Denk aan kwaliteitscontroles op architectuurbeslissingen of het testen van toegankelijkheidseisen. Waar mogelijk wordt wel een zo groot mogelijk deel van de testen en controles geautomatiseerd en als onderdeel van de pipeline uitgevoerd.
 De afdeling ICTU Software Diensten (ISD) voorziet in tools en ondersteuning, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
 ICTU gebruikt Jenkins, GitLab CI of Azure DevOps als tool voor de implementatie van de continuous delivery pipeline. ISD biedt de projecten een voorziening om releases van het totale product veilig op te leveren aan opdrachtgevende organisaties en beheerorganisaties.
@@ -497,7 +497,7 @@
           </rPr>
           <t xml:space="preserve">M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen
 Projecten laten periodiek de beveiliging van de ontwikkelde software beoordelen. Een beveiligingsexpert onderzoekt de code zowel geautomatiseerd als handmatig op veelvoorkomende kwetsbaarheden en op het voldoen aan voorgeschreven beveiligingsnormen. Overheidsspecifieke beveiligingsnormen of -raamwerken, zoals de BIO (Baseline Informatiebeveiliging Overheid), bieden een basis voor de beoordeling. Bevindingen uit de beveiligingstest worden vastgelegd als onderdeel van de werkvoorraad voor het ontwikkelproces.
-Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top-10 genoemd) vermeden zijn en of voldoende invulling gegeven is aan de normen die vanuit BIO en SSD gelden.
+Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top-10 genoemd) vermeden zijn en of voldoende invulling gegeven is aan de normen die vanuit BIO en SSD gelden. Penetratietesten op de software vinden plaats in de testomgeving van het project. Als ICTU verantwoordelijk is voor het operationeel beheer laat ICTU de penetratietesten op de software (ook) uitvoeren in een productie-like omgeving.
 ICTU zorgt ervoor dat de benodigde expertise op afroep beschikbaar gesteld kan worden aan projecten.
 De opdrachtgevende organisatie kan een derde partij opdracht geven beveiligingstesten uit te voeren in een daarvoor door de opdrachtgevende organisatie beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Als de opdrachtgevende organisatie dit structureel inricht en als deze beveiligingstesten voldoen aan de eisen die het project zou stellen, dan kunnen de opdrachtgevende organisatie en het project besluiten dat het project zelf geen beveiligingstesten laat uitvoeren. Afspraken hierover worden bij voorkeur al in de voorfase gemaakt, inclusief een controle dat de opdrachtgevende organisatie de benodigde contractuele mogelijkheden heeft beveiligingstesten uit te besteden. Het project ontvangt in dat geval de beveiligingstestrapportages van de opdrachtgevende organisatie.
 De beveiligingstesten vinden altijd plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software. Bevindingen uit beveiligingstesten en de continue analyse die niet direct worden opgelost, worden in Jira als issue vastgelegd op de product backlog.

</xml_diff>

<commit_message>
Maak onderhoud van producten per projectfase expliciet.
In M01 "Het project levert in elke fase vastgestelde producten en informatie op" expliciet gemaakt in welke fasen producten worden onderhouden.

Closes #1008.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -36,6 +36,7 @@
 2. Business impact analyse,
 3. Privacy impact assessment,
 4. Afspraken tussen opdrachtgevende organisatie en beheerorganisatie.
+Tevens onderhoudt de opdrachtgevende organisatie deze informatie tijdens de voorfase en realisatiefase.
 Als de benodigde informatie niet gereed is bij de start van de voorfase dan maken opdrachtgevende organisatie en ICTU nadere afspraken over de manier waarop de benodigde informatie nog tijdens de voorfase beschikbaar komt voor het project.
 Projectstartarchitectuur
 Een projectstartarchitectuur (PSA) is bedoeld om te borgen dat nieuwe ontwikkelingen en veranderingen in samenhang worden gerealiseerd en passen binnen de toekomstig gewenste informatievoorziening. De PSA is een concreet en doelgericht ICT-architectuurkader waarbinnen het project moet worden uitgevoerd. In de PSA zijn de architectuurvisie, enterprise-architectuur en overige architecturen van de opdrachtgevende organisatie vertaald naar aan het product te stellen eisen. Een PSA bevat in ieder geval de volgende onderwerpen:
@@ -91,20 +92,20 @@
           <t xml:space="preserve">M01: Het project levert in elke fase vastgestelde producten en informatie op
 Iedere projectfase levert specifieke informatie op. De voorfase levert inzicht in de functionele en niet-functionele eisen, ontwerp en architectuur, testplannen, operationele risico's, en benodigde kwaliteitsmaatregelen. Deze informatie wordt tijdens de realisatiefase waar nodig bijgewerkt. De realisatiefase levert één of meerdere werkende versies van de software met regressietests, aangevuld met een vrijgaveadvies, release notes en installatiedocumentatie.
 Opdrachtgevende organisatie, ICTU, beheerorganisatie en andere meewerkende partijen leveren de onderstaande informatie op. Voor een aantal documenten zijn als onderdeel van de Kwaliteitsaanpak templates beschikbaar. Ook kan gebruik worden gemaakt van bestaande templates uit bijvoorbeeld de NORA. Zie M29: ICTU organiseert voor aanvang van een project de interne dienstverlening.
-De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het ✔ geeft aan in welke fase ze worden opgeleverd.
+De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het vinkje (✔) geeft aan in welke fase ze (initieel) worden opgeleverd. Het tandwiel (⚙) geeft aan in welke fase de producten worden onderhouden en bijgewerkt.
 Product                                             Voor start Voorfase Realisatiefase Verantwoordelijke organisatie 
-Projectstartarchitectuur                            x                                  opdrachtgever                 
-Business impact analyse                             x                                  opdrachtgever                 
-Privacy impact assessment                           x                                  opdrachtgever                 
+Projectstartarchitectuur                            x          o        o              opdrachtgever                 
+Business impact analyse                             x          o        o              opdrachtgever                 
+Privacy impact assessment                           x          o        o              opdrachtgever                 
 Plan van aanpak: voorfase                           x                                  ICTU                          
-Beschrijving van functionele eisen                             x        x              opdrachtgever                 
-Beschrijving van niet-functionele eisen                        x        x              opdrachtgever                 
-Product backlog                                                x        x              opdrachtgever                 
-Ontwerp- en architectuurdocumentatie                           x        x              ICTU, beheerorganisatie       
-Mastertestplan                                                 x        x              opdrachtgever                 
-Detailtestplannen                                              x        x              ICTU, beheerorganisatie       
-Informatiebeveiligingsplan                                     x        x              opdrachtgever                 
-Kwaliteitsplan                                                 x        x              ICTU                          
+Beschrijving van functionele eisen                             x        o              opdrachtgever                 
+Beschrijving van niet-functionele eisen                        x        o              opdrachtgever                 
+Product backlog                                                x        o              opdrachtgever                 
+Ontwerp- en architectuurdocumentatie                           x        o              ICTU, beheerorganisatie       
+Mastertestplan                                                 x        o              opdrachtgever                 
+Detailtestplannen                                              x        o              ICTU, beheerorganisatie       
+Informatiebeveiligingsplan                                     x        o              opdrachtgever                 
+Kwaliteitsplan                                                 x        o              ICTU                          
 Plan van aanpak: realisatiefase                                x                       ICTU                          
 Deploybare versie van de software                                       x              ICTU                          
 Testrapportages                                                         x              ICTU, beheerorganisatie       

</xml_diff>

<commit_message>
Informatie over testomgevingen toegevoegd. (#1014)
- In M02 "Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet" bij het kopje "Realisatiefase: handmatige evaluatie" weggehaald dat de performance handmatig wordt getest; dit gebeurt in de praktijk altijd geautomatiseerd.
- In M07 "Het project gebruikt een continuous delivery pipeline om het product te bouwen, testen en op te leveren" toegevoegd in welke omgeving(en) performance- en beveiligingstests plaatsvinden.
- In M26 "Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen" toegevoegd in welke omgeving(en) penetratietesten plaatsvinden.

Closes #678.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -271,7 +271,7 @@
 Realisatiefase operationeel beheer: geautomatiseerde monitoring
 Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase monitort en test het project continue het gedrag van de software in gebruik en beheer. Hiertoe gebruikt het project operationele monitoringsoftware, bijvoorbeeld Nagios en/of Zabbix.
 Realisatiefase: handmatige evaluatie
-Kwaliteitseigenschappen van de software die niet (volledig) geautomatiseerd kunnen worden gemeten, worden tijdens de realisatiefase periodiek handmatig geëvalueerd. Minimaal betreft dit de beveiliging van de software, zie M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen. Ook zorgt het project dat de performance van de software regelmatig wordt getest. Voor kwaliteitsaspecten als toegankelijkheid en gebruikskwaliteit organiseert het project handmatige testen en/of evaluaties in een vorm en met een frequentie die aansluit bij de aard van de applicatie en de door de opdrachtgevende organisatie gestelde eisen. De kwaliteitsmanager houdt in Quality-time bij wanneer de laatste test of evaluatie is uitgevoerd en wanneer het tijd is voor de volgende.
+Kwaliteitseigenschappen van de software die niet (volledig) geautomatiseerd kunnen worden gemeten, worden tijdens de realisatiefase periodiek handmatig geëvalueerd. Minimaal betreft dit de beveiliging van de software, zie M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen. Voor kwaliteitsaspecten als toegankelijkheid en gebruikskwaliteit organiseert het project handmatige testen en/of evaluaties in een vorm en met een frequentie die aansluit bij de aard van de applicatie en de door de opdrachtgevende organisatie gestelde eisen. De kwaliteitsmanager houdt in Quality-time bij wanneer de laatste test of evaluatie is uitgevoerd en wanneer het tijd is voor de volgende.
 Realisatiefase: actualisering en review documentatie
 Documenten, die onderdeel uitmaken van het op te leveren projectresultaat, zijn zo veel mogelijk geactualiseerd; eventuele achterstand wordt planmatig weggewerkt. De kwaliteitscontrole van documenten gebeurt op basis van reviews. De auteur van een document en de software delivery manager zorgen dat de juiste reviewers benoemd zijn; hiertoe behoort in ieder geval de kwaliteitsmanager. De auteur van het document zorgt voor een correct versiebeheer van het document. De auteur koppelt aan de reviewers terug of en hoe het ontvangen commentaar is verwerkt in de volgende versie van het betreffende document.
 Escalatie
@@ -375,7 +375,7 @@
 8. Installatie van de software in test, acceptatie en/of productieomgevingen,
 9. Produceren van een "software bill of materials" (SBoM),
 10. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.
-Performance- en beveiligingstests zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats.
+Performance- en beveiligingstests op de software zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats. Performance- en beveiligingstests op de software vinden plaats in de testomgeving van het project. Als ICTU verantwoordelijk is voor het operationeel beheer laat ICTU de performance- en beveiligingstesten op de software (ook) uitvoeren in een productie-like omgeving.
 Niet alle testen en controles kunnen altijd geautomatiseerd worden uitgevoerd. Denk aan kwaliteitscontroles op architectuurbeslissingen of het testen van toegankelijkheidseisen. Waar mogelijk wordt wel een zo groot mogelijk deel van de testen en controles geautomatiseerd en als onderdeel van de pipeline uitgevoerd.
 De afdeling ICTU Software Diensten (ISD) voorziet in tools en ondersteuning, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
 ICTU gebruikt Jenkins, GitLab CI of Azure DevOps als tool voor de implementatie van de continuous delivery pipeline. ISD biedt de projecten een voorziening om releases van het totale product veilig op te leveren aan opdrachtgevende organisaties en beheerorganisaties.
@@ -497,7 +497,7 @@
           </rPr>
           <t xml:space="preserve">M26: Het project laat de beveiliging van het ontwikkelde product periodiek beoordelen
 Projecten laten periodiek de beveiliging van de ontwikkelde software beoordelen. Een beveiligingsexpert onderzoekt de code zowel geautomatiseerd als handmatig op veelvoorkomende kwetsbaarheden en op het voldoen aan voorgeschreven beveiligingsnormen. Overheidsspecifieke beveiligingsnormen of -raamwerken, zoals de BIO (Baseline Informatiebeveiliging Overheid), bieden een basis voor de beoordeling. Bevindingen uit de beveiligingstest worden vastgelegd als onderdeel van de werkvoorraad voor het ontwikkelproces.
-Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top-10 genoemd) vermeden zijn en of voldoende invulling gegeven is aan de normen die vanuit BIO en SSD gelden.
+Software wordt minimaal bij iedere grote release of ten minste twee keer per jaar onderworpen aan een beveiligingstest door beveiligingsexperts die ICTU daarvoor inhuurt. Op basis van documentatie en architectuurstudie, crystalbox security audits (broncodescan) en penetratieaudits beoordelen deze experts of de software voldoet aan de projectspecifieke niet-functionele eisen met betrekking tot beveiliging, of bekende kwetsbaarheden (zoals bijvoorbeeld in de OWASP Top-10 genoemd) vermeden zijn en of voldoende invulling gegeven is aan de normen die vanuit BIO en SSD gelden. Penetratietesten op de software vinden plaats in de testomgeving van het project. Als ICTU verantwoordelijk is voor het operationeel beheer laat ICTU de penetratietesten op de software (ook) uitvoeren in een productie-like omgeving.
 ICTU zorgt ervoor dat de benodigde expertise op afroep beschikbaar gesteld kan worden aan projecten.
 De opdrachtgevende organisatie kan een derde partij opdracht geven beveiligingstesten uit te voeren in een daarvoor door de opdrachtgevende organisatie beschikbaar gestelde omgeving. Dit kan zowel incidenteel als structureel worden ingericht. Als de opdrachtgevende organisatie dit structureel inricht en als deze beveiligingstesten voldoen aan de eisen die het project zou stellen, dan kunnen de opdrachtgevende organisatie en het project besluiten dat het project zelf geen beveiligingstesten laat uitvoeren. Afspraken hierover worden bij voorkeur al in de voorfase gemaakt, inclusief een controle dat de opdrachtgevende organisatie de benodigde contractuele mogelijkheden heeft beveiligingstesten uit te besteden. Het project ontvangt in dat geval de beveiligingstestrapportages van de opdrachtgevende organisatie.
 De beveiligingstesten vinden altijd plaats in aanvulling op de door tools uitgevoerde continue beveiligingsanalyse van de gerealiseerde software. Bevindingen uit beveiligingstesten en de continue analyse die niet direct worden opgelost, worden in Jira als issue vastgelegd op de product backlog.

</xml_diff>

<commit_message>
Maak onderhoud van producten per projectfase expliciet. (#1015)
In M01 "Het project levert in elke fase vastgestelde producten en informatie op" expliciet gemaakt in welke fasen producten worden onderhouden.

Closes #1008.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -36,6 +36,7 @@
 2. Business impact analyse,
 3. Privacy impact assessment,
 4. Afspraken tussen opdrachtgevende organisatie en beheerorganisatie.
+Tevens onderhoudt de opdrachtgevende organisatie deze informatie tijdens de voorfase en realisatiefase.
 Als de benodigde informatie niet gereed is bij de start van de voorfase dan maken opdrachtgevende organisatie en ICTU nadere afspraken over de manier waarop de benodigde informatie nog tijdens de voorfase beschikbaar komt voor het project.
 Projectstartarchitectuur
 Een projectstartarchitectuur (PSA) is bedoeld om te borgen dat nieuwe ontwikkelingen en veranderingen in samenhang worden gerealiseerd en passen binnen de toekomstig gewenste informatievoorziening. De PSA is een concreet en doelgericht ICT-architectuurkader waarbinnen het project moet worden uitgevoerd. In de PSA zijn de architectuurvisie, enterprise-architectuur en overige architecturen van de opdrachtgevende organisatie vertaald naar aan het product te stellen eisen. Een PSA bevat in ieder geval de volgende onderwerpen:
@@ -91,20 +92,20 @@
           <t xml:space="preserve">M01: Het project levert in elke fase vastgestelde producten en informatie op
 Iedere projectfase levert specifieke informatie op. De voorfase levert inzicht in de functionele en niet-functionele eisen, ontwerp en architectuur, testplannen, operationele risico's, en benodigde kwaliteitsmaatregelen. Deze informatie wordt tijdens de realisatiefase waar nodig bijgewerkt. De realisatiefase levert één of meerdere werkende versies van de software met regressietests, aangevuld met een vrijgaveadvies, release notes en installatiedocumentatie.
 Opdrachtgevende organisatie, ICTU, beheerorganisatie en andere meewerkende partijen leveren de onderstaande informatie op. Voor een aantal documenten zijn als onderdeel van de Kwaliteitsaanpak templates beschikbaar. Ook kan gebruik worden gemaakt van bestaande templates uit bijvoorbeeld de NORA. Zie M29: ICTU organiseert voor aanvang van een project de interne dienstverlening.
-De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het ✔ geeft aan in welke fase ze worden opgeleverd.
+De onderstaande tabel bevat de in deze paragraaf beschreven producten. Het vinkje (✔) geeft aan in welke fase ze (initieel) worden opgeleverd. Het tandwiel (⚙) geeft aan in welke fase de producten worden onderhouden en bijgewerkt.
 Product                                             Voor start Voorfase Realisatiefase Verantwoordelijke organisatie 
-Projectstartarchitectuur                            x                                  opdrachtgever                 
-Business impact analyse                             x                                  opdrachtgever                 
-Privacy impact assessment                           x                                  opdrachtgever                 
+Projectstartarchitectuur                            x          o        o              opdrachtgever                 
+Business impact analyse                             x          o        o              opdrachtgever                 
+Privacy impact assessment                           x          o        o              opdrachtgever                 
 Plan van aanpak: voorfase                           x                                  ICTU                          
-Beschrijving van functionele eisen                             x        x              opdrachtgever                 
-Beschrijving van niet-functionele eisen                        x        x              opdrachtgever                 
-Product backlog                                                x        x              opdrachtgever                 
-Ontwerp- en architectuurdocumentatie                           x        x              ICTU, beheerorganisatie       
-Mastertestplan                                                 x        x              opdrachtgever                 
-Detailtestplannen                                              x        x              ICTU, beheerorganisatie       
-Informatiebeveiligingsplan                                     x        x              opdrachtgever                 
-Kwaliteitsplan                                                 x        x              ICTU                          
+Beschrijving van functionele eisen                             x        o              opdrachtgever                 
+Beschrijving van niet-functionele eisen                        x        o              opdrachtgever                 
+Product backlog                                                x        o              opdrachtgever                 
+Ontwerp- en architectuurdocumentatie                           x        o              ICTU, beheerorganisatie       
+Mastertestplan                                                 x        o              opdrachtgever                 
+Detailtestplannen                                              x        o              ICTU, beheerorganisatie       
+Informatiebeveiligingsplan                                     x        o              opdrachtgever                 
+Kwaliteitsplan                                                 x        o              ICTU                          
 Plan van aanpak: realisatiefase                                x                       ICTU                          
 Deploybare versie van de software                                       x              ICTU                          
 Testrapportages                                                         x              ICTU, beheerorganisatie       

</xml_diff>

<commit_message>
Link maatregelen in self-assessment checklist.
De maatregelennummers in de self-assessment checklist linken naar de bijbehorende maatregelen in de online versie van de Kwaliteitsaanpak.

Closes #957.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -886,7 +886,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 04-03-2025.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
@@ -1328,7 +1328,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1346,6 +1346,14 @@
     </font>
     <font>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1402,13 +1410,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1825,591 +1836,591 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="5"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="5"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6" t="s">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="5"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6" t="s">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="5"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6" t="s">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6" t="s">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="5"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6" t="s">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="5"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6" t="s">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6" t="s">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6" t="s">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6" t="s">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="5"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6" t="s">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="5"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6" t="s">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="5"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="6"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6" t="s">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="5"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="6"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6" t="s">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="5"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="5"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6" t="s">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="5"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6" t="s">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="5"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="5"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="5"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6" t="s">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="7"/>
-      <c r="D71" s="5"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6" t="s">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="7"/>
-      <c r="D72" s="5"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6" t="s">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="7"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6" t="s">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="7"/>
-      <c r="D74" s="5"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6" t="s">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="7"/>
-      <c r="D75" s="5"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
@@ -2423,245 +2434,245 @@
       <c r="A79" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6" t="s">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="5"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6" t="s">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="7"/>
-      <c r="D84" s="5"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6" t="s">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="7"/>
-      <c r="D85" s="5"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6" t="s">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="7"/>
-      <c r="D86" s="5"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C88" s="4"/>
-      <c r="D88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C89" s="4"/>
-      <c r="D89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="4"/>
-      <c r="D90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="6"/>
-      <c r="B92" s="6" t="s">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="5"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6" t="s">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C93" s="7"/>
-      <c r="D93" s="5"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6" t="s">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="7"/>
-      <c r="D94" s="5"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="6"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6" t="s">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C95" s="7"/>
-      <c r="D95" s="5"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="6"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6" t="s">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="5"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="6"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6" t="s">
+      <c r="A97" s="7"/>
+      <c r="B97" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C97" s="7"/>
-      <c r="D97" s="5"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6" t="s">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="7"/>
-      <c r="D98" s="5"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6" t="s">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="7"/>
-      <c r="D99" s="5"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6" t="s">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="5"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6" t="s">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="7"/>
-      <c r="D101" s="5"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="6"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6" t="s">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C102" s="7"/>
-      <c r="D102" s="5"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="6"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6" t="s">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C103" s="7"/>
-      <c r="D103" s="5"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="6"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6" t="s">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="7"/>
-      <c r="D104" s="5"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="6"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6" t="s">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C105" s="7"/>
-      <c r="D105" s="5"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
@@ -2675,61 +2686,61 @@
       <c r="A108" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C108" s="4"/>
-      <c r="D108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="6"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C109" s="4"/>
-      <c r="D109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="6"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C110" s="4"/>
-      <c r="D110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="6"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C111" s="4"/>
-      <c r="D111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="6"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C112" s="4"/>
-      <c r="D112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="6"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C113" s="4"/>
-      <c r="D113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4525,8 +4536,37 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" location="m31"/>
+    <hyperlink ref="A12" r:id="rId2" location="m01"/>
+    <hyperlink ref="A32" r:id="rId3" location="m32"/>
+    <hyperlink ref="A36" r:id="rId4" location="m02"/>
+    <hyperlink ref="A43" r:id="rId5" location="m03"/>
+    <hyperlink ref="A44" r:id="rId6" location="m13"/>
+    <hyperlink ref="A45" r:id="rId7" location="m04"/>
+    <hyperlink ref="A46" r:id="rId8" location="m07"/>
+    <hyperlink ref="A57" r:id="rId9" location="m16"/>
+    <hyperlink ref="A76" r:id="rId10" location="m08"/>
+    <hyperlink ref="A77" r:id="rId11" location="m26"/>
+    <hyperlink ref="A79" r:id="rId12" location="m14"/>
+    <hyperlink ref="A80" r:id="rId13" location="m21"/>
+    <hyperlink ref="A81" r:id="rId14" location="m23"/>
+    <hyperlink ref="A82" r:id="rId15" location="m05"/>
+    <hyperlink ref="A87" r:id="rId16" location="m35"/>
+    <hyperlink ref="A88" r:id="rId17" location="m10"/>
+    <hyperlink ref="A89" r:id="rId18" location="m28"/>
+    <hyperlink ref="A90" r:id="rId19" location="m30"/>
+    <hyperlink ref="A91" r:id="rId20" location="m34"/>
+    <hyperlink ref="A106" r:id="rId21" location="m27"/>
+    <hyperlink ref="A108" r:id="rId22" location="m29"/>
+    <hyperlink ref="A109" r:id="rId23" location="m19"/>
+    <hyperlink ref="A110" r:id="rId24" location="m18"/>
+    <hyperlink ref="A111" r:id="rId25" location="m11"/>
+    <hyperlink ref="A112" r:id="rId26" location="m12"/>
+    <hyperlink ref="A113" r:id="rId27" location="m33"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Voeg kennis van KA toe aan M23.
De titel van maatregel M23 is veranderd van "Het project zorgt voor de aanwezigheid van ervaring met de Kwaliteitsaanpak" naar "Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak". Aan de inhoud is toegevoegd dat nieuwe projectleden uitleg over de Kwaliteitsaanpak krijgen.

Closes #794.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -554,8 +554,8 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M23: Het project zorgt voor de aanwezigheid van ervaring met de Kwaliteitsaanpak
-De software delivery manager zorgt ervoor dat bij nieuwe projecten wordt gestart met ten minste twee projectleden die bekend zijn met de Kwaliteitsaanpak.
+          <t xml:space="preserve">M23: Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak
+De software delivery manager zorgt ervoor dat bij nieuwe projecten wordt gestart met ten minste twee projectleden die bekend zijn met de Kwaliteitsaanpak. Projectleden die nog niet bekend zijn met de Kwaliteitsaanpak krijgen uitleg over de inhoud en achtergrond van de Kwaliteitsaanpak.
 Rationale
 Het inzetten van teamleden die bekend zijn met de Kwaliteitsaanpak zorgt voor een soepeler start van een nieuw project omdat zij bekend zijn met de inhoud van de Kwaliteitsaanpak, zoals kwaliteitsnormen en tools, en omdat zij al doende nieuwe teamleden bekend kunnen maken met de Kwaliteitsaanpak.
 </t>
@@ -1172,7 +1172,7 @@
     <t>M23</t>
   </si>
   <si>
-    <t>Het project zorgt voor de aanwezigheid van ervaring met de Kwaliteitsaanpak</t>
+    <t>Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak</t>
   </si>
   <si>
     <t>M05</t>

</xml_diff>

<commit_message>
M13 over ISO-25010 is vervallen.
Maatregel M13 "Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen" is vervallen. Het gebruik van ISO-25010 voor de specificatie van productkwaliteitseisen staat al genoemd in M01 "Het project levert in elke fase vastgestelde producten en informatie op".

Closes #950.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -290,24 +290,6 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M13: Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen
-Voor specificatie en documentatie van vereiste en gewenste kwaliteitseigenschappen, de niet-functionele eisen, maken projecten gebruik van de terminologie en categorisering uit NEN-ISO/IEC 25010:2023. Projecten gebruiken NEN-ISO/IEC 25010:2023 om te controleren of alle relevante kwaliteitseigenschappen van het op te leveren eindproduct worden meegenomen in de ontwikkeling en/of onderhoud van het product.
-De standaard NEN-ISO/IEC 25010:2023 biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. NEN-ISO/IEC 25010:2023 dekt een breed spectrum van kwaliteitseigenschappen af.
-Rationale
-NEN-ISO/IEC 25010:2023 biedt een model voor productkwaliteit. De standaard biedt geen concrete maatregelen, maar biedt wel een begrippenkader en dekt het volledige spectrum van mogelijk relevante kwaliteitseigenschappen af. Het gebruiken van een standaard voor specificatie van kwaliteit voorkomt miscommunicatie over kwaliteitseigenschappen en de breedte van de standaard zorgt ervoor dat alle relevante aspecten aan bod komen.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">M04: Het project borgt de correcte werking van het product met geautomatiseerde regressietests
 Regressietests - tests die verifiëren of eerder ontwikkelde software nog steeds correct werkt na wijzigingen in de software of aansluiting op andere externe koppelvlakken - zijn geautomatiseerd.
 Het project hanteert een norm voor de dekking van regressietests, legt deze vast in Quality-time en bewaakt deze.
@@ -317,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0">
+    <comment ref="B41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -346,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C42" authorId="0">
+    <comment ref="C41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -359,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0">
+    <comment ref="B51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C52" authorId="0">
+    <comment ref="C51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="0">
+    <comment ref="B69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -451,7 +433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -489,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -506,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C76" authorId="0">
+    <comment ref="C75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -542,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="0">
+    <comment ref="B80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -563,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -588,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -615,7 +597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -633,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -665,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C85" authorId="0">
+    <comment ref="C84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -678,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0">
+    <comment ref="B99" authorId="0">
       <text>
         <r>
           <rPr>
@@ -698,7 +680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B102" authorId="0">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -718,7 +700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +719,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -758,7 +740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -777,7 +759,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -795,7 +777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -826,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
@@ -964,12 +946,6 @@
   </si>
   <si>
     <t>Het project zorgt dat het product traceerbaar aan eisen voldoet</t>
-  </si>
-  <si>
-    <t>M13</t>
-  </si>
-  <si>
-    <t>Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen</t>
   </si>
   <si>
     <t>M04</t>
@@ -1684,7 +1660,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2042,23 +2018,21 @@
       <c r="B41" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="8"/>
+      <c r="C41" s="4"/>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="4"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="5"/>
@@ -2066,7 +2040,7 @@
     <row r="44" spans="1:4">
       <c r="A44" s="6"/>
       <c r="B44" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="5"/>
@@ -2074,7 +2048,7 @@
     <row r="45" spans="1:4">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="5"/>
@@ -2082,7 +2056,7 @@
     <row r="46" spans="1:4">
       <c r="A46" s="6"/>
       <c r="B46" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="5"/>
@@ -2090,7 +2064,7 @@
     <row r="47" spans="1:4">
       <c r="A47" s="6"/>
       <c r="B47" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="5"/>
@@ -2098,7 +2072,7 @@
     <row r="48" spans="1:4">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="5"/>
@@ -2106,7 +2080,7 @@
     <row r="49" spans="1:4">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="5"/>
@@ -2114,33 +2088,33 @@
     <row r="50" spans="1:4">
       <c r="A50" s="6"/>
       <c r="B50" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6" t="s">
+      <c r="A51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="4"/>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="6"/>
       <c r="B53" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="5"/>
@@ -2148,7 +2122,7 @@
     <row r="54" spans="1:4">
       <c r="A54" s="6"/>
       <c r="B54" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="5"/>
@@ -2156,7 +2130,7 @@
     <row r="55" spans="1:4">
       <c r="A55" s="6"/>
       <c r="B55" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="5"/>
@@ -2164,7 +2138,7 @@
     <row r="56" spans="1:4">
       <c r="A56" s="6"/>
       <c r="B56" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="5"/>
@@ -2172,7 +2146,7 @@
     <row r="57" spans="1:4">
       <c r="A57" s="6"/>
       <c r="B57" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="5"/>
@@ -2180,7 +2154,7 @@
     <row r="58" spans="1:4">
       <c r="A58" s="6"/>
       <c r="B58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="5"/>
@@ -2188,7 +2162,7 @@
     <row r="59" spans="1:4">
       <c r="A59" s="6"/>
       <c r="B59" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="5"/>
@@ -2196,7 +2170,7 @@
     <row r="60" spans="1:4">
       <c r="A60" s="6"/>
       <c r="B60" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="5"/>
@@ -2204,7 +2178,7 @@
     <row r="61" spans="1:4">
       <c r="A61" s="6"/>
       <c r="B61" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="5"/>
@@ -2212,7 +2186,7 @@
     <row r="62" spans="1:4">
       <c r="A62" s="6"/>
       <c r="B62" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="5"/>
@@ -2220,7 +2194,7 @@
     <row r="63" spans="1:4">
       <c r="A63" s="6"/>
       <c r="B63" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="5"/>
@@ -2228,7 +2202,7 @@
     <row r="64" spans="1:4">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="5"/>
@@ -2236,7 +2210,7 @@
     <row r="65" spans="1:4">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="5"/>
@@ -2244,7 +2218,7 @@
     <row r="66" spans="1:4">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="5"/>
@@ -2252,7 +2226,7 @@
     <row r="67" spans="1:4">
       <c r="A67" s="6"/>
       <c r="B67" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="5"/>
@@ -2260,17 +2234,19 @@
     <row r="68" spans="1:4">
       <c r="A68" s="6"/>
       <c r="B68" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="A69" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="7"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
@@ -2284,22 +2260,22 @@
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="5"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
@@ -2328,23 +2304,21 @@
       <c r="B75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C75" s="8"/>
+      <c r="C75" s="4"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C76" s="4"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="6"/>
       <c r="B77" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="5"/>
@@ -2352,7 +2326,7 @@
     <row r="78" spans="1:4">
       <c r="A78" s="6"/>
       <c r="B78" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="5"/>
@@ -2360,17 +2334,19 @@
     <row r="79" spans="1:4">
       <c r="A79" s="6"/>
       <c r="B79" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6" t="s">
+      <c r="A80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C80" s="7"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
@@ -2410,23 +2386,21 @@
       <c r="B84" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C84" s="8"/>
+      <c r="C84" s="4"/>
       <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C85" s="4"/>
+      <c r="C85" s="7"/>
       <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="6"/>
       <c r="B86" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="5"/>
@@ -2434,7 +2408,7 @@
     <row r="87" spans="1:4">
       <c r="A87" s="6"/>
       <c r="B87" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="5"/>
@@ -2442,7 +2416,7 @@
     <row r="88" spans="1:4">
       <c r="A88" s="6"/>
       <c r="B88" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="5"/>
@@ -2450,7 +2424,7 @@
     <row r="89" spans="1:4">
       <c r="A89" s="6"/>
       <c r="B89" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="5"/>
@@ -2458,7 +2432,7 @@
     <row r="90" spans="1:4">
       <c r="A90" s="6"/>
       <c r="B90" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="5"/>
@@ -2466,7 +2440,7 @@
     <row r="91" spans="1:4">
       <c r="A91" s="6"/>
       <c r="B91" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="5"/>
@@ -2474,7 +2448,7 @@
     <row r="92" spans="1:4">
       <c r="A92" s="6"/>
       <c r="B92" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="5"/>
@@ -2482,7 +2456,7 @@
     <row r="93" spans="1:4">
       <c r="A93" s="6"/>
       <c r="B93" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="5"/>
@@ -2490,7 +2464,7 @@
     <row r="94" spans="1:4">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="5"/>
@@ -2498,7 +2472,7 @@
     <row r="95" spans="1:4">
       <c r="A95" s="6"/>
       <c r="B95" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="5"/>
@@ -2506,7 +2480,7 @@
     <row r="96" spans="1:4">
       <c r="A96" s="6"/>
       <c r="B96" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="5"/>
@@ -2514,7 +2488,7 @@
     <row r="97" spans="1:4">
       <c r="A97" s="6"/>
       <c r="B97" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="5"/>
@@ -2522,36 +2496,38 @@
     <row r="98" spans="1:4">
       <c r="A98" s="6"/>
       <c r="B98" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6" t="s">
+      <c r="A99" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C99" s="7"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="5"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1" t="s">
+      <c r="B101" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="5"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
@@ -2602,16 +2578,6 @@
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="5"/>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2634,7 +2600,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
+  <conditionalFormatting sqref="C101">
     <cfRule type="cellIs" dxfId="0" priority="341" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2718,20 +2684,6 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="cellIs" dxfId="0" priority="365" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="366" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="367" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="368" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3124,7 +3076,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
+  <conditionalFormatting sqref="C42">
     <cfRule type="cellIs" dxfId="0" priority="125" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3250,7 +3202,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="0" priority="161" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3516,7 +3468,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
+  <conditionalFormatting sqref="C72">
     <cfRule type="cellIs" dxfId="0" priority="237" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3558,7 +3510,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
+  <conditionalFormatting sqref="C76">
     <cfRule type="cellIs" dxfId="0" priority="249" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3684,7 +3636,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="281" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3908,7 +3860,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="92">
+  <dataValidations count="91">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4002,7 +3954,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43">
@@ -4029,7 +3981,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53">
@@ -4086,7 +4038,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C70">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C72">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C73">
@@ -4095,7 +4047,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77">
@@ -4119,7 +4071,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
@@ -4164,7 +4116,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C99">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
@@ -4180,9 +4132,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C106">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4191,31 +4140,30 @@
     <hyperlink ref="A28" r:id="rId2" location="m32"/>
     <hyperlink ref="A32" r:id="rId3" location="m02"/>
     <hyperlink ref="A39" r:id="rId4" location="m03"/>
-    <hyperlink ref="A40" r:id="rId5" location="m13"/>
-    <hyperlink ref="A41" r:id="rId6" location="m04"/>
-    <hyperlink ref="A42" r:id="rId7" location="m07"/>
-    <hyperlink ref="A52" r:id="rId8" location="m16"/>
-    <hyperlink ref="A70" r:id="rId9" location="m08"/>
-    <hyperlink ref="A71" r:id="rId10" location="m26"/>
-    <hyperlink ref="A73" r:id="rId11" location="m14"/>
-    <hyperlink ref="A74" r:id="rId12" location="m21"/>
-    <hyperlink ref="A75" r:id="rId13" location="m23"/>
-    <hyperlink ref="A76" r:id="rId14" location="m05"/>
-    <hyperlink ref="A81" r:id="rId15" location="m35"/>
-    <hyperlink ref="A82" r:id="rId16" location="m10"/>
-    <hyperlink ref="A83" r:id="rId17" location="m28"/>
-    <hyperlink ref="A84" r:id="rId18" location="m30"/>
-    <hyperlink ref="A85" r:id="rId19" location="m34"/>
-    <hyperlink ref="A100" r:id="rId20" location="m27"/>
-    <hyperlink ref="A102" r:id="rId21" location="m29"/>
-    <hyperlink ref="A103" r:id="rId22" location="m19"/>
-    <hyperlink ref="A104" r:id="rId23" location="m18"/>
-    <hyperlink ref="A105" r:id="rId24" location="m11"/>
-    <hyperlink ref="A106" r:id="rId25" location="m12"/>
-    <hyperlink ref="A107" r:id="rId26" location="m33"/>
+    <hyperlink ref="A40" r:id="rId5" location="m04"/>
+    <hyperlink ref="A41" r:id="rId6" location="m07"/>
+    <hyperlink ref="A51" r:id="rId7" location="m16"/>
+    <hyperlink ref="A69" r:id="rId8" location="m08"/>
+    <hyperlink ref="A70" r:id="rId9" location="m26"/>
+    <hyperlink ref="A72" r:id="rId10" location="m14"/>
+    <hyperlink ref="A73" r:id="rId11" location="m21"/>
+    <hyperlink ref="A74" r:id="rId12" location="m23"/>
+    <hyperlink ref="A75" r:id="rId13" location="m05"/>
+    <hyperlink ref="A80" r:id="rId14" location="m35"/>
+    <hyperlink ref="A81" r:id="rId15" location="m10"/>
+    <hyperlink ref="A82" r:id="rId16" location="m28"/>
+    <hyperlink ref="A83" r:id="rId17" location="m30"/>
+    <hyperlink ref="A84" r:id="rId18" location="m34"/>
+    <hyperlink ref="A99" r:id="rId19" location="m27"/>
+    <hyperlink ref="A101" r:id="rId20" location="m29"/>
+    <hyperlink ref="A102" r:id="rId21" location="m19"/>
+    <hyperlink ref="A103" r:id="rId22" location="m18"/>
+    <hyperlink ref="A104" r:id="rId23" location="m11"/>
+    <hyperlink ref="A105" r:id="rId24" location="m12"/>
+    <hyperlink ref="A106" r:id="rId25" location="m33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId27"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -4235,7 +4183,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4243,10 +4191,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
In M16 de twee opsommingen gecombineerd in 1 tabel.
In M16 "Het project gebruikt tools voor vastgestelde taken" de opsomming van taken gecombineerd met de opsomming van tools in één tabel.

Closes #937.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -337,12 +337,9 @@
 6. Toegankelijkheidstests,
 7. Broncodekwaliteitscontroles,
 8. Installatie van de software in test, acceptatie en/of productieomgevingen,
-9. Produceren van een "software bill of materials" (SBoM),
-10. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.
+9. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.
 Performance- en beveiligingstests op de software zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats. Performance- en beveiligingstests op de software vinden plaats in de testomgeving van het project. Als ICTU verantwoordelijk is voor het operationeel beheer laat ICTU de performance- en beveiligingstesten op de software (ook) uitvoeren in een productie-like omgeving.
 Niet alle testen en controles kunnen altijd geautomatiseerd worden uitgevoerd. Denk aan kwaliteitscontroles op architectuurbeslissingen of het testen van toegankelijkheidseisen. Waar mogelijk wordt wel een zo groot mogelijk deel van de testen en controles geautomatiseerd en als onderdeel van de pipeline uitgevoerd.
-De afdeling ICTU Software Diensten (ISD) voorziet in tools en ondersteuning, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
-ICTU gebruikt Jenkins, GitLab CI of Azure DevOps als tool voor de implementatie van de continuous delivery pipeline. ISD biedt de projecten een voorziening om releases van het totale product veilig op te leveren aan opdrachtgevende organisaties en beheerorganisaties.
 Rationale
 Software incrementeel opleveren vereist dat de software frequent gebouwd, getest en opgeleverd kan worden. Om dit efficiënt en foutvrij te doen, dient het proces van bouwen, testen en opleveren geautomatiseerd te zijn; een continuous delivery pipeline faciliteert dit.
 </t>
@@ -362,7 +359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="0">
+    <comment ref="B52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -372,50 +369,34 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">M16: Het project gebruikt tools voor vastgestelde taken
-ICTU stelt het gebruik van tools verplicht voor de volgende taken:
-1. product en sprint backlog management en agile werken,
-2. inrichten en uitvoeren van een continuous delivery pipeline,
-3. monitoren van de kwaliteit van broncode,
-4. versiebeheer van op te leveren producten,
-5. release van software,
-6. maken van testrapportages,
-7. maken van kwaliteitsrapportages,
-8. controleren van door de applicatie gebruikte versies van externe software op aanwezigheid van bekende kwetsbaarheden,
-9. statische controle van de software op aanwezigheid van kwetsbare constructies,
-10. dynamische controle van de software op aanwezigheid van kwetsbare constructies,
-11. controleren van container images op aanwezigheid van bekende kwetsbaarheden,
-12. testen van performance en schaalbaarheid,
-13. testen op toegankelijkheid van de applicatie,
-14. produceren van een "software bill of materials" (SBoM),
-15. opslaan van artifacten,
-16. registratie van incidenten bij gebruik en beheer, en
-17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving.
-Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
-ICTU adviseert en ondersteunt voor de genoemde taken onderstaande tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven:
-1. product en sprint backlog management en agile werken: Azure DevOps of Jira,
-2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,
-3. monitoren van de kwaliteit van broncode: SonarQube,
-4. versiebeheer van op te leveren producten: GitLab of Azure DevOps,
-5. release van software: Releaseserver in het ontwikkelplatform,
-6. maken van testrapportages: JUnit, Robot Framework, TestNG, of hiermee compatible tools,
-7. maken van kwaliteitsrapportages: Quality-time,
-8. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,
-9. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,
-10. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,
-11. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,
-12. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,
-13. testen op toegankelijkheid van de applicatie: Axe,
-14. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,
-15. opslaan van artifacten: Nexus of Harbor,
-16. registratie van incidenten bij gebruik en beheer: Jira, en
-17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.
+Voor vastgestelde taken bij het ontwikkelen, onderhouden en operationeel beheren van software, stelt ICTU het gebruik van tools verplicht. ICTU adviseert per taak specifieke tools en ondersteunt projecten bij het gebruik daarvan.
+ICTU adviseert en ondersteunt voor de hieronder genoemde taken specifieke tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven.
+Activiteit                                                                                   Tools                                                                                    
+Product en sprint backlog management en agile werken                                         Azure DevOps of Jira                                                                     
+Inrichten en uitvoeren van een continuous delivery pipeline                                  Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps 
+Monitoren van de kwaliteit van broncode                                                      SonarQube                                                                                
+Versiebeheer van op te leveren producten                                                     GitLab of Azure DevOps                                                                   
+Release van software                                                                         Releaseserver in het ontwikkelplatform                                                   
+Maken van testrapportages                                                                    JUnit, Robot Framework, TestNG, of hiermee compatible tools                              
+Maken van kwaliteitsrapportages                                                              Quality-time                                                                             
+Controleren op aanwezigheid van bekende kwetsbaarheden in externe software                   OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track    
+Statische controle van de software op aanwezigheid van kwetsbare constructies                SonarQube                                                                                
+Dynamische controle van de software op aanwezigheid van kwetsbare constructies               ZAP (Zed Attack Proxy) by Checkmarx                                                      
+Controleren van container images op aanwezigheid van bekende kwetsbaarheden                  Trivy                                                                                    
+Testen van performance en schaalbaarheid                                                     JMeter en Performancetestrunner                                                          
+Testen op toegankelijkheid van de applicatie                                                 Axe                                                                                      
+Produceren van een "software bill of materials" (SBoM)                                       Tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren            
+Opslaan van artifacten                                                                       Nexus of Harbor                                                                          
+Registratie van incidenten bij gebruik en beheer                                             Jira                                                                                     
+Bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving Ansible                                                                                  
+N.B. Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
 Rationale
 Projecten hebben een redelijke vrijheid bij het kiezen en gebruiken van tools, maar voor een aantal taken is het gebruik verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van de Kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren; daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af. Tot slot is het gebruik in een aantal gevallen, ten behoeve van informatiebeveiliging bij de overheid, verplicht.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C53" authorId="0">
+    <comment ref="C52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -428,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B77" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -548,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C77" authorId="0">
+    <comment ref="C76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -561,7 +542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -582,7 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -607,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -634,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -652,7 +633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="0">
+    <comment ref="B85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -684,7 +665,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C86" authorId="0">
+    <comment ref="C85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -697,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B101" authorId="0">
+    <comment ref="B100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -717,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +748,7 @@
           </rPr>
           <t xml:space="preserve">M18: ICTU biedt ondersteuning voor verplicht gestelde tools
 ICTU zorgt voor technische en functionele ondersteuning aan projecten bij het gebruik van alle verplichte tools.
-ICTU zorgt voor ondersteuning van de bij M16: Het project gebruikt tools voor vastgestelde taken verplicht gestelde tools. Een team van specialisten met kennis, ervaring en capaciteit is beschikbaar voor ondersteuning aan projecten.
+ICTU zorgt voor ondersteuning van de in M16: Het project gebruikt tools voor vastgestelde taken verplicht gestelde tools. Een team van specialisten met kennis, ervaring en capaciteit is beschikbaar voor ondersteuning aan projecten. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
 Bij de selectie van tools ter ondersteuning van de projectuitvoering geeft ICTU de voorkeur aan open source tools. Ook tools die ICTU zelf ontwikkelt ter ondersteuning van softwareontwikkelprojecten worden bij voorkeur open source beschikbaar gesteld.
 Rationale
 De keuze om het gebruik van een aantal tools verplicht te stellen (M16: Het project gebruikt tools voor vastgestelde taken) volgt uit de belangrijke rol die die tools spelen in de ontwikkelstraat en in Quality-time, het kwaliteitssysteem van ICTU. Met de verplichting komt ook een verantwoordelijkheid: om projecten in staat te stellen snel en effectief met deze tools te werken, moeten die projecten ondersteund worden.
@@ -777,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -796,7 +777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -814,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B108" authorId="0">
+    <comment ref="B107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -845,7 +826,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
@@ -1027,10 +1008,7 @@
     <t>8. Installatie van de software in test, acceptatie en/of productieomgevingen,</t>
   </si>
   <si>
-    <t>9. Produceren van een "software bill of materials" (SBoM),</t>
-  </si>
-  <si>
-    <t>10. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.</t>
+    <t>9. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.</t>
   </si>
   <si>
     <t>M16</t>
@@ -1039,55 +1017,55 @@
     <t>Het project gebruikt tools voor vastgestelde taken</t>
   </si>
   <si>
-    <t>1. product en sprint backlog management en agile werken: Azure DevOps of Jira,</t>
-  </si>
-  <si>
-    <t>2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,</t>
-  </si>
-  <si>
-    <t>3. monitoren van de kwaliteit van broncode: SonarQube,</t>
-  </si>
-  <si>
-    <t>4. versiebeheer van op te leveren producten: GitLab of Azure DevOps,</t>
-  </si>
-  <si>
-    <t>5. release van software: Releaseserver in het ontwikkelplatform,</t>
-  </si>
-  <si>
-    <t>6. maken van testrapportages: JUnit, Robot Framework, TestNG, of hiermee compatible tools,</t>
-  </si>
-  <si>
-    <t>7. maken van kwaliteitsrapportages: Quality-time,</t>
-  </si>
-  <si>
-    <t>8. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,</t>
-  </si>
-  <si>
-    <t>9. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,</t>
-  </si>
-  <si>
-    <t>10. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,</t>
-  </si>
-  <si>
-    <t>11. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,</t>
-  </si>
-  <si>
-    <t>12. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,</t>
-  </si>
-  <si>
-    <t>13. testen op toegankelijkheid van de applicatie: Axe,</t>
-  </si>
-  <si>
-    <t>14. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,</t>
-  </si>
-  <si>
-    <t>15. opslaan van artifacten: Nexus of Harbor,</t>
-  </si>
-  <si>
-    <t>16. registratie van incidenten bij gebruik en beheer: Jira, en</t>
-  </si>
-  <si>
-    <t>17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.</t>
+    <t>1. Product en sprint backlog management en agile werken</t>
+  </si>
+  <si>
+    <t>2. Inrichten en uitvoeren van een continuous delivery pipeline</t>
+  </si>
+  <si>
+    <t>3. Monitoren van de kwaliteit van broncode</t>
+  </si>
+  <si>
+    <t>4. Versiebeheer van op te leveren producten</t>
+  </si>
+  <si>
+    <t>5. Release van software</t>
+  </si>
+  <si>
+    <t>6. Maken van testrapportages</t>
+  </si>
+  <si>
+    <t>7. Maken van kwaliteitsrapportages</t>
+  </si>
+  <si>
+    <t>8. Controleren op aanwezigheid van bekende kwetsbaarheden in externe software</t>
+  </si>
+  <si>
+    <t>9. Statische controle van de software op aanwezigheid van kwetsbare constructies</t>
+  </si>
+  <si>
+    <t>10. Dynamische controle van de software op aanwezigheid van kwetsbare constructies</t>
+  </si>
+  <si>
+    <t>11. Controleren van container images op aanwezigheid van bekende kwetsbaarheden</t>
+  </si>
+  <si>
+    <t>12. Testen van performance en schaalbaarheid</t>
+  </si>
+  <si>
+    <t>13. Testen op toegankelijkheid van de applicatie</t>
+  </si>
+  <si>
+    <t>14. Produceren van een "software bill of materials" (SBoM)</t>
+  </si>
+  <si>
+    <t>15. Opslaan van artifacten</t>
+  </si>
+  <si>
+    <t>16. Registratie van incidenten bij gebruik en beheer</t>
+  </si>
+  <si>
+    <t>17. Bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving</t>
   </si>
   <si>
     <t>M08</t>
@@ -1706,7 +1684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2150,21 +2128,21 @@
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="7"/>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
@@ -2296,79 +2274,79 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="7"/>
+      <c r="B70" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="8"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="4" t="s">
+      <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="5"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="B73" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B77" s="4" t="s">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="4"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:4">
@@ -2396,61 +2374,61 @@
       <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6" t="s">
+      <c r="A81" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="7"/>
+      <c r="B81" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" s="8"/>
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="5"/>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C85" s="8"/>
+        <v>106</v>
+      </c>
+      <c r="C85" s="4"/>
       <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B86" s="4" t="s">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C86" s="4"/>
+      <c r="C86" s="7"/>
       <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
@@ -2558,90 +2536,82 @@
       <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6" t="s">
+      <c r="A100" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C100" s="7"/>
+      <c r="B100" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="8"/>
       <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B101" s="4" t="s">
+      <c r="A101" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="5"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
+      <c r="B102" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="5"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="5"/>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2678,7 +2648,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
+  <conditionalFormatting sqref="C102">
     <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2762,20 +2732,6 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3308,7 +3264,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C53">
     <cfRule type="cellIs" dxfId="0" priority="165" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3574,7 +3530,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C72">
+  <conditionalFormatting sqref="C73">
     <cfRule type="cellIs" dxfId="0" priority="241" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3616,7 +3572,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C77">
     <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3742,7 +3698,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C86">
     <cfRule type="cellIs" dxfId="0" priority="285" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3952,7 +3908,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="93">
+  <dataValidations count="92">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4076,7 +4032,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54">
@@ -4133,7 +4089,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C72">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C73">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74">
@@ -4142,7 +4098,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C78">
@@ -4166,7 +4122,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C87">
@@ -4211,7 +4167,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103">
@@ -4227,9 +4183,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C108">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4241,25 +4194,25 @@
     <hyperlink ref="A40" r:id="rId5" location="m13"/>
     <hyperlink ref="A41" r:id="rId6" location="m04"/>
     <hyperlink ref="A42" r:id="rId7" location="m07"/>
-    <hyperlink ref="A53" r:id="rId8" location="m16"/>
-    <hyperlink ref="A71" r:id="rId9" location="m08"/>
-    <hyperlink ref="A72" r:id="rId10" location="m26"/>
-    <hyperlink ref="A74" r:id="rId11" location="m14"/>
-    <hyperlink ref="A75" r:id="rId12" location="m21"/>
-    <hyperlink ref="A76" r:id="rId13" location="m23"/>
-    <hyperlink ref="A77" r:id="rId14" location="m05"/>
-    <hyperlink ref="A82" r:id="rId15" location="m35"/>
-    <hyperlink ref="A83" r:id="rId16" location="m10"/>
-    <hyperlink ref="A84" r:id="rId17" location="m28"/>
-    <hyperlink ref="A85" r:id="rId18" location="m30"/>
-    <hyperlink ref="A86" r:id="rId19" location="m34"/>
-    <hyperlink ref="A101" r:id="rId20" location="m27"/>
-    <hyperlink ref="A103" r:id="rId21" location="m29"/>
-    <hyperlink ref="A104" r:id="rId22" location="m19"/>
-    <hyperlink ref="A105" r:id="rId23" location="m18"/>
-    <hyperlink ref="A106" r:id="rId24" location="m11"/>
-    <hyperlink ref="A107" r:id="rId25" location="m12"/>
-    <hyperlink ref="A108" r:id="rId26" location="m33"/>
+    <hyperlink ref="A52" r:id="rId8" location="m16"/>
+    <hyperlink ref="A70" r:id="rId9" location="m08"/>
+    <hyperlink ref="A71" r:id="rId10" location="m26"/>
+    <hyperlink ref="A73" r:id="rId11" location="m14"/>
+    <hyperlink ref="A74" r:id="rId12" location="m21"/>
+    <hyperlink ref="A75" r:id="rId13" location="m23"/>
+    <hyperlink ref="A76" r:id="rId14" location="m05"/>
+    <hyperlink ref="A81" r:id="rId15" location="m35"/>
+    <hyperlink ref="A82" r:id="rId16" location="m10"/>
+    <hyperlink ref="A83" r:id="rId17" location="m28"/>
+    <hyperlink ref="A84" r:id="rId18" location="m30"/>
+    <hyperlink ref="A85" r:id="rId19" location="m34"/>
+    <hyperlink ref="A100" r:id="rId20" location="m27"/>
+    <hyperlink ref="A102" r:id="rId21" location="m29"/>
+    <hyperlink ref="A103" r:id="rId22" location="m19"/>
+    <hyperlink ref="A104" r:id="rId23" location="m18"/>
+    <hyperlink ref="A105" r:id="rId24" location="m11"/>
+    <hyperlink ref="A106" r:id="rId25" location="m12"/>
+    <hyperlink ref="A107" r:id="rId26" location="m33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId27"/>
@@ -4282,7 +4235,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4290,10 +4243,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Hoofdmaatregelen niet scoren bij self-assessments.
Maak het scoren van hoofdmaatregelen onmogelijk bij maatregelen met submaatregelen.

Closes #952.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -76,7 +76,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -204,7 +204,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -240,7 +240,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -295,7 +295,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -395,7 +395,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -596,7 +596,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -732,7 +732,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -889,7 +889,7 @@
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
   <si>
-    <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
+    <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Vul bij maatregelen met submaatregelen alleen de status van de submaatregelen in.</t>
   </si>
   <si>
     <t>Bij maatregelen die primair door een project moeten worden toegepast geeft de status aan in hoevere het project dat doet. Bij maatregelen die primair door ICTU moeten worden toegepast geeft de status aan in hoeverre ICTU dat doet, gezien vanuit het perspectief van het project.</t>
@@ -1387,13 +1387,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFED32D"/>
+        <fgColor rgb="FFFFFFA5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA5"/>
+        <fgColor rgb="FFFED32D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1427,14 +1427,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" indent="1" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1839,40 +1839,40 @@
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
@@ -1881,160 +1881,160 @@
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
@@ -2043,32 +2043,32 @@
       <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
@@ -2077,56 +2077,56 @@
       <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
@@ -2135,8 +2135,8 @@
       <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
@@ -2145,8 +2145,8 @@
       <c r="B44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
@@ -2155,8 +2155,8 @@
       <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
@@ -2165,88 +2165,88 @@
       <c r="B46" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7" t="s">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7" t="s">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7" t="s">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
@@ -2255,152 +2255,152 @@
       <c r="B57" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7" t="s">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="6"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7" t="s">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="5"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="6"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="5"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="6"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="6"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7" t="s">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="6"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7" t="s">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="6"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="5"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7" t="s">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="6"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7" t="s">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="6"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7" t="s">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="6"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="6"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7" t="s">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="6"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7" t="s">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="6"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="6"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7" t="s">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="6"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7" t="s">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="6"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7" t="s">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="6"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7" t="s">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="6"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
@@ -2409,8 +2409,8 @@
       <c r="B76" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="6"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
@@ -2419,8 +2419,8 @@
       <c r="B77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="6"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
@@ -2437,8 +2437,8 @@
       <c r="B79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="6"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
@@ -2447,8 +2447,8 @@
       <c r="B80" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="6"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
@@ -2457,8 +2457,8 @@
       <c r="B81" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="6"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
@@ -2467,40 +2467,40 @@
       <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="6"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7" t="s">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="6"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="5"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7" t="s">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="6"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7" t="s">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="6"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="7"/>
-      <c r="B86" s="7" t="s">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="6"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
@@ -2509,8 +2509,8 @@
       <c r="B87" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="6"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="5"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
@@ -2519,8 +2519,8 @@
       <c r="B88" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="6"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="5"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
@@ -2529,8 +2529,8 @@
       <c r="B89" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="5"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
@@ -2539,8 +2539,8 @@
       <c r="B90" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="6"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="5"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
@@ -2549,120 +2549,120 @@
       <c r="B91" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="6"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="5"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7" t="s">
+      <c r="A92" s="6"/>
+      <c r="B92" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C92" s="8"/>
-      <c r="D92" s="6"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="5"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7" t="s">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="6"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="5"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7" t="s">
+      <c r="A94" s="6"/>
+      <c r="B94" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="8"/>
-      <c r="D94" s="6"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="5"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7" t="s">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="6"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="5"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7" t="s">
+      <c r="A96" s="6"/>
+      <c r="B96" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="6"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="5"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7" t="s">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C97" s="8"/>
-      <c r="D97" s="6"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="5"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7" t="s">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="8"/>
-      <c r="D98" s="6"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7" t="s">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="6"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7" t="s">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="6"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7" t="s">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="6"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="5"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7" t="s">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="6"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="5"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7" t="s">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="6"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7" t="s">
+      <c r="A104" s="6"/>
+      <c r="B104" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="6"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7" t="s">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="6"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
@@ -2671,8 +2671,8 @@
       <c r="B106" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="6"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
@@ -2689,8 +2689,8 @@
       <c r="B108" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="6"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="5"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
@@ -2699,8 +2699,8 @@
       <c r="B109" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="6"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="5"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
@@ -2709,8 +2709,8 @@
       <c r="B110" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C110" s="5"/>
-      <c r="D110" s="6"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="5"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
@@ -2719,8 +2719,8 @@
       <c r="B111" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="6"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="5"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
@@ -2729,8 +2729,8 @@
       <c r="B112" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="6"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="5"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
@@ -2739,8 +2739,8 @@
       <c r="B113" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2750,6 +2750,146 @@
     <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100">
+    <cfRule type="cellIs" dxfId="0" priority="337" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="338" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="339" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="340" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C101">
+    <cfRule type="cellIs" dxfId="0" priority="341" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="342" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="343" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="344" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102">
+    <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="346" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="347" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="348" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C103">
+    <cfRule type="cellIs" dxfId="0" priority="349" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="350" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="351" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="352" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C104">
+    <cfRule type="cellIs" dxfId="0" priority="353" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="354" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="355" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="356" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C105">
+    <cfRule type="cellIs" dxfId="0" priority="357" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="358" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="359" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="360" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106">
+    <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="362" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="363" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="364" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C108">
+    <cfRule type="cellIs" dxfId="0" priority="365" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="366" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="367" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="368" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C109">
+    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2763,21 +2903,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
-    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
+  <conditionalFormatting sqref="C110">
     <cfRule type="cellIs" dxfId="0" priority="373" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2791,7 +2917,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
+  <conditionalFormatting sqref="C111">
     <cfRule type="cellIs" dxfId="0" priority="377" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2805,7 +2931,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C103">
+  <conditionalFormatting sqref="C112">
     <cfRule type="cellIs" dxfId="0" priority="381" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2819,7 +2945,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C104">
+  <conditionalFormatting sqref="C113">
     <cfRule type="cellIs" dxfId="0" priority="385" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2833,63 +2959,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C105">
-    <cfRule type="cellIs" dxfId="0" priority="389" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="390" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="391" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="392" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
-    <cfRule type="cellIs" dxfId="0" priority="393" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="394" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="395" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="396" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="0" priority="397" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="398" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="399" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="400" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C109">
-    <cfRule type="cellIs" dxfId="0" priority="401" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="402" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="403" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="404" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+  <conditionalFormatting sqref="C13">
     <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2903,63 +2973,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C110">
-    <cfRule type="cellIs" dxfId="0" priority="405" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="406" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="407" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="408" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="0" priority="409" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="410" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="411" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="412" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112">
-    <cfRule type="cellIs" dxfId="0" priority="413" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="414" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="415" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="416" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="0" priority="417" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="418" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="419" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="420" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+  <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2973,7 +2987,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2987,7 +3001,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="0" priority="29" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3001,7 +3015,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="0" priority="33" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3015,7 +3029,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+  <conditionalFormatting sqref="C18">
     <cfRule type="cellIs" dxfId="0" priority="37" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3029,7 +3043,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="0" priority="41" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3043,7 +3057,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C20">
     <cfRule type="cellIs" dxfId="0" priority="45" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3057,7 +3071,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="0" priority="49" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3071,7 +3085,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C22">
     <cfRule type="cellIs" dxfId="0" priority="53" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3085,7 +3099,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C23">
     <cfRule type="cellIs" dxfId="0" priority="57" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3099,7 +3113,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
+  <conditionalFormatting sqref="C24">
     <cfRule type="cellIs" dxfId="0" priority="61" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3113,7 +3127,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="0" priority="65" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3127,7 +3141,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+  <conditionalFormatting sqref="C26">
     <cfRule type="cellIs" dxfId="0" priority="69" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3141,7 +3155,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+  <conditionalFormatting sqref="C27">
     <cfRule type="cellIs" dxfId="0" priority="73" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3155,7 +3169,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
+  <conditionalFormatting sqref="C28">
     <cfRule type="cellIs" dxfId="0" priority="77" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3169,7 +3183,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C29">
     <cfRule type="cellIs" dxfId="0" priority="81" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3183,7 +3197,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
+  <conditionalFormatting sqref="C30">
     <cfRule type="cellIs" dxfId="0" priority="85" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3197,7 +3211,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="C31">
     <cfRule type="cellIs" dxfId="0" priority="89" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3211,7 +3225,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="C33">
     <cfRule type="cellIs" dxfId="0" priority="93" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3225,7 +3239,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="0" priority="97" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3239,7 +3253,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
+  <conditionalFormatting sqref="C35">
     <cfRule type="cellIs" dxfId="0" priority="101" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3253,7 +3267,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="0" priority="105" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3267,7 +3281,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C38">
     <cfRule type="cellIs" dxfId="0" priority="109" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3281,7 +3295,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C39">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3295,7 +3309,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C40">
     <cfRule type="cellIs" dxfId="0" priority="117" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3309,7 +3323,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C41">
     <cfRule type="cellIs" dxfId="0" priority="121" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3323,7 +3337,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C42">
     <cfRule type="cellIs" dxfId="0" priority="125" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3337,7 +3351,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="0" priority="129" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3351,7 +3365,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C44">
     <cfRule type="cellIs" dxfId="0" priority="133" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3365,7 +3379,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
+  <conditionalFormatting sqref="C45">
     <cfRule type="cellIs" dxfId="0" priority="137" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3379,7 +3393,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C47">
     <cfRule type="cellIs" dxfId="0" priority="141" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3393,7 +3407,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
+  <conditionalFormatting sqref="C48">
     <cfRule type="cellIs" dxfId="0" priority="145" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3407,7 +3421,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
+  <conditionalFormatting sqref="C49">
     <cfRule type="cellIs" dxfId="0" priority="149" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3421,7 +3435,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
+  <conditionalFormatting sqref="C50">
     <cfRule type="cellIs" dxfId="0" priority="153" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3435,7 +3449,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
+  <conditionalFormatting sqref="C51">
     <cfRule type="cellIs" dxfId="0" priority="157" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3449,7 +3463,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="0" priority="161" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3463,7 +3477,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
+  <conditionalFormatting sqref="C53">
     <cfRule type="cellIs" dxfId="0" priority="165" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3477,7 +3491,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
+  <conditionalFormatting sqref="C54">
     <cfRule type="cellIs" dxfId="0" priority="169" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3491,7 +3505,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
+  <conditionalFormatting sqref="C55">
     <cfRule type="cellIs" dxfId="0" priority="173" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3505,7 +3519,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C56">
     <cfRule type="cellIs" dxfId="0" priority="177" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3519,7 +3533,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="0" priority="181" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3533,7 +3547,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
+  <conditionalFormatting sqref="C59">
     <cfRule type="cellIs" dxfId="0" priority="185" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3547,7 +3561,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+  <conditionalFormatting sqref="C60">
     <cfRule type="cellIs" dxfId="0" priority="189" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3561,7 +3575,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="0" priority="193" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3575,7 +3589,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C62">
     <cfRule type="cellIs" dxfId="0" priority="197" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3589,7 +3603,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
+  <conditionalFormatting sqref="C63">
     <cfRule type="cellIs" dxfId="0" priority="201" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3603,7 +3617,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
+  <conditionalFormatting sqref="C64">
     <cfRule type="cellIs" dxfId="0" priority="205" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3617,7 +3631,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="C65">
     <cfRule type="cellIs" dxfId="0" priority="209" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3631,7 +3645,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C66">
     <cfRule type="cellIs" dxfId="0" priority="213" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3645,7 +3659,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
+  <conditionalFormatting sqref="C67">
     <cfRule type="cellIs" dxfId="0" priority="217" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3659,7 +3673,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
+  <conditionalFormatting sqref="C68">
     <cfRule type="cellIs" dxfId="0" priority="221" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3673,7 +3687,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+  <conditionalFormatting sqref="C69">
     <cfRule type="cellIs" dxfId="0" priority="225" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3687,7 +3701,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
+  <conditionalFormatting sqref="C70">
     <cfRule type="cellIs" dxfId="0" priority="229" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3701,7 +3715,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
+  <conditionalFormatting sqref="C71">
     <cfRule type="cellIs" dxfId="0" priority="233" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3715,7 +3729,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
+  <conditionalFormatting sqref="C72">
     <cfRule type="cellIs" dxfId="0" priority="237" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3729,7 +3743,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
+  <conditionalFormatting sqref="C73">
     <cfRule type="cellIs" dxfId="0" priority="241" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3743,7 +3757,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
+  <conditionalFormatting sqref="C74">
     <cfRule type="cellIs" dxfId="0" priority="245" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3757,7 +3771,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
+  <conditionalFormatting sqref="C75">
     <cfRule type="cellIs" dxfId="0" priority="249" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3771,7 +3785,49 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
+  <conditionalFormatting sqref="C76">
+    <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="254" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="255" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="256" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="cellIs" dxfId="0" priority="257" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="258" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="259" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="260" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79">
+    <cfRule type="cellIs" dxfId="0" priority="261" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="262" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="263" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="264" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3785,49 +3841,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="254" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="255" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="256" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="0" priority="257" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="258" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="259" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="260" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C72">
-    <cfRule type="cellIs" dxfId="0" priority="261" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="262" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="263" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="264" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
+  <conditionalFormatting sqref="C80">
     <cfRule type="cellIs" dxfId="0" priority="265" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3841,7 +3855,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
+  <conditionalFormatting sqref="C81">
     <cfRule type="cellIs" dxfId="0" priority="269" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3855,7 +3869,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
+  <conditionalFormatting sqref="C83">
     <cfRule type="cellIs" dxfId="0" priority="273" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3869,7 +3883,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C84">
     <cfRule type="cellIs" dxfId="0" priority="277" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3883,7 +3897,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="281" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3897,7 +3911,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C79">
+  <conditionalFormatting sqref="C86">
     <cfRule type="cellIs" dxfId="0" priority="285" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3911,7 +3925,49 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C87">
+    <cfRule type="cellIs" dxfId="0" priority="289" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="290" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="291" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="292" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88">
+    <cfRule type="cellIs" dxfId="0" priority="293" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="294" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="295" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="296" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="cellIs" dxfId="0" priority="297" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="298" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="299" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="300" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3925,49 +3981,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="0" priority="289" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="290" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="291" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="292" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C81">
-    <cfRule type="cellIs" dxfId="0" priority="293" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="294" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="295" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="296" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
-    <cfRule type="cellIs" dxfId="0" priority="297" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="298" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="299" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="300" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
+  <conditionalFormatting sqref="C90">
     <cfRule type="cellIs" dxfId="0" priority="301" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3981,7 +3995,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C92">
     <cfRule type="cellIs" dxfId="0" priority="305" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3995,7 +4009,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C93">
     <cfRule type="cellIs" dxfId="0" priority="309" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4009,7 +4023,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C86">
+  <conditionalFormatting sqref="C94">
     <cfRule type="cellIs" dxfId="0" priority="313" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4023,7 +4037,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C87">
+  <conditionalFormatting sqref="C95">
     <cfRule type="cellIs" dxfId="0" priority="317" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4037,7 +4051,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88">
+  <conditionalFormatting sqref="C96">
     <cfRule type="cellIs" dxfId="0" priority="321" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4051,7 +4065,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89">
+  <conditionalFormatting sqref="C97">
     <cfRule type="cellIs" dxfId="0" priority="325" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4065,21 +4079,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C90">
+  <conditionalFormatting sqref="C98">
     <cfRule type="cellIs" dxfId="0" priority="329" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4093,7 +4093,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
+  <conditionalFormatting sqref="C99">
     <cfRule type="cellIs" dxfId="0" priority="333" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4107,122 +4107,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C92">
-    <cfRule type="cellIs" dxfId="0" priority="337" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="338" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="339" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="340" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C93">
-    <cfRule type="cellIs" dxfId="0" priority="341" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="342" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="343" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="344" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C94">
-    <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="346" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="347" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="348" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="cellIs" dxfId="0" priority="349" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="350" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="351" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="352" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C96">
-    <cfRule type="cellIs" dxfId="0" priority="353" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="354" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="355" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="356" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
-    <cfRule type="cellIs" dxfId="0" priority="357" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="358" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="359" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="360" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="362" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="363" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="364" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C99">
-    <cfRule type="cellIs" dxfId="0" priority="365" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="366" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="367" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="368" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="105">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
+  <dataValidations count="97">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4235,9 +4120,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4295,9 +4177,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4307,9 +4186,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C35">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C37">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4337,9 +4213,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C45">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C46">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4370,9 +4243,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C56">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4442,9 +4312,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C81">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C82">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4467,9 +4334,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C90">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C91">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C92">

</xml_diff>

<commit_message>
Link maatregelen in self-assessment checklist. (#1022)
De maatregelennummers in de self-assessment checklist linken naar de bijbehorende maatregelen in de online versie van de Kwaliteitsaanpak.

Closes #957.

Co-authored-by: dependabot[bot] <49699333+dependabot[bot]@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -886,7 +886,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 04-03-2025.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
@@ -1328,7 +1328,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1346,6 +1346,14 @@
     </font>
     <font>
       <sz val="13"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1402,13 +1410,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1825,591 +1836,591 @@
       <c r="A7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6" t="s">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="6"/>
-      <c r="B9" s="6" t="s">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="6"/>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="7"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="6"/>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="6"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="6"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6" t="s">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="6"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="6"/>
-      <c r="B16" s="6" t="s">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="6"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="6"/>
-      <c r="B18" s="6" t="s">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="6"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6" t="s">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="6"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="6"/>
-      <c r="B20" s="6" t="s">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="7"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="6"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="6"/>
-      <c r="B21" s="6" t="s">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="6"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="6"/>
-      <c r="B22" s="6" t="s">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="7"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="6"/>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="7"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="6"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="6"/>
-      <c r="B24" s="6" t="s">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="7"/>
-      <c r="D24" s="5"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="6"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="6"/>
-      <c r="B25" s="6" t="s">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6" t="s">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6" t="s">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="6"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6" t="s">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="7"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="6"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6" t="s">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="6"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="6"/>
-      <c r="B30" s="6" t="s">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="6"/>
-      <c r="B31" s="6" t="s">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="7"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="6"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="6"/>
-      <c r="B33" s="6" t="s">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="7"/>
-      <c r="D33" s="5"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="6"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="6"/>
-      <c r="B34" s="6" t="s">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="7"/>
-      <c r="D34" s="5"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="6"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="6"/>
-      <c r="B35" s="6" t="s">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="7"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="8"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="6"/>
-      <c r="B37" s="6" t="s">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="7"/>
-      <c r="D37" s="5"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="6"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6" t="s">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="7"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="6"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="6"/>
-      <c r="B39" s="6" t="s">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="5"/>
+      <c r="C39" s="8"/>
+      <c r="D39" s="6"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="7"/>
-      <c r="D40" s="5"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="6"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6" t="s">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="7"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="6"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="6"/>
-      <c r="B42" s="6" t="s">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="7"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="8"/>
+      <c r="D42" s="6"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="4"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6" t="s">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="7"/>
-      <c r="D47" s="5"/>
+      <c r="C47" s="8"/>
+      <c r="D47" s="6"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6" t="s">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="5"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="6"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6" t="s">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="7"/>
-      <c r="D49" s="5"/>
+      <c r="C49" s="8"/>
+      <c r="D49" s="6"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6" t="s">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="7"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="6"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6" t="s">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="7"/>
-      <c r="D51" s="5"/>
+      <c r="C51" s="8"/>
+      <c r="D51" s="6"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="6"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6" t="s">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="7"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="6"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6" t="s">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="7"/>
-      <c r="D54" s="5"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="6"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6" t="s">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="7"/>
-      <c r="D55" s="5"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="6"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="6"/>
-      <c r="B56" s="6" t="s">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="7"/>
-      <c r="D56" s="5"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="6"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="4"/>
-      <c r="D57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="6"/>
-      <c r="B58" s="6" t="s">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="7"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="6"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6" t="s">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="6"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="6"/>
-      <c r="B60" s="6" t="s">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="7"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="6"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="6"/>
-      <c r="B61" s="6" t="s">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="7"/>
-      <c r="D61" s="5"/>
+      <c r="C61" s="8"/>
+      <c r="D61" s="6"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="6"/>
-      <c r="B62" s="6" t="s">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="5"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="6"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="6"/>
-      <c r="B63" s="6" t="s">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="7"/>
-      <c r="D63" s="5"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="6"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="6"/>
-      <c r="B64" s="6" t="s">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="C64" s="7"/>
-      <c r="D64" s="5"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="6"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="6"/>
-      <c r="B65" s="6" t="s">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="7"/>
-      <c r="D65" s="5"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="6"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="6"/>
-      <c r="B66" s="6" t="s">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="7"/>
-      <c r="D66" s="5"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="6"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="6"/>
-      <c r="B67" s="6" t="s">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="7"/>
-      <c r="D67" s="5"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="6"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="6"/>
-      <c r="B68" s="6" t="s">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="7"/>
-      <c r="D68" s="5"/>
+      <c r="C68" s="8"/>
+      <c r="D68" s="6"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C69" s="7"/>
-      <c r="D69" s="5"/>
+      <c r="C69" s="8"/>
+      <c r="D69" s="6"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="7"/>
-      <c r="D70" s="5"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="6"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="6"/>
-      <c r="B71" s="6" t="s">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="7"/>
-      <c r="D71" s="5"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="6"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="6"/>
-      <c r="B72" s="6" t="s">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="7"/>
-      <c r="D72" s="5"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="6"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="6"/>
-      <c r="B73" s="6" t="s">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="7"/>
-      <c r="D73" s="5"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="6"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="6"/>
-      <c r="B74" s="6" t="s">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="7"/>
-      <c r="D74" s="5"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="6"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6" t="s">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="7"/>
-      <c r="D75" s="5"/>
+      <c r="C75" s="8"/>
+      <c r="D75" s="6"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="B76" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="6"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B77" s="3" t="s">
+      <c r="B77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="4"/>
-      <c r="D77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="6"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
@@ -2423,245 +2434,245 @@
       <c r="A79" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C79" s="4"/>
-      <c r="D79" s="5"/>
+      <c r="C79" s="5"/>
+      <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B80" s="3" t="s">
+      <c r="B80" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C80" s="4"/>
-      <c r="D80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B81" s="3" t="s">
+      <c r="B81" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="4"/>
-      <c r="D81" s="5"/>
+      <c r="C81" s="5"/>
+      <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B82" s="3" t="s">
+      <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="4"/>
-      <c r="D82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="6"/>
-      <c r="B83" s="6" t="s">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="7"/>
-      <c r="D83" s="5"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="6"/>
-      <c r="B84" s="6" t="s">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="7"/>
-      <c r="D84" s="5"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="6"/>
-      <c r="B85" s="6" t="s">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="7"/>
-      <c r="D85" s="5"/>
+      <c r="C85" s="8"/>
+      <c r="D85" s="6"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6" t="s">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="7"/>
-      <c r="D86" s="5"/>
+      <c r="C86" s="8"/>
+      <c r="D86" s="6"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B87" s="3" t="s">
+      <c r="B87" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C87" s="4"/>
-      <c r="D87" s="5"/>
+      <c r="C87" s="5"/>
+      <c r="D87" s="6"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="B88" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C88" s="4"/>
-      <c r="D88" s="5"/>
+      <c r="C88" s="5"/>
+      <c r="D88" s="6"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="3" t="s">
+      <c r="B89" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C89" s="4"/>
-      <c r="D89" s="5"/>
+      <c r="C89" s="5"/>
+      <c r="D89" s="6"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B90" s="3" t="s">
+      <c r="B90" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="4"/>
-      <c r="D90" s="5"/>
+      <c r="C90" s="5"/>
+      <c r="D90" s="6"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="B91" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C91" s="4"/>
-      <c r="D91" s="5"/>
+      <c r="C91" s="5"/>
+      <c r="D91" s="6"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="6"/>
-      <c r="B92" s="6" t="s">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C92" s="7"/>
-      <c r="D92" s="5"/>
+      <c r="C92" s="8"/>
+      <c r="D92" s="6"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="6"/>
-      <c r="B93" s="6" t="s">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="C93" s="7"/>
-      <c r="D93" s="5"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="6"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="6"/>
-      <c r="B94" s="6" t="s">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="7"/>
-      <c r="D94" s="5"/>
+      <c r="C94" s="8"/>
+      <c r="D94" s="6"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="6"/>
-      <c r="B95" s="6" t="s">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="C95" s="7"/>
-      <c r="D95" s="5"/>
+      <c r="C95" s="8"/>
+      <c r="D95" s="6"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="6"/>
-      <c r="B96" s="6" t="s">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C96" s="7"/>
-      <c r="D96" s="5"/>
+      <c r="C96" s="8"/>
+      <c r="D96" s="6"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="6"/>
-      <c r="B97" s="6" t="s">
+      <c r="A97" s="7"/>
+      <c r="B97" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="C97" s="7"/>
-      <c r="D97" s="5"/>
+      <c r="C97" s="8"/>
+      <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="6"/>
-      <c r="B98" s="6" t="s">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="7"/>
-      <c r="D98" s="5"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="6"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6" t="s">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="7"/>
-      <c r="D99" s="5"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="6"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6" t="s">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="7"/>
-      <c r="D100" s="5"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="6"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="6"/>
-      <c r="B101" s="6" t="s">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="7"/>
-      <c r="D101" s="5"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="6"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="6"/>
-      <c r="B102" s="6" t="s">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="C102" s="7"/>
-      <c r="D102" s="5"/>
+      <c r="C102" s="8"/>
+      <c r="D102" s="6"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="6"/>
-      <c r="B103" s="6" t="s">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C103" s="7"/>
-      <c r="D103" s="5"/>
+      <c r="C103" s="8"/>
+      <c r="D103" s="6"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="6"/>
-      <c r="B104" s="6" t="s">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="7"/>
-      <c r="D104" s="5"/>
+      <c r="C104" s="8"/>
+      <c r="D104" s="6"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6" t="s">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="C105" s="7"/>
-      <c r="D105" s="5"/>
+      <c r="C105" s="8"/>
+      <c r="D105" s="6"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="B106" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="5"/>
+      <c r="C106" s="5"/>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
@@ -2675,61 +2686,61 @@
       <c r="A108" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="B108" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C108" s="4"/>
-      <c r="D108" s="5"/>
+      <c r="C108" s="5"/>
+      <c r="D108" s="6"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B109" s="3" t="s">
+      <c r="B109" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C109" s="4"/>
-      <c r="D109" s="5"/>
+      <c r="C109" s="5"/>
+      <c r="D109" s="6"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="B110" s="3" t="s">
+      <c r="B110" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C110" s="4"/>
-      <c r="D110" s="5"/>
+      <c r="C110" s="5"/>
+      <c r="D110" s="6"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="B111" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C111" s="4"/>
-      <c r="D111" s="5"/>
+      <c r="C111" s="5"/>
+      <c r="D111" s="6"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B112" s="3" t="s">
+      <c r="B112" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C112" s="4"/>
-      <c r="D112" s="5"/>
+      <c r="C112" s="5"/>
+      <c r="D112" s="6"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="B113" s="3" t="s">
+      <c r="B113" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C113" s="4"/>
-      <c r="D113" s="5"/>
+      <c r="C113" s="5"/>
+      <c r="D113" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4525,8 +4536,37 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A7" r:id="rId1" location="m31"/>
+    <hyperlink ref="A12" r:id="rId2" location="m01"/>
+    <hyperlink ref="A32" r:id="rId3" location="m32"/>
+    <hyperlink ref="A36" r:id="rId4" location="m02"/>
+    <hyperlink ref="A43" r:id="rId5" location="m03"/>
+    <hyperlink ref="A44" r:id="rId6" location="m13"/>
+    <hyperlink ref="A45" r:id="rId7" location="m04"/>
+    <hyperlink ref="A46" r:id="rId8" location="m07"/>
+    <hyperlink ref="A57" r:id="rId9" location="m16"/>
+    <hyperlink ref="A76" r:id="rId10" location="m08"/>
+    <hyperlink ref="A77" r:id="rId11" location="m26"/>
+    <hyperlink ref="A79" r:id="rId12" location="m14"/>
+    <hyperlink ref="A80" r:id="rId13" location="m21"/>
+    <hyperlink ref="A81" r:id="rId14" location="m23"/>
+    <hyperlink ref="A82" r:id="rId15" location="m05"/>
+    <hyperlink ref="A87" r:id="rId16" location="m35"/>
+    <hyperlink ref="A88" r:id="rId17" location="m10"/>
+    <hyperlink ref="A89" r:id="rId18" location="m28"/>
+    <hyperlink ref="A90" r:id="rId19" location="m30"/>
+    <hyperlink ref="A91" r:id="rId20" location="m34"/>
+    <hyperlink ref="A106" r:id="rId21" location="m27"/>
+    <hyperlink ref="A108" r:id="rId22" location="m29"/>
+    <hyperlink ref="A109" r:id="rId23" location="m19"/>
+    <hyperlink ref="A110" r:id="rId24" location="m18"/>
+    <hyperlink ref="A111" r:id="rId25" location="m11"/>
+    <hyperlink ref="A112" r:id="rId26" location="m12"/>
+    <hyperlink ref="A113" r:id="rId27" location="m33"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId28"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Hoofdmaatregelen niet scoren bij self-assessments. (#1021)
Maak het scoren van hoofdmaatregelen onmogelijk bij maatregelen met submaatregelen.

Closes #952.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -76,7 +76,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -204,7 +204,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -240,7 +240,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -295,7 +295,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -395,7 +395,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -463,7 +463,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -596,7 +596,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -732,7 +732,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tip: bepaal eerst de status per submaatregel en daarna de status van de hoofdmaatregel.</t>
+          <t>Bepaal a.u.b. de status per submaatregel.</t>
         </r>
       </text>
     </comment>
@@ -889,7 +889,7 @@
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
   <si>
-    <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Bij maatregelen met submaatregelen hoeft alleen de status van de submaatregelen te worden ingevuld.</t>
+    <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Vul bij maatregelen met submaatregelen alleen de status van de submaatregelen in.</t>
   </si>
   <si>
     <t>Bij maatregelen die primair door een project moeten worden toegepast geeft de status aan in hoevere het project dat doet. Bij maatregelen die primair door ICTU moeten worden toegepast geeft de status aan in hoeverre ICTU dat doet, gezien vanuit het perspectief van het project.</t>
@@ -1387,13 +1387,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFED32D"/>
+        <fgColor rgb="FFFFFFA5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFA5"/>
+        <fgColor rgb="FFFED32D"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1427,14 +1427,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" indent="1" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1839,40 +1839,40 @@
       <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="6"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="6"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="6"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="8"/>
-      <c r="D11" s="6"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
@@ -1881,160 +1881,160 @@
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7" t="s">
+      <c r="A13" s="6"/>
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="6"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="6"/>
+      <c r="B15" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7" t="s">
+      <c r="A16" s="6"/>
+      <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7" t="s">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7" t="s">
+      <c r="A18" s="6"/>
+      <c r="B18" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7" t="s">
+      <c r="A19" s="6"/>
+      <c r="B19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7" t="s">
+      <c r="A20" s="6"/>
+      <c r="B20" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
+      <c r="A21" s="6"/>
+      <c r="B21" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7" t="s">
+      <c r="A22" s="6"/>
+      <c r="B22" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7" t="s">
+      <c r="A23" s="6"/>
+      <c r="B23" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7" t="s">
+      <c r="A24" s="6"/>
+      <c r="B24" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7" t="s">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7" t="s">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7" t="s">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="5"/>
     </row>
     <row r="29" spans="1:4">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7" t="s">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7" t="s">
+      <c r="A30" s="6"/>
+      <c r="B30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7" t="s">
+      <c r="A31" s="6"/>
+      <c r="B31" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
@@ -2043,32 +2043,32 @@
       <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7" t="s">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7" t="s">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="8"/>
-      <c r="D34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
@@ -2077,56 +2077,56 @@
       <c r="B36" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="6"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7" t="s">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7" t="s">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
@@ -2135,8 +2135,8 @@
       <c r="B43" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
@@ -2145,8 +2145,8 @@
       <c r="B44" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
@@ -2155,8 +2155,8 @@
       <c r="B45" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
@@ -2165,88 +2165,88 @@
       <c r="B46" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7" t="s">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7" t="s">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7" t="s">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C49" s="8"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7" t="s">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="C50" s="8"/>
-      <c r="D50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7" t="s">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C51" s="8"/>
-      <c r="D51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C52" s="8"/>
-      <c r="D52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="8"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7" t="s">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C54" s="8"/>
-      <c r="D54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7" t="s">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="C55" s="8"/>
-      <c r="D55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7" t="s">
+      <c r="A56" s="6"/>
+      <c r="B56" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C56" s="8"/>
-      <c r="D56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="5"/>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
@@ -2255,152 +2255,152 @@
       <c r="B57" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="6"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7" t="s">
+      <c r="A58" s="6"/>
+      <c r="B58" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="C58" s="8"/>
-      <c r="D58" s="6"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="7"/>
-      <c r="B59" s="7" t="s">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C59" s="8"/>
-      <c r="D59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="5"/>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="7"/>
-      <c r="B60" s="7" t="s">
+      <c r="A60" s="6"/>
+      <c r="B60" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="6"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="5"/>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="7"/>
-      <c r="B61" s="7" t="s">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="8"/>
-      <c r="D61" s="6"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7" t="s">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="8"/>
-      <c r="D62" s="6"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4">
-      <c r="A63" s="7"/>
-      <c r="B63" s="7" t="s">
+      <c r="A63" s="6"/>
+      <c r="B63" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C63" s="8"/>
-      <c r="D63" s="6"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="7"/>
-      <c r="B64" s="7" t="s">
+      <c r="A64" s="6"/>
+      <c r="B64" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="C64" s="8"/>
-      <c r="D64" s="6"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="5"/>
     </row>
     <row r="65" spans="1:4">
-      <c r="A65" s="7"/>
-      <c r="B65" s="7" t="s">
+      <c r="A65" s="6"/>
+      <c r="B65" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C65" s="8"/>
-      <c r="D65" s="6"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
-      <c r="A66" s="7"/>
-      <c r="B66" s="7" t="s">
+      <c r="A66" s="6"/>
+      <c r="B66" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="C66" s="8"/>
-      <c r="D66" s="6"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
-      <c r="A67" s="7"/>
-      <c r="B67" s="7" t="s">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="8"/>
-      <c r="D67" s="6"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
-      <c r="A68" s="7"/>
-      <c r="B68" s="7" t="s">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="8"/>
-      <c r="D68" s="6"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="7"/>
-      <c r="B69" s="7" t="s">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="C69" s="8"/>
-      <c r="D69" s="6"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="7"/>
-      <c r="B70" s="7" t="s">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="C70" s="8"/>
-      <c r="D70" s="6"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="7"/>
-      <c r="B71" s="7" t="s">
+      <c r="A71" s="6"/>
+      <c r="B71" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="6"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="7"/>
-      <c r="B72" s="7" t="s">
+      <c r="A72" s="6"/>
+      <c r="B72" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="6"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="7"/>
-      <c r="B73" s="7" t="s">
+      <c r="A73" s="6"/>
+      <c r="B73" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="6"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
-      <c r="A74" s="7"/>
-      <c r="B74" s="7" t="s">
+      <c r="A74" s="6"/>
+      <c r="B74" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="8"/>
-      <c r="D74" s="6"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="7"/>
-      <c r="B75" s="7" t="s">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="8"/>
-      <c r="D75" s="6"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
@@ -2409,8 +2409,8 @@
       <c r="B76" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="6"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
@@ -2419,8 +2419,8 @@
       <c r="B77" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="6"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="1" t="s">
@@ -2437,8 +2437,8 @@
       <c r="B79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="6"/>
+      <c r="C79" s="8"/>
+      <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
@@ -2447,8 +2447,8 @@
       <c r="B80" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C80" s="5"/>
-      <c r="D80" s="6"/>
+      <c r="C80" s="8"/>
+      <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
@@ -2457,8 +2457,8 @@
       <c r="B81" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="6"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
@@ -2467,40 +2467,40 @@
       <c r="B82" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="6"/>
+      <c r="C82" s="4"/>
+      <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="7"/>
-      <c r="B83" s="7" t="s">
+      <c r="A83" s="6"/>
+      <c r="B83" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="C83" s="8"/>
-      <c r="D83" s="6"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="5"/>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="7"/>
-      <c r="B84" s="7" t="s">
+      <c r="A84" s="6"/>
+      <c r="B84" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="8"/>
-      <c r="D84" s="6"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="7"/>
-      <c r="B85" s="7" t="s">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="C85" s="8"/>
-      <c r="D85" s="6"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="7"/>
-      <c r="B86" s="7" t="s">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="8"/>
-      <c r="D86" s="6"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
@@ -2509,8 +2509,8 @@
       <c r="B87" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="6"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="5"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
@@ -2519,8 +2519,8 @@
       <c r="B88" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C88" s="5"/>
-      <c r="D88" s="6"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="5"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
@@ -2529,8 +2529,8 @@
       <c r="B89" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="6"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="5"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
@@ -2539,8 +2539,8 @@
       <c r="B90" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="6"/>
+      <c r="C90" s="8"/>
+      <c r="D90" s="5"/>
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
@@ -2549,120 +2549,120 @@
       <c r="B91" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="6"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="5"/>
     </row>
     <row r="92" spans="1:4">
-      <c r="A92" s="7"/>
-      <c r="B92" s="7" t="s">
+      <c r="A92" s="6"/>
+      <c r="B92" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="C92" s="8"/>
-      <c r="D92" s="6"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="5"/>
     </row>
     <row r="93" spans="1:4">
-      <c r="A93" s="7"/>
-      <c r="B93" s="7" t="s">
+      <c r="A93" s="6"/>
+      <c r="B93" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C93" s="8"/>
-      <c r="D93" s="6"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="5"/>
     </row>
     <row r="94" spans="1:4">
-      <c r="A94" s="7"/>
-      <c r="B94" s="7" t="s">
+      <c r="A94" s="6"/>
+      <c r="B94" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="C94" s="8"/>
-      <c r="D94" s="6"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="5"/>
     </row>
     <row r="95" spans="1:4">
-      <c r="A95" s="7"/>
-      <c r="B95" s="7" t="s">
+      <c r="A95" s="6"/>
+      <c r="B95" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C95" s="8"/>
-      <c r="D95" s="6"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="5"/>
     </row>
     <row r="96" spans="1:4">
-      <c r="A96" s="7"/>
-      <c r="B96" s="7" t="s">
+      <c r="A96" s="6"/>
+      <c r="B96" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="C96" s="8"/>
-      <c r="D96" s="6"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="5"/>
     </row>
     <row r="97" spans="1:4">
-      <c r="A97" s="7"/>
-      <c r="B97" s="7" t="s">
+      <c r="A97" s="6"/>
+      <c r="B97" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C97" s="8"/>
-      <c r="D97" s="6"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="5"/>
     </row>
     <row r="98" spans="1:4">
-      <c r="A98" s="7"/>
-      <c r="B98" s="7" t="s">
+      <c r="A98" s="6"/>
+      <c r="B98" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="C98" s="8"/>
-      <c r="D98" s="6"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="7"/>
-      <c r="B99" s="7" t="s">
+      <c r="A99" s="6"/>
+      <c r="B99" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C99" s="8"/>
-      <c r="D99" s="6"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="7"/>
-      <c r="B100" s="7" t="s">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="6"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="7"/>
-      <c r="B101" s="7" t="s">
+      <c r="A101" s="6"/>
+      <c r="B101" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="6"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="5"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="7"/>
-      <c r="B102" s="7" t="s">
+      <c r="A102" s="6"/>
+      <c r="B102" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="6"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="5"/>
     </row>
     <row r="103" spans="1:4">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7" t="s">
+      <c r="A103" s="6"/>
+      <c r="B103" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="C103" s="8"/>
-      <c r="D103" s="6"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7" t="s">
+      <c r="A104" s="6"/>
+      <c r="B104" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C104" s="8"/>
-      <c r="D104" s="6"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7" t="s">
+      <c r="A105" s="6"/>
+      <c r="B105" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="C105" s="8"/>
-      <c r="D105" s="6"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
@@ -2671,8 +2671,8 @@
       <c r="B106" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="6"/>
+      <c r="C106" s="8"/>
+      <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="1" t="s">
@@ -2689,8 +2689,8 @@
       <c r="B108" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="6"/>
+      <c r="C108" s="8"/>
+      <c r="D108" s="5"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
@@ -2699,8 +2699,8 @@
       <c r="B109" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="6"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="5"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
@@ -2709,8 +2709,8 @@
       <c r="B110" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C110" s="5"/>
-      <c r="D110" s="6"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="5"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
@@ -2719,8 +2719,8 @@
       <c r="B111" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="6"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="5"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
@@ -2729,8 +2729,8 @@
       <c r="B112" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="6"/>
+      <c r="C112" s="8"/>
+      <c r="D112" s="5"/>
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
@@ -2739,8 +2739,8 @@
       <c r="B113" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="C113" s="5"/>
-      <c r="D113" s="6"/>
+      <c r="C113" s="8"/>
+      <c r="D113" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2750,6 +2750,146 @@
     <mergeCell ref="A4:D4"/>
   </mergeCells>
   <conditionalFormatting sqref="C10">
+    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C100">
+    <cfRule type="cellIs" dxfId="0" priority="337" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="338" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="339" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="340" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C101">
+    <cfRule type="cellIs" dxfId="0" priority="341" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="342" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="343" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="344" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C102">
+    <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="346" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="347" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="348" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C103">
+    <cfRule type="cellIs" dxfId="0" priority="349" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="350" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="351" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="352" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C104">
+    <cfRule type="cellIs" dxfId="0" priority="353" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="354" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="355" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="356" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C105">
+    <cfRule type="cellIs" dxfId="0" priority="357" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="358" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="359" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="360" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C106">
+    <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="362" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="363" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="364" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C108">
+    <cfRule type="cellIs" dxfId="0" priority="365" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="366" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="367" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="368" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C109">
+    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2763,21 +2903,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
-    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
+  <conditionalFormatting sqref="C110">
     <cfRule type="cellIs" dxfId="0" priority="373" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2791,7 +2917,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
+  <conditionalFormatting sqref="C111">
     <cfRule type="cellIs" dxfId="0" priority="377" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2805,7 +2931,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C103">
+  <conditionalFormatting sqref="C112">
     <cfRule type="cellIs" dxfId="0" priority="381" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2819,7 +2945,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C104">
+  <conditionalFormatting sqref="C113">
     <cfRule type="cellIs" dxfId="0" priority="385" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2833,63 +2959,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C105">
-    <cfRule type="cellIs" dxfId="0" priority="389" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="390" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="391" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="392" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
-    <cfRule type="cellIs" dxfId="0" priority="393" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="394" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="395" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="396" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="0" priority="397" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="398" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="399" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="400" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C109">
-    <cfRule type="cellIs" dxfId="0" priority="401" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="402" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="403" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="404" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C11">
+  <conditionalFormatting sqref="C13">
     <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2903,63 +2973,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C110">
-    <cfRule type="cellIs" dxfId="0" priority="405" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="406" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="407" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="408" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C111">
-    <cfRule type="cellIs" dxfId="0" priority="409" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="410" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="411" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="412" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C112">
-    <cfRule type="cellIs" dxfId="0" priority="413" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="414" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="415" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="416" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="0" priority="417" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="418" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="419" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="420" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12">
+  <conditionalFormatting sqref="C14">
     <cfRule type="cellIs" dxfId="0" priority="21" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2973,7 +2987,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C13">
+  <conditionalFormatting sqref="C15">
     <cfRule type="cellIs" dxfId="0" priority="25" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2987,7 +3001,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
+  <conditionalFormatting sqref="C16">
     <cfRule type="cellIs" dxfId="0" priority="29" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3001,7 +3015,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
+  <conditionalFormatting sqref="C17">
     <cfRule type="cellIs" dxfId="0" priority="33" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3015,7 +3029,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C16">
+  <conditionalFormatting sqref="C18">
     <cfRule type="cellIs" dxfId="0" priority="37" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3029,7 +3043,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17">
+  <conditionalFormatting sqref="C19">
     <cfRule type="cellIs" dxfId="0" priority="41" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3043,7 +3057,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18">
+  <conditionalFormatting sqref="C20">
     <cfRule type="cellIs" dxfId="0" priority="45" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3057,7 +3071,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19">
+  <conditionalFormatting sqref="C21">
     <cfRule type="cellIs" dxfId="0" priority="49" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3071,7 +3085,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C20">
+  <conditionalFormatting sqref="C22">
     <cfRule type="cellIs" dxfId="0" priority="53" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3085,7 +3099,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C21">
+  <conditionalFormatting sqref="C23">
     <cfRule type="cellIs" dxfId="0" priority="57" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3099,7 +3113,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C22">
+  <conditionalFormatting sqref="C24">
     <cfRule type="cellIs" dxfId="0" priority="61" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3113,7 +3127,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C23">
+  <conditionalFormatting sqref="C25">
     <cfRule type="cellIs" dxfId="0" priority="65" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3127,7 +3141,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C24">
+  <conditionalFormatting sqref="C26">
     <cfRule type="cellIs" dxfId="0" priority="69" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3141,7 +3155,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C25">
+  <conditionalFormatting sqref="C27">
     <cfRule type="cellIs" dxfId="0" priority="73" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3155,7 +3169,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C26">
+  <conditionalFormatting sqref="C28">
     <cfRule type="cellIs" dxfId="0" priority="77" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3169,7 +3183,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C27">
+  <conditionalFormatting sqref="C29">
     <cfRule type="cellIs" dxfId="0" priority="81" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3183,7 +3197,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C28">
+  <conditionalFormatting sqref="C30">
     <cfRule type="cellIs" dxfId="0" priority="85" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3197,7 +3211,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C29">
+  <conditionalFormatting sqref="C31">
     <cfRule type="cellIs" dxfId="0" priority="89" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3211,7 +3225,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C30">
+  <conditionalFormatting sqref="C33">
     <cfRule type="cellIs" dxfId="0" priority="93" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3225,7 +3239,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C31">
+  <conditionalFormatting sqref="C34">
     <cfRule type="cellIs" dxfId="0" priority="97" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3239,7 +3253,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C32">
+  <conditionalFormatting sqref="C35">
     <cfRule type="cellIs" dxfId="0" priority="101" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3253,7 +3267,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C33">
+  <conditionalFormatting sqref="C37">
     <cfRule type="cellIs" dxfId="0" priority="105" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3267,7 +3281,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C34">
+  <conditionalFormatting sqref="C38">
     <cfRule type="cellIs" dxfId="0" priority="109" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3281,7 +3295,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C35">
+  <conditionalFormatting sqref="C39">
     <cfRule type="cellIs" dxfId="0" priority="113" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3295,7 +3309,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C36">
+  <conditionalFormatting sqref="C40">
     <cfRule type="cellIs" dxfId="0" priority="117" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3309,7 +3323,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37">
+  <conditionalFormatting sqref="C41">
     <cfRule type="cellIs" dxfId="0" priority="121" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3323,7 +3337,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38">
+  <conditionalFormatting sqref="C42">
     <cfRule type="cellIs" dxfId="0" priority="125" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3337,7 +3351,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C39">
+  <conditionalFormatting sqref="C43">
     <cfRule type="cellIs" dxfId="0" priority="129" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3351,7 +3365,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C40">
+  <conditionalFormatting sqref="C44">
     <cfRule type="cellIs" dxfId="0" priority="133" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3365,7 +3379,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
+  <conditionalFormatting sqref="C45">
     <cfRule type="cellIs" dxfId="0" priority="137" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3379,7 +3393,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C47">
     <cfRule type="cellIs" dxfId="0" priority="141" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3393,7 +3407,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43">
+  <conditionalFormatting sqref="C48">
     <cfRule type="cellIs" dxfId="0" priority="145" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3407,7 +3421,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
+  <conditionalFormatting sqref="C49">
     <cfRule type="cellIs" dxfId="0" priority="149" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3421,7 +3435,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C45">
+  <conditionalFormatting sqref="C50">
     <cfRule type="cellIs" dxfId="0" priority="153" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3435,7 +3449,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C46">
+  <conditionalFormatting sqref="C51">
     <cfRule type="cellIs" dxfId="0" priority="157" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3449,7 +3463,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C47">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="0" priority="161" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3463,7 +3477,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C48">
+  <conditionalFormatting sqref="C53">
     <cfRule type="cellIs" dxfId="0" priority="165" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3477,7 +3491,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C49">
+  <conditionalFormatting sqref="C54">
     <cfRule type="cellIs" dxfId="0" priority="169" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3491,7 +3505,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C50">
+  <conditionalFormatting sqref="C55">
     <cfRule type="cellIs" dxfId="0" priority="173" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3505,7 +3519,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C56">
     <cfRule type="cellIs" dxfId="0" priority="177" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3519,7 +3533,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C58">
     <cfRule type="cellIs" dxfId="0" priority="181" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3533,7 +3547,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C53">
+  <conditionalFormatting sqref="C59">
     <cfRule type="cellIs" dxfId="0" priority="185" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3547,7 +3561,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C54">
+  <conditionalFormatting sqref="C60">
     <cfRule type="cellIs" dxfId="0" priority="189" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3561,7 +3575,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C55">
+  <conditionalFormatting sqref="C61">
     <cfRule type="cellIs" dxfId="0" priority="193" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3575,7 +3589,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C56">
+  <conditionalFormatting sqref="C62">
     <cfRule type="cellIs" dxfId="0" priority="197" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3589,7 +3603,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C57">
+  <conditionalFormatting sqref="C63">
     <cfRule type="cellIs" dxfId="0" priority="201" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3603,7 +3617,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C58">
+  <conditionalFormatting sqref="C64">
     <cfRule type="cellIs" dxfId="0" priority="205" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3617,7 +3631,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C59">
+  <conditionalFormatting sqref="C65">
     <cfRule type="cellIs" dxfId="0" priority="209" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3631,7 +3645,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60">
+  <conditionalFormatting sqref="C66">
     <cfRule type="cellIs" dxfId="0" priority="213" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3645,7 +3659,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C61">
+  <conditionalFormatting sqref="C67">
     <cfRule type="cellIs" dxfId="0" priority="217" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3659,7 +3673,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62">
+  <conditionalFormatting sqref="C68">
     <cfRule type="cellIs" dxfId="0" priority="221" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3673,7 +3687,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63">
+  <conditionalFormatting sqref="C69">
     <cfRule type="cellIs" dxfId="0" priority="225" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3687,7 +3701,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C64">
+  <conditionalFormatting sqref="C70">
     <cfRule type="cellIs" dxfId="0" priority="229" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3701,7 +3715,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C65">
+  <conditionalFormatting sqref="C71">
     <cfRule type="cellIs" dxfId="0" priority="233" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3715,7 +3729,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C66">
+  <conditionalFormatting sqref="C72">
     <cfRule type="cellIs" dxfId="0" priority="237" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3729,7 +3743,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C67">
+  <conditionalFormatting sqref="C73">
     <cfRule type="cellIs" dxfId="0" priority="241" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3743,7 +3757,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C68">
+  <conditionalFormatting sqref="C74">
     <cfRule type="cellIs" dxfId="0" priority="245" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3757,7 +3771,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C69">
+  <conditionalFormatting sqref="C75">
     <cfRule type="cellIs" dxfId="0" priority="249" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3771,7 +3785,49 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7">
+  <conditionalFormatting sqref="C76">
+    <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="254" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="255" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="256" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C77">
+    <cfRule type="cellIs" dxfId="0" priority="257" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="258" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="259" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="260" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C79">
+    <cfRule type="cellIs" dxfId="0" priority="261" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="262" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="263" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="264" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3785,49 +3841,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C70">
-    <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="254" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="255" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="256" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
-    <cfRule type="cellIs" dxfId="0" priority="257" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="258" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="259" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="260" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C72">
-    <cfRule type="cellIs" dxfId="0" priority="261" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="262" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="263" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="264" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
+  <conditionalFormatting sqref="C80">
     <cfRule type="cellIs" dxfId="0" priority="265" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3841,7 +3855,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C74">
+  <conditionalFormatting sqref="C81">
     <cfRule type="cellIs" dxfId="0" priority="269" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3855,7 +3869,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
+  <conditionalFormatting sqref="C83">
     <cfRule type="cellIs" dxfId="0" priority="273" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3869,7 +3883,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C84">
     <cfRule type="cellIs" dxfId="0" priority="277" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3883,7 +3897,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="281" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3897,7 +3911,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C79">
+  <conditionalFormatting sqref="C86">
     <cfRule type="cellIs" dxfId="0" priority="285" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3911,7 +3925,49 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C8">
+  <conditionalFormatting sqref="C87">
+    <cfRule type="cellIs" dxfId="0" priority="289" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="290" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="291" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="292" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C88">
+    <cfRule type="cellIs" dxfId="0" priority="293" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="294" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="295" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="296" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C89">
+    <cfRule type="cellIs" dxfId="0" priority="297" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="298" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="299" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="300" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
     <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3925,49 +3981,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C80">
-    <cfRule type="cellIs" dxfId="0" priority="289" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="290" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="291" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="292" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C81">
-    <cfRule type="cellIs" dxfId="0" priority="293" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="294" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="295" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="296" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C82">
-    <cfRule type="cellIs" dxfId="0" priority="297" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="298" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="299" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="300" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C83">
+  <conditionalFormatting sqref="C90">
     <cfRule type="cellIs" dxfId="0" priority="301" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3981,7 +3995,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C92">
     <cfRule type="cellIs" dxfId="0" priority="305" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3995,7 +4009,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C93">
     <cfRule type="cellIs" dxfId="0" priority="309" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4009,7 +4023,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C86">
+  <conditionalFormatting sqref="C94">
     <cfRule type="cellIs" dxfId="0" priority="313" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4023,7 +4037,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C87">
+  <conditionalFormatting sqref="C95">
     <cfRule type="cellIs" dxfId="0" priority="317" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4037,7 +4051,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C88">
+  <conditionalFormatting sqref="C96">
     <cfRule type="cellIs" dxfId="0" priority="321" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4051,7 +4065,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C89">
+  <conditionalFormatting sqref="C97">
     <cfRule type="cellIs" dxfId="0" priority="325" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4065,21 +4079,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C9">
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="10" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="12" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C90">
+  <conditionalFormatting sqref="C98">
     <cfRule type="cellIs" dxfId="0" priority="329" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4093,7 +4093,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C91">
+  <conditionalFormatting sqref="C99">
     <cfRule type="cellIs" dxfId="0" priority="333" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4107,122 +4107,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C92">
-    <cfRule type="cellIs" dxfId="0" priority="337" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="338" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="339" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="340" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C93">
-    <cfRule type="cellIs" dxfId="0" priority="341" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="342" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="343" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="344" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C94">
-    <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="346" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="347" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="348" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C95">
-    <cfRule type="cellIs" dxfId="0" priority="349" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="350" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="351" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="352" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C96">
-    <cfRule type="cellIs" dxfId="0" priority="353" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="354" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="355" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="356" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C97">
-    <cfRule type="cellIs" dxfId="0" priority="357" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="358" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="359" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="360" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C98">
-    <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="362" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="363" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="364" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C99">
-    <cfRule type="cellIs" dxfId="0" priority="365" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="366" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="367" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="368" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="105">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
+  <dataValidations count="97">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4235,9 +4120,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C12">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C13">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4295,9 +4177,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C31">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C32">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4307,9 +4186,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C35">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C36">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C37">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4337,9 +4213,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C45">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C46">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C47">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4370,9 +4243,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C56">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C57">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C58">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4442,9 +4312,6 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C81">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C82">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4467,9 +4334,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C90">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C91">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C92">

</xml_diff>

<commit_message>
Voeg kennis van KA toe aan M23. (#1017)
* Verwijzigingen naar OpenVAS verwijderd. (#1007)

Closes #949.

* Voeg template voor voortgang voorfase producten toe. (#986)

Closes #760.

* Voeg kennis van KA toe aan M23.

De titel van maatregel M23 is veranderd van "Het project zorgt voor de aanwezigheid van ervaring met de Kwaliteitsaanpak" naar "Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak". Aan de inhoud is toegevoegd dat nieuwe projectleden uitleg over de Kwaliteitsaanpak krijgen.

Closes #794.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -417,17 +417,16 @@
 5. release van software,
 6. maken van testrapportages,
 7. maken van kwaliteitsrapportages,
-8. controleren van de configuratie op aanwezigheid van bekende kwetsbaarheden,
-9. controleren van door de applicatie gebruikte versies van externe software op aanwezigheid van bekende kwetsbaarheden,
-10. statische controle van de software op aanwezigheid van kwetsbare constructies,
-11. dynamische controle van de software op aanwezigheid van kwetsbare constructies,
-12. controleren van container images op aanwezigheid van bekende kwetsbaarheden,
-13. testen van performance en schaalbaarheid,
-14. testen op toegankelijkheid van de applicatie,
-15. produceren van een "software bill of materials" (SBoM),
-16. opslaan van artifacten,
-17. registratie van incidenten bij gebruik en beheer, en
-18. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving.
+8. controleren van door de applicatie gebruikte versies van externe software op aanwezigheid van bekende kwetsbaarheden,
+9. statische controle van de software op aanwezigheid van kwetsbare constructies,
+10. dynamische controle van de software op aanwezigheid van kwetsbare constructies,
+11. controleren van container images op aanwezigheid van bekende kwetsbaarheden,
+12. testen van performance en schaalbaarheid,
+13. testen op toegankelijkheid van de applicatie,
+14. produceren van een "software bill of materials" (SBoM),
+15. opslaan van artifacten,
+16. registratie van incidenten bij gebruik en beheer, en
+17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving.
 Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
 ICTU adviseert en ondersteunt voor de genoemde taken onderstaande tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven:
 1. product en sprint backlog management en agile werken: Azure DevOps of Jira,
@@ -437,17 +436,16 @@
 5. release van software: Releaseserver in het ontwikkelplatform,
 6. maken van testrapportages: JUnit, Robot Framework, TestNG, of hiermee compatible tools,
 7. maken van kwaliteitsrapportages: Quality-time,
-8. controleren van de configuratie op aanwezigheid van bekende kwetsbaarheden in configuratie: OpenVAS (Vulnerability Assessment System),
-9. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,
-10. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,
-11. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,
-12. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,
-13. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,
-14. testen op toegankelijkheid van de applicatie: Axe,
-15. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,
-16. opslaan van artifacten: Nexus of Harbor,
-17. registratie van incidenten bij gebruik en beheer: Jira, en
-18. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.
+8. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,
+9. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,
+10. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,
+11. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,
+12. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,
+13. testen op toegankelijkheid van de applicatie: Axe,
+14. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,
+15. opslaan van artifacten: Nexus of Harbor,
+16. registratie van incidenten bij gebruik en beheer: Jira, en
+17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.
 Rationale
 Projecten hebben een redelijke vrijheid bij het kiezen en gebruiken van tools, maar voor een aantal taken is het gebruik verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van de Kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren; daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af. Tot slot is het gebruik in een aantal gevallen, ten behoeve van informatiebeveiliging bij de overheid, verplicht.
 </t>
@@ -467,7 +465,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -487,7 +485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B77" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -509,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B79" authorId="0">
+    <comment ref="B78" authorId="0">
       <text>
         <r>
           <rPr>
@@ -530,7 +528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B80" authorId="0">
+    <comment ref="B79" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="0">
+    <comment ref="B80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -556,15 +554,15 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M23: Het project zorgt voor de aanwezigheid van ervaring met de Kwaliteitsaanpak
-De software delivery manager zorgt ervoor dat bij nieuwe projecten wordt gestart met ten minste twee projectleden die bekend zijn met de Kwaliteitsaanpak.
+          <t xml:space="preserve">M23: Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak
+De software delivery manager zorgt ervoor dat bij nieuwe projecten wordt gestart met ten minste twee projectleden die bekend zijn met de Kwaliteitsaanpak. Projectleden die nog niet bekend zijn met de Kwaliteitsaanpak krijgen uitleg over de inhoud en achtergrond van de Kwaliteitsaanpak.
 Rationale
 Het inzetten van teamleden die bekend zijn met de Kwaliteitsaanpak zorgt voor een soepeler start van een nieuw project omdat zij bekend zijn met de inhoud van de Kwaliteitsaanpak, zoals kwaliteitsnormen en tools, en omdat zij al doende nieuwe teamleden bekend kunnen maken met de Kwaliteitsaanpak.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -587,7 +585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C82" authorId="0">
+    <comment ref="C81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -600,7 +598,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B87" authorId="0">
+    <comment ref="B86" authorId="0">
       <text>
         <r>
           <rPr>
@@ -621,7 +619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B88" authorId="0">
+    <comment ref="B87" authorId="0">
       <text>
         <r>
           <rPr>
@@ -646,7 +644,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B89" authorId="0">
+    <comment ref="B88" authorId="0">
       <text>
         <r>
           <rPr>
@@ -673,7 +671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B90" authorId="0">
+    <comment ref="B89" authorId="0">
       <text>
         <r>
           <rPr>
@@ -691,7 +689,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B91" authorId="0">
+    <comment ref="B90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -723,7 +721,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C91" authorId="0">
+    <comment ref="C90" authorId="0">
       <text>
         <r>
           <rPr>
@@ -736,7 +734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +754,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B108" authorId="0">
+    <comment ref="B107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -776,7 +774,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B109" authorId="0">
+    <comment ref="B108" authorId="0">
       <text>
         <r>
           <rPr>
@@ -795,7 +793,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B110" authorId="0">
+    <comment ref="B109" authorId="0">
       <text>
         <r>
           <rPr>
@@ -816,7 +814,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B111" authorId="0">
+    <comment ref="B110" authorId="0">
       <text>
         <r>
           <rPr>
@@ -835,7 +833,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B112" authorId="0">
+    <comment ref="B111" authorId="0">
       <text>
         <r>
           <rPr>
@@ -853,7 +851,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B113" authorId="0">
+    <comment ref="B112" authorId="0">
       <text>
         <r>
           <rPr>
@@ -884,7 +882,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="145">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
@@ -1114,37 +1112,34 @@
     <t>7. maken van kwaliteitsrapportages: Quality-time,</t>
   </si>
   <si>
-    <t>8. controleren van de configuratie op aanwezigheid van bekende kwetsbaarheden in configuratie: OpenVAS (Vulnerability Assessment System),</t>
-  </si>
-  <si>
-    <t>9. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,</t>
-  </si>
-  <si>
-    <t>10. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,</t>
-  </si>
-  <si>
-    <t>11. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,</t>
-  </si>
-  <si>
-    <t>12. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,</t>
-  </si>
-  <si>
-    <t>13. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,</t>
-  </si>
-  <si>
-    <t>14. testen op toegankelijkheid van de applicatie: Axe,</t>
-  </si>
-  <si>
-    <t>15. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,</t>
-  </si>
-  <si>
-    <t>16. opslaan van artifacten: Nexus of Harbor,</t>
-  </si>
-  <si>
-    <t>17. registratie van incidenten bij gebruik en beheer: Jira, en</t>
-  </si>
-  <si>
-    <t>18. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.</t>
+    <t>8. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,</t>
+  </si>
+  <si>
+    <t>9. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,</t>
+  </si>
+  <si>
+    <t>10. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,</t>
+  </si>
+  <si>
+    <t>11. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,</t>
+  </si>
+  <si>
+    <t>12. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,</t>
+  </si>
+  <si>
+    <t>13. testen op toegankelijkheid van de applicatie: Axe,</t>
+  </si>
+  <si>
+    <t>14. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,</t>
+  </si>
+  <si>
+    <t>15. opslaan van artifacten: Nexus of Harbor,</t>
+  </si>
+  <si>
+    <t>16. registratie van incidenten bij gebruik en beheer: Jira, en</t>
+  </si>
+  <si>
+    <t>17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.</t>
   </si>
   <si>
     <t>M08</t>
@@ -1177,7 +1172,7 @@
     <t>M23</t>
   </si>
   <si>
-    <t>Het project zorgt voor de aanwezigheid van ervaring met de Kwaliteitsaanpak</t>
+    <t>Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak</t>
   </si>
   <si>
     <t>M05</t>
@@ -1763,7 +1758,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D112"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2395,79 +2390,79 @@
       <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
-      <c r="A75" s="6"/>
-      <c r="B75" s="6" t="s">
+      <c r="A75" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C75" s="7"/>
+      <c r="B75" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="8"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C76" s="8"/>
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B77" s="4" t="s">
+      <c r="A77" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C77" s="8"/>
-      <c r="D77" s="5"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B78" s="1"/>
-      <c r="C78" s="1"/>
-      <c r="D78" s="1"/>
+      <c r="B78" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78" s="8"/>
+      <c r="D78" s="5"/>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C79" s="8"/>
       <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C80" s="8"/>
       <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="8"/>
+        <v>98</v>
+      </c>
+      <c r="C81" s="4"/>
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
-      <c r="A82" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B82" s="4" t="s">
+      <c r="A82" s="6"/>
+      <c r="B82" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="C82" s="4"/>
+      <c r="C82" s="7"/>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
@@ -2495,61 +2490,61 @@
       <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6" t="s">
+      <c r="A86" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C86" s="7"/>
+      <c r="B86" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C86" s="8"/>
       <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C87" s="8"/>
       <c r="D87" s="5"/>
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C88" s="8"/>
       <c r="D88" s="5"/>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C89" s="8"/>
       <c r="D89" s="5"/>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C90" s="8"/>
+        <v>112</v>
+      </c>
+      <c r="C90" s="4"/>
       <c r="D90" s="5"/>
     </row>
     <row r="91" spans="1:4">
-      <c r="A91" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B91" s="4" t="s">
+      <c r="A91" s="6"/>
+      <c r="B91" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C91" s="4"/>
+      <c r="C91" s="7"/>
       <c r="D91" s="5"/>
     </row>
     <row r="92" spans="1:4">
@@ -2657,90 +2652,82 @@
       <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4">
-      <c r="A105" s="6"/>
-      <c r="B105" s="6" t="s">
+      <c r="A105" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C105" s="7"/>
+      <c r="B105" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C105" s="8"/>
       <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4">
-      <c r="A106" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B106" s="4" t="s">
+      <c r="A106" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="C106" s="8"/>
-      <c r="D106" s="5"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+      <c r="D106" s="1"/>
     </row>
     <row r="107" spans="1:4">
-      <c r="A107" s="1" t="s">
+      <c r="A107" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B107" s="1"/>
-      <c r="C107" s="1"/>
-      <c r="D107" s="1"/>
+      <c r="B107" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="5"/>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C108" s="8"/>
       <c r="D108" s="5"/>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C109" s="8"/>
       <c r="D109" s="5"/>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C110" s="8"/>
       <c r="D110" s="5"/>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C111" s="8"/>
       <c r="D111" s="5"/>
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C112" s="8"/>
       <c r="D112" s="5"/>
-    </row>
-    <row r="113" spans="1:4">
-      <c r="A113" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B113" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C113" s="8"/>
-      <c r="D113" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2847,7 +2834,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C106">
+  <conditionalFormatting sqref="C107">
     <cfRule type="cellIs" dxfId="0" priority="361" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2945,20 +2932,6 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C113">
-    <cfRule type="cellIs" dxfId="0" priority="385" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="386" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="387" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="388" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C13">
     <cfRule type="cellIs" dxfId="0" priority="17" operator="equal">
       <formula>"voldoet"</formula>
@@ -3799,7 +3772,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C78">
     <cfRule type="cellIs" dxfId="0" priority="257" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3855,7 +3828,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C81">
+  <conditionalFormatting sqref="C82">
     <cfRule type="cellIs" dxfId="0" priority="269" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3981,7 +3954,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C90">
+  <conditionalFormatting sqref="C91">
     <cfRule type="cellIs" dxfId="0" priority="301" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -4107,7 +4080,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="97">
+  <dataValidations count="96">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4300,7 +4273,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C78">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C79">
@@ -4309,7 +4282,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C80">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C81">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C82">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
@@ -4333,7 +4306,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C89">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C90">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C91">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C92">
@@ -4378,7 +4351,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C105">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C108">
@@ -4394,9 +4367,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C112">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C113">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4410,24 +4380,24 @@
     <hyperlink ref="A45" r:id="rId7" location="m04"/>
     <hyperlink ref="A46" r:id="rId8" location="m07"/>
     <hyperlink ref="A57" r:id="rId9" location="m16"/>
-    <hyperlink ref="A76" r:id="rId10" location="m08"/>
-    <hyperlink ref="A77" r:id="rId11" location="m26"/>
-    <hyperlink ref="A79" r:id="rId12" location="m14"/>
-    <hyperlink ref="A80" r:id="rId13" location="m21"/>
-    <hyperlink ref="A81" r:id="rId14" location="m23"/>
-    <hyperlink ref="A82" r:id="rId15" location="m05"/>
-    <hyperlink ref="A87" r:id="rId16" location="m35"/>
-    <hyperlink ref="A88" r:id="rId17" location="m10"/>
-    <hyperlink ref="A89" r:id="rId18" location="m28"/>
-    <hyperlink ref="A90" r:id="rId19" location="m30"/>
-    <hyperlink ref="A91" r:id="rId20" location="m34"/>
-    <hyperlink ref="A106" r:id="rId21" location="m27"/>
-    <hyperlink ref="A108" r:id="rId22" location="m29"/>
-    <hyperlink ref="A109" r:id="rId23" location="m19"/>
-    <hyperlink ref="A110" r:id="rId24" location="m18"/>
-    <hyperlink ref="A111" r:id="rId25" location="m11"/>
-    <hyperlink ref="A112" r:id="rId26" location="m12"/>
-    <hyperlink ref="A113" r:id="rId27" location="m33"/>
+    <hyperlink ref="A75" r:id="rId10" location="m08"/>
+    <hyperlink ref="A76" r:id="rId11" location="m26"/>
+    <hyperlink ref="A78" r:id="rId12" location="m14"/>
+    <hyperlink ref="A79" r:id="rId13" location="m21"/>
+    <hyperlink ref="A80" r:id="rId14" location="m23"/>
+    <hyperlink ref="A81" r:id="rId15" location="m05"/>
+    <hyperlink ref="A86" r:id="rId16" location="m35"/>
+    <hyperlink ref="A87" r:id="rId17" location="m10"/>
+    <hyperlink ref="A88" r:id="rId18" location="m28"/>
+    <hyperlink ref="A89" r:id="rId19" location="m30"/>
+    <hyperlink ref="A90" r:id="rId20" location="m34"/>
+    <hyperlink ref="A105" r:id="rId21" location="m27"/>
+    <hyperlink ref="A107" r:id="rId22" location="m29"/>
+    <hyperlink ref="A108" r:id="rId23" location="m19"/>
+    <hyperlink ref="A109" r:id="rId24" location="m18"/>
+    <hyperlink ref="A110" r:id="rId25" location="m11"/>
+    <hyperlink ref="A111" r:id="rId26" location="m12"/>
+    <hyperlink ref="A112" r:id="rId27" location="m33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId28"/>
@@ -4450,7 +4420,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4458,10 +4428,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
937 duplicatie tussen m01 m07 en m16 oplossen (#1019)
In M16 de twee opsommingen gecombineerd in 1 tabel.

In M16 "Het project gebruikt tools voor vastgestelde taken" de opsomming van taken gecombineerd met de opsomming van tools in één tabel.

Closes #937.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -337,12 +337,9 @@
 6. Toegankelijkheidstests,
 7. Broncodekwaliteitscontroles,
 8. Installatie van de software in test, acceptatie en/of productieomgevingen,
-9. Produceren van een "software bill of materials" (SBoM),
-10. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.
+9. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.
 Performance- en beveiligingstests op de software zijn ook onderdeel van de continuous delivery pipeline, maar vanwege doorlooptijden en licenties is dat niet altijd haalbaar; in dat geval vinden de performance- en beveiligingstests zo veel mogelijk, en bij voorkeur dagelijks, plaats. Performance- en beveiligingstests op de software vinden plaats in de testomgeving van het project. Als ICTU verantwoordelijk is voor het operationeel beheer laat ICTU de performance- en beveiligingstesten op de software (ook) uitvoeren in een productie-like omgeving.
 Niet alle testen en controles kunnen altijd geautomatiseerd worden uitgevoerd. Denk aan kwaliteitscontroles op architectuurbeslissingen of het testen van toegankelijkheidseisen. Waar mogelijk wordt wel een zo groot mogelijk deel van de testen en controles geautomatiseerd en als onderdeel van de pipeline uitgevoerd.
-De afdeling ICTU Software Diensten (ISD) voorziet in tools en ondersteuning, zodat projecten deze pipeline kunnen toepassen. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
-ICTU gebruikt Jenkins, GitLab CI of Azure DevOps als tool voor de implementatie van de continuous delivery pipeline. ISD biedt de projecten een voorziening om releases van het totale product veilig op te leveren aan opdrachtgevende organisaties en beheerorganisaties.
 Rationale
 Software incrementeel opleveren vereist dat de software frequent gebouwd, getest en opgeleverd kan worden. Om dit efficiënt en foutvrij te doen, dient het proces van bouwen, testen en opleveren geautomatiseerd te zijn; een continuous delivery pipeline faciliteert dit.
 </t>
@@ -362,7 +359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B53" authorId="0">
+    <comment ref="B52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -372,50 +369,34 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">M16: Het project gebruikt tools voor vastgestelde taken
-ICTU stelt het gebruik van tools verplicht voor de volgende taken:
-1. product en sprint backlog management en agile werken,
-2. inrichten en uitvoeren van een continuous delivery pipeline,
-3. monitoren van de kwaliteit van broncode,
-4. versiebeheer van op te leveren producten,
-5. release van software,
-6. maken van testrapportages,
-7. maken van kwaliteitsrapportages,
-8. controleren van door de applicatie gebruikte versies van externe software op aanwezigheid van bekende kwetsbaarheden,
-9. statische controle van de software op aanwezigheid van kwetsbare constructies,
-10. dynamische controle van de software op aanwezigheid van kwetsbare constructies,
-11. controleren van container images op aanwezigheid van bekende kwetsbaarheden,
-12. testen van performance en schaalbaarheid,
-13. testen op toegankelijkheid van de applicatie,
-14. produceren van een "software bill of materials" (SBoM),
-15. opslaan van artifacten,
-16. registratie van incidenten bij gebruik en beheer, en
-17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving.
-Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
-ICTU adviseert en ondersteunt voor de genoemde taken onderstaande tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven:
-1. product en sprint backlog management en agile werken: Azure DevOps of Jira,
-2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,
-3. monitoren van de kwaliteit van broncode: SonarQube,
-4. versiebeheer van op te leveren producten: GitLab of Azure DevOps,
-5. release van software: Releaseserver in het ontwikkelplatform,
-6. maken van testrapportages: JUnit, Robot Framework, TestNG, of hiermee compatible tools,
-7. maken van kwaliteitsrapportages: Quality-time,
-8. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,
-9. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,
-10. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,
-11. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,
-12. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,
-13. testen op toegankelijkheid van de applicatie: Axe,
-14. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,
-15. opslaan van artifacten: Nexus of Harbor,
-16. registratie van incidenten bij gebruik en beheer: Jira, en
-17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.
+Voor vastgestelde taken bij het ontwikkelen, onderhouden en operationeel beheren van software, stelt ICTU het gebruik van tools verplicht. ICTU adviseert per taak specifieke tools en ondersteunt projecten bij het gebruik daarvan.
+ICTU adviseert en ondersteunt voor de hieronder genoemde taken specifieke tools. Projecten gebruiken deze tools, of gelijkwaardige alternatieven.
+Activiteit                                                                                   Tools                                                                                    
+Product en sprint backlog management en agile werken                                         Azure DevOps of Jira                                                                     
+Inrichten en uitvoeren van een continuous delivery pipeline                                  Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps 
+Monitoren van de kwaliteit van broncode                                                      SonarQube                                                                                
+Versiebeheer van op te leveren producten                                                     GitLab of Azure DevOps                                                                   
+Release van software                                                                         Releaseserver in het ontwikkelplatform                                                   
+Maken van testrapportages                                                                    JUnit, Robot Framework, TestNG, of hiermee compatible tools                              
+Maken van kwaliteitsrapportages                                                              Quality-time                                                                             
+Controleren op aanwezigheid van bekende kwetsbaarheden in externe software                   OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track    
+Statische controle van de software op aanwezigheid van kwetsbare constructies                SonarQube                                                                                
+Dynamische controle van de software op aanwezigheid van kwetsbare constructies               ZAP (Zed Attack Proxy) by Checkmarx                                                      
+Controleren van container images op aanwezigheid van bekende kwetsbaarheden                  Trivy                                                                                    
+Testen van performance en schaalbaarheid                                                     JMeter en Performancetestrunner                                                          
+Testen op toegankelijkheid van de applicatie                                                 Axe                                                                                      
+Produceren van een "software bill of materials" (SBoM)                                       Tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren            
+Opslaan van artifacten                                                                       Nexus of Harbor                                                                          
+Registratie van incidenten bij gebruik en beheer                                             Jira                                                                                     
+Bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving Ansible                                                                                  
+N.B. Onder het ondersteunen van "agile werken" vallen het opvoeren van eisen, het opvoeren van logische testgevallen, het koppelen van logische testgevallen aan eisen, het bijhouden van een werkvoorraad, het plannen van iteraties en het toewijzen van eisen aan iteraties. De 'eisen' worden, conform Scrumterminologie, geregistreerd als epics en/of user stories, de werkvoorraad als product backlog en de iteraties als sprints. Het toewijzen van eisen aan iteraties gebeurt via de sprint backlog.
 Rationale
 Projecten hebben een redelijke vrijheid bij het kiezen en gebruiken van tools, maar voor een aantal taken is het gebruik verplicht gesteld. Deze tools zijn nodig voor een efficiënte uitvoering van de Kwaliteitsaanpak. Uniform gebruik van deze tools maakt het mogelijk koppeling tussen die tools voor alle projecten te standaardiseren; daarnaast bevordert het de uitwisselbaarheid van medewerkers en neemt het risico op het gebruik van onvolwassen tools af. Tot slot is het gebruik in een aantal gevallen, ten behoeve van informatiebeveiliging bij de overheid, verplicht.
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C53" authorId="0">
+    <comment ref="C52" authorId="0">
       <text>
         <r>
           <rPr>
@@ -428,7 +409,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B72" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -470,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -491,7 +472,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -525,7 +506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B77" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -548,7 +529,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C77" authorId="0">
+    <comment ref="C76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -561,7 +542,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -582,7 +563,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -607,7 +588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -634,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -652,7 +633,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B86" authorId="0">
+    <comment ref="B85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -684,7 +665,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C86" authorId="0">
+    <comment ref="C85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -697,7 +678,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B101" authorId="0">
+    <comment ref="B100" authorId="0">
       <text>
         <r>
           <rPr>
@@ -717,7 +698,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +718,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -756,7 +737,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -767,7 +748,7 @@
           </rPr>
           <t xml:space="preserve">M18: ICTU biedt ondersteuning voor verplicht gestelde tools
 ICTU zorgt voor technische en functionele ondersteuning aan projecten bij het gebruik van alle verplichte tools.
-ICTU zorgt voor ondersteuning van de bij M16: Het project gebruikt tools voor vastgestelde taken verplicht gestelde tools. Een team van specialisten met kennis, ervaring en capaciteit is beschikbaar voor ondersteuning aan projecten.
+ICTU zorgt voor ondersteuning van de in M16: Het project gebruikt tools voor vastgestelde taken verplicht gestelde tools. Een team van specialisten met kennis, ervaring en capaciteit is beschikbaar voor ondersteuning aan projecten. Projecten zijn verantwoordelijk voor de correcte werking van de pipeline.
 Bij de selectie van tools ter ondersteuning van de projectuitvoering geeft ICTU de voorkeur aan open source tools. Ook tools die ICTU zelf ontwikkelt ter ondersteuning van softwareontwikkelprojecten worden bij voorkeur open source beschikbaar gesteld.
 Rationale
 De keuze om het gebruik van een aantal tools verplicht te stellen (M16: Het project gebruikt tools voor vastgestelde taken) volgt uit de belangrijke rol die die tools spelen in de ontwikkelstraat en in Quality-time, het kwaliteitssysteem van ICTU. Met de verplichting komt ook een verantwoordelijkheid: om projecten in staat te stellen snel en effectief met deze tools te werken, moeten die projecten ondersteund worden.
@@ -777,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -796,7 +777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -814,7 +795,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B108" authorId="0">
+    <comment ref="B107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -845,7 +826,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
@@ -1027,10 +1008,7 @@
     <t>8. Installatie van de software in test, acceptatie en/of productieomgevingen,</t>
   </si>
   <si>
-    <t>9. Produceren van een "software bill of materials" (SBoM),</t>
-  </si>
-  <si>
-    <t>10. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.</t>
+    <t>9. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.</t>
   </si>
   <si>
     <t>M16</t>
@@ -1039,55 +1017,55 @@
     <t>Het project gebruikt tools voor vastgestelde taken</t>
   </si>
   <si>
-    <t>1. product en sprint backlog management en agile werken: Azure DevOps of Jira,</t>
-  </si>
-  <si>
-    <t>2. inrichten en uitvoeren van een continuous delivery pipeline: Jenkins, GitLab CI/CD (Continuous Integration, Delivery, and Deployment) of Azure DevOps,</t>
-  </si>
-  <si>
-    <t>3. monitoren van de kwaliteit van broncode: SonarQube,</t>
-  </si>
-  <si>
-    <t>4. versiebeheer van op te leveren producten: GitLab of Azure DevOps,</t>
-  </si>
-  <si>
-    <t>5. release van software: Releaseserver in het ontwikkelplatform,</t>
-  </si>
-  <si>
-    <t>6. maken van testrapportages: JUnit, Robot Framework, TestNG, of hiermee compatible tools,</t>
-  </si>
-  <si>
-    <t>7. maken van kwaliteitsrapportages: Quality-time,</t>
-  </si>
-  <si>
-    <t>8. controleren op aanwezigheid van bekende kwetsbaarheden in externe software: OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track,</t>
-  </si>
-  <si>
-    <t>9. statische controle van de software op aanwezigheid van kwetsbare constructies: SonarQube,</t>
-  </si>
-  <si>
-    <t>10. dynamische controle van de software op aanwezigheid van kwetsbare constructies: ZAP (Zed Attack Proxy) by Checkmarx,</t>
-  </si>
-  <si>
-    <t>11. controleren van container images op aanwezigheid van bekende kwetsbaarheden: Trivy,</t>
-  </si>
-  <si>
-    <t>12. testen van performance en schaalbaarheid: JMeter en Performancetestrunner,</t>
-  </si>
-  <si>
-    <t>13. testen op toegankelijkheid van de applicatie: Axe,</t>
-  </si>
-  <si>
-    <t>14. produceren van een "software bill of materials" (SBoM): tools die een SBoM in CycloneDX-formaat (zie https://cyclonedx.org) genereren,</t>
-  </si>
-  <si>
-    <t>15. opslaan van artifacten: Nexus of Harbor,</t>
-  </si>
-  <si>
-    <t>16. registratie van incidenten bij gebruik en beheer: Jira, en</t>
-  </si>
-  <si>
-    <t>17. bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving: Ansible.</t>
+    <t>1. Product en sprint backlog management en agile werken</t>
+  </si>
+  <si>
+    <t>2. Inrichten en uitvoeren van een continuous delivery pipeline</t>
+  </si>
+  <si>
+    <t>3. Monitoren van de kwaliteit van broncode</t>
+  </si>
+  <si>
+    <t>4. Versiebeheer van op te leveren producten</t>
+  </si>
+  <si>
+    <t>5. Release van software</t>
+  </si>
+  <si>
+    <t>6. Maken van testrapportages</t>
+  </si>
+  <si>
+    <t>7. Maken van kwaliteitsrapportages</t>
+  </si>
+  <si>
+    <t>8. Controleren op aanwezigheid van bekende kwetsbaarheden in externe software</t>
+  </si>
+  <si>
+    <t>9. Statische controle van de software op aanwezigheid van kwetsbare constructies</t>
+  </si>
+  <si>
+    <t>10. Dynamische controle van de software op aanwezigheid van kwetsbare constructies</t>
+  </si>
+  <si>
+    <t>11. Controleren van container images op aanwezigheid van bekende kwetsbaarheden</t>
+  </si>
+  <si>
+    <t>12. Testen van performance en schaalbaarheid</t>
+  </si>
+  <si>
+    <t>13. Testen op toegankelijkheid van de applicatie</t>
+  </si>
+  <si>
+    <t>14. Produceren van een "software bill of materials" (SBoM)</t>
+  </si>
+  <si>
+    <t>15. Opslaan van artifacten</t>
+  </si>
+  <si>
+    <t>16. Registratie van incidenten bij gebruik en beheer</t>
+  </si>
+  <si>
+    <t>17. Bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving</t>
   </si>
   <si>
     <t>M08</t>
@@ -1706,7 +1684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2150,21 +2128,21 @@
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="6"/>
-      <c r="B52" s="6" t="s">
+      <c r="A52" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C52" s="7"/>
+      <c r="B52" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" s="4"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="6"/>
+      <c r="B53" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="7"/>
       <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
@@ -2296,79 +2274,79 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="6"/>
-      <c r="B70" s="6" t="s">
+      <c r="A70" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C70" s="7"/>
+      <c r="B70" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C70" s="8"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B72" s="4" t="s">
+      <c r="A72" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C72" s="8"/>
-      <c r="D72" s="5"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
-      <c r="D73" s="1"/>
+      <c r="B73" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="5"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C76" s="8"/>
+        <v>92</v>
+      </c>
+      <c r="C76" s="4"/>
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B77" s="4" t="s">
+      <c r="A77" s="6"/>
+      <c r="B77" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="C77" s="4"/>
+      <c r="C77" s="7"/>
       <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:4">
@@ -2396,61 +2374,61 @@
       <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6" t="s">
+      <c r="A81" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="7"/>
+      <c r="B81" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C81" s="8"/>
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="5"/>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C85" s="8"/>
+        <v>106</v>
+      </c>
+      <c r="C85" s="4"/>
       <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B86" s="4" t="s">
+      <c r="A86" s="6"/>
+      <c r="B86" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="C86" s="4"/>
+      <c r="C86" s="7"/>
       <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
@@ -2558,90 +2536,82 @@
       <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="6"/>
-      <c r="B100" s="6" t="s">
+      <c r="A100" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C100" s="7"/>
+      <c r="B100" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="8"/>
       <c r="D100" s="5"/>
     </row>
     <row r="101" spans="1:4">
-      <c r="A101" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B101" s="4" t="s">
+      <c r="A101" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="C101" s="8"/>
-      <c r="D101" s="5"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B102" s="1"/>
-      <c r="C102" s="1"/>
-      <c r="D102" s="1"/>
+      <c r="B102" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="5"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="3" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="5"/>
-    </row>
-    <row r="108" spans="1:4">
-      <c r="A108" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B108" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="C108" s="8"/>
-      <c r="D108" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2678,7 +2648,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C101">
+  <conditionalFormatting sqref="C102">
     <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2762,20 +2732,6 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C108">
-    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3308,7 +3264,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C52">
+  <conditionalFormatting sqref="C53">
     <cfRule type="cellIs" dxfId="0" priority="165" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3574,7 +3530,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C72">
+  <conditionalFormatting sqref="C73">
     <cfRule type="cellIs" dxfId="0" priority="241" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3616,7 +3572,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C76">
+  <conditionalFormatting sqref="C77">
     <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3742,7 +3698,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C85">
+  <conditionalFormatting sqref="C86">
     <cfRule type="cellIs" dxfId="0" priority="285" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3952,7 +3908,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="93">
+  <dataValidations count="92">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4076,7 +4032,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C54">
@@ -4133,7 +4089,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C72">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C73">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74">
@@ -4142,7 +4098,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C78">
@@ -4166,7 +4122,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C87">
@@ -4211,7 +4167,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103">
@@ -4227,9 +4183,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C108">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4241,25 +4194,25 @@
     <hyperlink ref="A40" r:id="rId5" location="m13"/>
     <hyperlink ref="A41" r:id="rId6" location="m04"/>
     <hyperlink ref="A42" r:id="rId7" location="m07"/>
-    <hyperlink ref="A53" r:id="rId8" location="m16"/>
-    <hyperlink ref="A71" r:id="rId9" location="m08"/>
-    <hyperlink ref="A72" r:id="rId10" location="m26"/>
-    <hyperlink ref="A74" r:id="rId11" location="m14"/>
-    <hyperlink ref="A75" r:id="rId12" location="m21"/>
-    <hyperlink ref="A76" r:id="rId13" location="m23"/>
-    <hyperlink ref="A77" r:id="rId14" location="m05"/>
-    <hyperlink ref="A82" r:id="rId15" location="m35"/>
-    <hyperlink ref="A83" r:id="rId16" location="m10"/>
-    <hyperlink ref="A84" r:id="rId17" location="m28"/>
-    <hyperlink ref="A85" r:id="rId18" location="m30"/>
-    <hyperlink ref="A86" r:id="rId19" location="m34"/>
-    <hyperlink ref="A101" r:id="rId20" location="m27"/>
-    <hyperlink ref="A103" r:id="rId21" location="m29"/>
-    <hyperlink ref="A104" r:id="rId22" location="m19"/>
-    <hyperlink ref="A105" r:id="rId23" location="m18"/>
-    <hyperlink ref="A106" r:id="rId24" location="m11"/>
-    <hyperlink ref="A107" r:id="rId25" location="m12"/>
-    <hyperlink ref="A108" r:id="rId26" location="m33"/>
+    <hyperlink ref="A52" r:id="rId8" location="m16"/>
+    <hyperlink ref="A70" r:id="rId9" location="m08"/>
+    <hyperlink ref="A71" r:id="rId10" location="m26"/>
+    <hyperlink ref="A73" r:id="rId11" location="m14"/>
+    <hyperlink ref="A74" r:id="rId12" location="m21"/>
+    <hyperlink ref="A75" r:id="rId13" location="m23"/>
+    <hyperlink ref="A76" r:id="rId14" location="m05"/>
+    <hyperlink ref="A81" r:id="rId15" location="m35"/>
+    <hyperlink ref="A82" r:id="rId16" location="m10"/>
+    <hyperlink ref="A83" r:id="rId17" location="m28"/>
+    <hyperlink ref="A84" r:id="rId18" location="m30"/>
+    <hyperlink ref="A85" r:id="rId19" location="m34"/>
+    <hyperlink ref="A100" r:id="rId20" location="m27"/>
+    <hyperlink ref="A102" r:id="rId21" location="m29"/>
+    <hyperlink ref="A103" r:id="rId22" location="m19"/>
+    <hyperlink ref="A104" r:id="rId23" location="m18"/>
+    <hyperlink ref="A105" r:id="rId24" location="m11"/>
+    <hyperlink ref="A106" r:id="rId25" location="m12"/>
+    <hyperlink ref="A107" r:id="rId26" location="m33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId27"/>
@@ -4282,7 +4235,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4290,10 +4243,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
M13 over ISO-25010 is vervallen. (#1018)
* Voeg template voor voortgang voorfase producten toe. (#986)

Closes #760.

* M13 over ISO-25010 is vervallen.

Maatregel M13 "Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen" is vervallen. Het gebruik van ISO-25010 voor de specificatie van productkwaliteitseisen staat al genoemd in M01 "Het project levert in elke fase vastgestelde producten en informatie op".

Closes #950.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -290,24 +290,6 @@
             <rFont val="Courier"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">M13: Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen
-Voor specificatie en documentatie van vereiste en gewenste kwaliteitseigenschappen, de niet-functionele eisen, maken projecten gebruik van de terminologie en categorisering uit NEN-ISO/IEC 25010:2023. Projecten gebruiken NEN-ISO/IEC 25010:2023 om te controleren of alle relevante kwaliteitseigenschappen van het op te leveren eindproduct worden meegenomen in de ontwikkeling en/of onderhoud van het product.
-De standaard NEN-ISO/IEC 25010:2023 biedt een model voor het beschrijven van productkwaliteit. Kwaliteitseigenschappen zijn voorzien van een naam, definitie en classificatie. NEN-ISO/IEC 25010:2023 dekt een breed spectrum van kwaliteitseigenschappen af.
-Rationale
-NEN-ISO/IEC 25010:2023 biedt een model voor productkwaliteit. De standaard biedt geen concrete maatregelen, maar biedt wel een begrippenkader en dekt het volledige spectrum van mogelijk relevante kwaliteitseigenschappen af. Het gebruiken van een standaard voor specificatie van kwaliteit voorkomt miscommunicatie over kwaliteitseigenschappen en de breedte van de standaard zorgt ervoor dat alle relevante aspecten aan bod komen.
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B41" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Courier"/>
-            <family val="2"/>
-          </rPr>
           <t xml:space="preserve">M04: Het project borgt de correcte werking van het product met geautomatiseerde regressietests
 Regressietests - tests die verifiëren of eerder ontwikkelde software nog steeds correct werkt na wijzigingen in de software of aansluiting op andere externe koppelvlakken - zijn geautomatiseerd.
 Het project hanteert een norm voor de dekking van regressietests, legt deze vast in Quality-time en bewaakt deze.
@@ -317,7 +299,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B42" authorId="0">
+    <comment ref="B41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -346,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C42" authorId="0">
+    <comment ref="C41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -359,7 +341,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B52" authorId="0">
+    <comment ref="B51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -396,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C52" authorId="0">
+    <comment ref="C51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -409,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="0">
+    <comment ref="B69" authorId="0">
       <text>
         <r>
           <rPr>
@@ -429,7 +411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B70" authorId="0">
       <text>
         <r>
           <rPr>
@@ -451,7 +433,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -472,7 +454,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B73" authorId="0">
       <text>
         <r>
           <rPr>
@@ -489,7 +471,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -506,7 +488,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -529,7 +511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C76" authorId="0">
+    <comment ref="C75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -542,7 +524,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="0">
+    <comment ref="B80" authorId="0">
       <text>
         <r>
           <rPr>
@@ -563,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B81" authorId="0">
       <text>
         <r>
           <rPr>
@@ -588,7 +570,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -615,7 +597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -633,7 +615,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -665,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C85" authorId="0">
+    <comment ref="C84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -678,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0">
+    <comment ref="B99" authorId="0">
       <text>
         <r>
           <rPr>
@@ -698,7 +680,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B102" authorId="0">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -718,7 +700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B102" authorId="0">
       <text>
         <r>
           <rPr>
@@ -737,7 +719,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -758,7 +740,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -777,7 +759,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -795,7 +777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -826,7 +808,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="137">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-03-2025.</t>
   </si>
@@ -964,12 +946,6 @@
   </si>
   <si>
     <t>Het project zorgt dat het product traceerbaar aan eisen voldoet</t>
-  </si>
-  <si>
-    <t>M13</t>
-  </si>
-  <si>
-    <t>Het project gebruikt ISO-25010 voor de specificatie van productkwaliteitseisen</t>
   </si>
   <si>
     <t>M04</t>
@@ -1684,7 +1660,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2042,23 +2018,21 @@
       <c r="B41" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C41" s="8"/>
+      <c r="C41" s="4"/>
       <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B42" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C42" s="4"/>
+      <c r="C42" s="7"/>
       <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="6"/>
       <c r="B43" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="7"/>
       <c r="D43" s="5"/>
@@ -2066,7 +2040,7 @@
     <row r="44" spans="1:4">
       <c r="A44" s="6"/>
       <c r="B44" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="7"/>
       <c r="D44" s="5"/>
@@ -2074,7 +2048,7 @@
     <row r="45" spans="1:4">
       <c r="A45" s="6"/>
       <c r="B45" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C45" s="7"/>
       <c r="D45" s="5"/>
@@ -2082,7 +2056,7 @@
     <row r="46" spans="1:4">
       <c r="A46" s="6"/>
       <c r="B46" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="5"/>
@@ -2090,7 +2064,7 @@
     <row r="47" spans="1:4">
       <c r="A47" s="6"/>
       <c r="B47" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C47" s="7"/>
       <c r="D47" s="5"/>
@@ -2098,7 +2072,7 @@
     <row r="48" spans="1:4">
       <c r="A48" s="6"/>
       <c r="B48" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C48" s="7"/>
       <c r="D48" s="5"/>
@@ -2106,7 +2080,7 @@
     <row r="49" spans="1:4">
       <c r="A49" s="6"/>
       <c r="B49" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C49" s="7"/>
       <c r="D49" s="5"/>
@@ -2114,33 +2088,33 @@
     <row r="50" spans="1:4">
       <c r="A50" s="6"/>
       <c r="B50" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C50" s="7"/>
       <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="6"/>
-      <c r="B51" s="6" t="s">
+      <c r="A51" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C51" s="7"/>
+      <c r="C51" s="4"/>
       <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="6"/>
+      <c r="B52" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B52" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C52" s="4"/>
+      <c r="C52" s="7"/>
       <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="6"/>
       <c r="B53" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C53" s="7"/>
       <c r="D53" s="5"/>
@@ -2148,7 +2122,7 @@
     <row r="54" spans="1:4">
       <c r="A54" s="6"/>
       <c r="B54" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C54" s="7"/>
       <c r="D54" s="5"/>
@@ -2156,7 +2130,7 @@
     <row r="55" spans="1:4">
       <c r="A55" s="6"/>
       <c r="B55" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C55" s="7"/>
       <c r="D55" s="5"/>
@@ -2164,7 +2138,7 @@
     <row r="56" spans="1:4">
       <c r="A56" s="6"/>
       <c r="B56" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C56" s="7"/>
       <c r="D56" s="5"/>
@@ -2172,7 +2146,7 @@
     <row r="57" spans="1:4">
       <c r="A57" s="6"/>
       <c r="B57" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C57" s="7"/>
       <c r="D57" s="5"/>
@@ -2180,7 +2154,7 @@
     <row r="58" spans="1:4">
       <c r="A58" s="6"/>
       <c r="B58" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C58" s="7"/>
       <c r="D58" s="5"/>
@@ -2188,7 +2162,7 @@
     <row r="59" spans="1:4">
       <c r="A59" s="6"/>
       <c r="B59" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C59" s="7"/>
       <c r="D59" s="5"/>
@@ -2196,7 +2170,7 @@
     <row r="60" spans="1:4">
       <c r="A60" s="6"/>
       <c r="B60" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C60" s="7"/>
       <c r="D60" s="5"/>
@@ -2204,7 +2178,7 @@
     <row r="61" spans="1:4">
       <c r="A61" s="6"/>
       <c r="B61" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C61" s="7"/>
       <c r="D61" s="5"/>
@@ -2212,7 +2186,7 @@
     <row r="62" spans="1:4">
       <c r="A62" s="6"/>
       <c r="B62" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C62" s="7"/>
       <c r="D62" s="5"/>
@@ -2220,7 +2194,7 @@
     <row r="63" spans="1:4">
       <c r="A63" s="6"/>
       <c r="B63" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C63" s="7"/>
       <c r="D63" s="5"/>
@@ -2228,7 +2202,7 @@
     <row r="64" spans="1:4">
       <c r="A64" s="6"/>
       <c r="B64" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C64" s="7"/>
       <c r="D64" s="5"/>
@@ -2236,7 +2210,7 @@
     <row r="65" spans="1:4">
       <c r="A65" s="6"/>
       <c r="B65" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C65" s="7"/>
       <c r="D65" s="5"/>
@@ -2244,7 +2218,7 @@
     <row r="66" spans="1:4">
       <c r="A66" s="6"/>
       <c r="B66" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C66" s="7"/>
       <c r="D66" s="5"/>
@@ -2252,7 +2226,7 @@
     <row r="67" spans="1:4">
       <c r="A67" s="6"/>
       <c r="B67" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C67" s="7"/>
       <c r="D67" s="5"/>
@@ -2260,17 +2234,19 @@
     <row r="68" spans="1:4">
       <c r="A68" s="6"/>
       <c r="B68" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C68" s="7"/>
       <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4">
-      <c r="A69" s="6"/>
-      <c r="B69" s="6" t="s">
+      <c r="A69" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C69" s="7"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
@@ -2284,22 +2260,22 @@
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
-      <c r="A71" s="3" t="s">
+      <c r="A71" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B71" s="4" t="s">
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C71" s="8"/>
-      <c r="D71" s="5"/>
-    </row>
-    <row r="72" spans="1:4">
-      <c r="A72" s="1" t="s">
+      <c r="B72" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
@@ -2328,23 +2304,21 @@
       <c r="B75" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="C75" s="8"/>
+      <c r="C75" s="4"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
-      <c r="A76" s="3" t="s">
+      <c r="A76" s="6"/>
+      <c r="B76" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B76" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C76" s="4"/>
+      <c r="C76" s="7"/>
       <c r="D76" s="5"/>
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="6"/>
       <c r="B77" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C77" s="7"/>
       <c r="D77" s="5"/>
@@ -2352,7 +2326,7 @@
     <row r="78" spans="1:4">
       <c r="A78" s="6"/>
       <c r="B78" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C78" s="7"/>
       <c r="D78" s="5"/>
@@ -2360,17 +2334,19 @@
     <row r="79" spans="1:4">
       <c r="A79" s="6"/>
       <c r="B79" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C79" s="7"/>
       <c r="D79" s="5"/>
     </row>
     <row r="80" spans="1:4">
-      <c r="A80" s="6"/>
-      <c r="B80" s="6" t="s">
+      <c r="A80" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="C80" s="7"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
@@ -2410,23 +2386,21 @@
       <c r="B84" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="C84" s="8"/>
+      <c r="C84" s="4"/>
       <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="3" t="s">
+      <c r="A85" s="6"/>
+      <c r="B85" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="B85" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="C85" s="4"/>
+      <c r="C85" s="7"/>
       <c r="D85" s="5"/>
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="6"/>
       <c r="B86" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C86" s="7"/>
       <c r="D86" s="5"/>
@@ -2434,7 +2408,7 @@
     <row r="87" spans="1:4">
       <c r="A87" s="6"/>
       <c r="B87" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C87" s="7"/>
       <c r="D87" s="5"/>
@@ -2442,7 +2416,7 @@
     <row r="88" spans="1:4">
       <c r="A88" s="6"/>
       <c r="B88" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C88" s="7"/>
       <c r="D88" s="5"/>
@@ -2450,7 +2424,7 @@
     <row r="89" spans="1:4">
       <c r="A89" s="6"/>
       <c r="B89" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C89" s="7"/>
       <c r="D89" s="5"/>
@@ -2458,7 +2432,7 @@
     <row r="90" spans="1:4">
       <c r="A90" s="6"/>
       <c r="B90" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C90" s="7"/>
       <c r="D90" s="5"/>
@@ -2466,7 +2440,7 @@
     <row r="91" spans="1:4">
       <c r="A91" s="6"/>
       <c r="B91" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C91" s="7"/>
       <c r="D91" s="5"/>
@@ -2474,7 +2448,7 @@
     <row r="92" spans="1:4">
       <c r="A92" s="6"/>
       <c r="B92" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="5"/>
@@ -2482,7 +2456,7 @@
     <row r="93" spans="1:4">
       <c r="A93" s="6"/>
       <c r="B93" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C93" s="7"/>
       <c r="D93" s="5"/>
@@ -2490,7 +2464,7 @@
     <row r="94" spans="1:4">
       <c r="A94" s="6"/>
       <c r="B94" s="6" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C94" s="7"/>
       <c r="D94" s="5"/>
@@ -2498,7 +2472,7 @@
     <row r="95" spans="1:4">
       <c r="A95" s="6"/>
       <c r="B95" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C95" s="7"/>
       <c r="D95" s="5"/>
@@ -2506,7 +2480,7 @@
     <row r="96" spans="1:4">
       <c r="A96" s="6"/>
       <c r="B96" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C96" s="7"/>
       <c r="D96" s="5"/>
@@ -2514,7 +2488,7 @@
     <row r="97" spans="1:4">
       <c r="A97" s="6"/>
       <c r="B97" s="6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C97" s="7"/>
       <c r="D97" s="5"/>
@@ -2522,36 +2496,38 @@
     <row r="98" spans="1:4">
       <c r="A98" s="6"/>
       <c r="B98" s="6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C98" s="7"/>
       <c r="D98" s="5"/>
     </row>
     <row r="99" spans="1:4">
-      <c r="A99" s="6"/>
-      <c r="B99" s="6" t="s">
+      <c r="A99" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B99" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C99" s="7"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+      <c r="D100" s="1"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="5"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1" t="s">
+      <c r="B101" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="5"/>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
@@ -2602,16 +2578,6 @@
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="5"/>
-    </row>
-    <row r="107" spans="1:4">
-      <c r="A107" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="C107" s="8"/>
-      <c r="D107" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2634,7 +2600,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C100">
+  <conditionalFormatting sqref="C101">
     <cfRule type="cellIs" dxfId="0" priority="341" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2718,20 +2684,6 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C107">
-    <cfRule type="cellIs" dxfId="0" priority="365" operator="equal">
-      <formula>"voldoet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="366" operator="equal">
-      <formula>"voldoet deels"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="367" operator="equal">
-      <formula>"voldoet niet"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="368" operator="equal">
-      <formula>"niet van toepassing"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3124,7 +3076,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41">
+  <conditionalFormatting sqref="C42">
     <cfRule type="cellIs" dxfId="0" priority="125" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3250,7 +3202,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C51">
+  <conditionalFormatting sqref="C52">
     <cfRule type="cellIs" dxfId="0" priority="161" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3516,7 +3468,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
+  <conditionalFormatting sqref="C72">
     <cfRule type="cellIs" dxfId="0" priority="237" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3558,7 +3510,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C75">
+  <conditionalFormatting sqref="C76">
     <cfRule type="cellIs" dxfId="0" priority="249" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3684,7 +3636,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C84">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="281" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3908,7 +3860,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="92">
+  <dataValidations count="91">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4002,7 +3954,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C40">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C41">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C42">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C43">
@@ -4029,7 +3981,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C50">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C52">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C53">
@@ -4086,7 +4038,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C70">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C72">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C73">
@@ -4095,7 +4047,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77">
@@ -4119,7 +4071,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C83">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
@@ -4164,7 +4116,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C99">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
@@ -4180,9 +4132,6 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C106">
-      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4191,31 +4140,30 @@
     <hyperlink ref="A28" r:id="rId2" location="m32"/>
     <hyperlink ref="A32" r:id="rId3" location="m02"/>
     <hyperlink ref="A39" r:id="rId4" location="m03"/>
-    <hyperlink ref="A40" r:id="rId5" location="m13"/>
-    <hyperlink ref="A41" r:id="rId6" location="m04"/>
-    <hyperlink ref="A42" r:id="rId7" location="m07"/>
-    <hyperlink ref="A52" r:id="rId8" location="m16"/>
-    <hyperlink ref="A70" r:id="rId9" location="m08"/>
-    <hyperlink ref="A71" r:id="rId10" location="m26"/>
-    <hyperlink ref="A73" r:id="rId11" location="m14"/>
-    <hyperlink ref="A74" r:id="rId12" location="m21"/>
-    <hyperlink ref="A75" r:id="rId13" location="m23"/>
-    <hyperlink ref="A76" r:id="rId14" location="m05"/>
-    <hyperlink ref="A81" r:id="rId15" location="m35"/>
-    <hyperlink ref="A82" r:id="rId16" location="m10"/>
-    <hyperlink ref="A83" r:id="rId17" location="m28"/>
-    <hyperlink ref="A84" r:id="rId18" location="m30"/>
-    <hyperlink ref="A85" r:id="rId19" location="m34"/>
-    <hyperlink ref="A100" r:id="rId20" location="m27"/>
-    <hyperlink ref="A102" r:id="rId21" location="m29"/>
-    <hyperlink ref="A103" r:id="rId22" location="m19"/>
-    <hyperlink ref="A104" r:id="rId23" location="m18"/>
-    <hyperlink ref="A105" r:id="rId24" location="m11"/>
-    <hyperlink ref="A106" r:id="rId25" location="m12"/>
-    <hyperlink ref="A107" r:id="rId26" location="m33"/>
+    <hyperlink ref="A40" r:id="rId5" location="m04"/>
+    <hyperlink ref="A41" r:id="rId6" location="m07"/>
+    <hyperlink ref="A51" r:id="rId7" location="m16"/>
+    <hyperlink ref="A69" r:id="rId8" location="m08"/>
+    <hyperlink ref="A70" r:id="rId9" location="m26"/>
+    <hyperlink ref="A72" r:id="rId10" location="m14"/>
+    <hyperlink ref="A73" r:id="rId11" location="m21"/>
+    <hyperlink ref="A74" r:id="rId12" location="m23"/>
+    <hyperlink ref="A75" r:id="rId13" location="m05"/>
+    <hyperlink ref="A80" r:id="rId14" location="m35"/>
+    <hyperlink ref="A81" r:id="rId15" location="m10"/>
+    <hyperlink ref="A82" r:id="rId16" location="m28"/>
+    <hyperlink ref="A83" r:id="rId17" location="m30"/>
+    <hyperlink ref="A84" r:id="rId18" location="m34"/>
+    <hyperlink ref="A99" r:id="rId19" location="m27"/>
+    <hyperlink ref="A101" r:id="rId20" location="m29"/>
+    <hyperlink ref="A102" r:id="rId21" location="m19"/>
+    <hyperlink ref="A103" r:id="rId22" location="m18"/>
+    <hyperlink ref="A104" r:id="rId23" location="m11"/>
+    <hyperlink ref="A105" r:id="rId24" location="m12"/>
+    <hyperlink ref="A106" r:id="rId25" location="m33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId27"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
 
@@ -4235,7 +4183,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4243,10 +4191,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Actueel houden externe software.
In maatregel M16 "Het project gebruikt tools voor vastgestelde taken" de taak "actueel houden van externe software" toegevoegd.

Closes #392.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -367,6 +367,7 @@
 Release van software                                                                         Releaseserver in het ontwikkelplatform                                                   
 Maken van testrapportages                                                                    JUnit, Robot Framework, TestNG, of hiermee compatible tools                              
 Maken van kwaliteitsrapportages                                                              Quality-time                                                                             
+Actueel houden van externe software                                                          RenovateBot                                                                              
 Controleren op aanwezigheid van bekende kwetsbaarheden in externe software                   OWASP (Open Web Application Security Project) Dependency-Check en/of Dependency-Track    
 Statische controle van de software op aanwezigheid van kwetsbare constructies                SonarQube                                                                                
 Dynamische controle van de software op aanwezigheid van kwetsbare constructies               ZAP (Zed Attack Proxy) by Checkmarx                                                      
@@ -397,7 +398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B70" authorId="0">
+    <comment ref="B71" authorId="0">
       <text>
         <r>
           <rPr>
@@ -417,7 +418,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B71" authorId="0">
+    <comment ref="B72" authorId="0">
       <text>
         <r>
           <rPr>
@@ -439,7 +440,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B73" authorId="0">
+    <comment ref="B74" authorId="0">
       <text>
         <r>
           <rPr>
@@ -460,7 +461,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B74" authorId="0">
+    <comment ref="B75" authorId="0">
       <text>
         <r>
           <rPr>
@@ -477,7 +478,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B75" authorId="0">
+    <comment ref="B76" authorId="0">
       <text>
         <r>
           <rPr>
@@ -494,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B76" authorId="0">
+    <comment ref="B77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -517,7 +518,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C76" authorId="0">
+    <comment ref="C77" authorId="0">
       <text>
         <r>
           <rPr>
@@ -530,7 +531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="0">
+    <comment ref="B82" authorId="0">
       <text>
         <r>
           <rPr>
@@ -551,7 +552,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B82" authorId="0">
+    <comment ref="B83" authorId="0">
       <text>
         <r>
           <rPr>
@@ -576,7 +577,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B83" authorId="0">
+    <comment ref="B84" authorId="0">
       <text>
         <r>
           <rPr>
@@ -603,7 +604,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B84" authorId="0">
+    <comment ref="B85" authorId="0">
       <text>
         <r>
           <rPr>
@@ -621,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B85" authorId="0">
+    <comment ref="B86" authorId="0">
       <text>
         <r>
           <rPr>
@@ -653,7 +654,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C85" authorId="0">
+    <comment ref="C86" authorId="0">
       <text>
         <r>
           <rPr>
@@ -666,7 +667,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B100" authorId="0">
+    <comment ref="B101" authorId="0">
       <text>
         <r>
           <rPr>
@@ -686,7 +687,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B102" authorId="0">
+    <comment ref="B103" authorId="0">
       <text>
         <r>
           <rPr>
@@ -706,7 +707,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B103" authorId="0">
+    <comment ref="B104" authorId="0">
       <text>
         <r>
           <rPr>
@@ -725,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B104" authorId="0">
+    <comment ref="B105" authorId="0">
       <text>
         <r>
           <rPr>
@@ -746,7 +747,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B105" authorId="0">
+    <comment ref="B106" authorId="0">
       <text>
         <r>
           <rPr>
@@ -765,7 +766,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B106" authorId="0">
+    <comment ref="B107" authorId="0">
       <text>
         <r>
           <rPr>
@@ -783,7 +784,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B107" authorId="0">
+    <comment ref="B108" authorId="0">
       <text>
         <r>
           <rPr>
@@ -814,7 +815,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="139">
   <si>
     <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 11-04-2025.</t>
   </si>
@@ -1023,34 +1024,37 @@
     <t>7. Maken van kwaliteitsrapportages</t>
   </si>
   <si>
-    <t>8. Controleren op aanwezigheid van bekende kwetsbaarheden in externe software</t>
-  </si>
-  <si>
-    <t>9. Statische controle van de software op aanwezigheid van kwetsbare constructies</t>
-  </si>
-  <si>
-    <t>10. Dynamische controle van de software op aanwezigheid van kwetsbare constructies</t>
-  </si>
-  <si>
-    <t>11. Controleren van container images op aanwezigheid van bekende kwetsbaarheden</t>
-  </si>
-  <si>
-    <t>12. Testen van performance en schaalbaarheid</t>
-  </si>
-  <si>
-    <t>13. Testen op toegankelijkheid van de applicatie</t>
-  </si>
-  <si>
-    <t>14. Produceren van een "software bill of materials" (SBoM)</t>
-  </si>
-  <si>
-    <t>15. Opslaan van artifacten</t>
-  </si>
-  <si>
-    <t>16. Registratie van incidenten bij gebruik en beheer</t>
-  </si>
-  <si>
-    <t>17. Bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving</t>
+    <t>8. Actueel houden van externe software</t>
+  </si>
+  <si>
+    <t>9. Controleren op aanwezigheid van bekende kwetsbaarheden in externe software</t>
+  </si>
+  <si>
+    <t>10. Statische controle van de software op aanwezigheid van kwetsbare constructies</t>
+  </si>
+  <si>
+    <t>11. Dynamische controle van de software op aanwezigheid van kwetsbare constructies</t>
+  </si>
+  <si>
+    <t>12. Controleren van container images op aanwezigheid van bekende kwetsbaarheden</t>
+  </si>
+  <si>
+    <t>13. Testen van performance en schaalbaarheid</t>
+  </si>
+  <si>
+    <t>14. Testen op toegankelijkheid van de applicatie</t>
+  </si>
+  <si>
+    <t>15. Produceren van een "software bill of materials" (SBoM)</t>
+  </si>
+  <si>
+    <t>16. Opslaan van artifacten</t>
+  </si>
+  <si>
+    <t>17. Registratie van incidenten bij gebruik en beheer</t>
+  </si>
+  <si>
+    <t>18. Bij het uitvoeren van operationeel beheer; uitrollen van de software in de productieomgeving</t>
   </si>
   <si>
     <t>M08</t>
@@ -1669,7 +1673,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
@@ -2257,79 +2261,79 @@
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
-      <c r="A70" s="3" t="s">
+      <c r="A70" s="6"/>
+      <c r="B70" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B70" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C70" s="8"/>
+      <c r="C70" s="7"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B71" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>82</v>
       </c>
       <c r="C71" s="8"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B72" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="1"/>
-      <c r="D72" s="1"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:4">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B73" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C73" s="8"/>
-      <c r="D73" s="5"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B74" s="4" t="s">
         <v>86</v>
-      </c>
-      <c r="B74" s="4" t="s">
-        <v>87</v>
       </c>
       <c r="C74" s="8"/>
       <c r="D74" s="5"/>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B75" s="4" t="s">
         <v>88</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="C75" s="8"/>
       <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="C76" s="8"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C76" s="4"/>
-      <c r="D76" s="5"/>
-    </row>
-    <row r="77" spans="1:4">
-      <c r="A77" s="6"/>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="C77" s="7"/>
+      <c r="C77" s="4"/>
       <c r="D77" s="5"/>
     </row>
     <row r="78" spans="1:4">
@@ -2357,61 +2361,61 @@
       <c r="D80" s="5"/>
     </row>
     <row r="81" spans="1:4">
-      <c r="A81" s="3" t="s">
+      <c r="A81" s="6"/>
+      <c r="B81" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="8"/>
+      <c r="C81" s="7"/>
       <c r="D81" s="5"/>
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B82" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="B82" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="C82" s="8"/>
       <c r="D82" s="5"/>
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B83" s="4" t="s">
         <v>100</v>
-      </c>
-      <c r="B83" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="C83" s="8"/>
       <c r="D83" s="5"/>
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B84" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="B84" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="C84" s="8"/>
       <c r="D84" s="5"/>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B85" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="C85" s="8"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C85" s="4"/>
-      <c r="D85" s="5"/>
-    </row>
-    <row r="86" spans="1:4">
-      <c r="A86" s="6"/>
-      <c r="B86" s="6" t="s">
+      <c r="B86" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="C86" s="7"/>
+      <c r="C86" s="4"/>
       <c r="D86" s="5"/>
     </row>
     <row r="87" spans="1:4">
@@ -2519,82 +2523,90 @@
       <c r="D99" s="5"/>
     </row>
     <row r="100" spans="1:4">
-      <c r="A100" s="3" t="s">
+      <c r="A100" s="6"/>
+      <c r="B100" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="B100" s="4" t="s">
+      <c r="C100" s="7"/>
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C100" s="8"/>
-      <c r="D100" s="5"/>
-    </row>
-    <row r="101" spans="1:4">
-      <c r="A101" s="1" t="s">
+      <c r="B101" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B101" s="1"/>
-      <c r="C101" s="1"/>
-      <c r="D101" s="1"/>
+      <c r="C101" s="8"/>
+      <c r="D101" s="5"/>
     </row>
     <row r="102" spans="1:4">
-      <c r="A102" s="3" t="s">
+      <c r="A102" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="B102" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C102" s="8"/>
-      <c r="D102" s="5"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B103" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="B103" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="C103" s="8"/>
       <c r="D103" s="5"/>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B104" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="B104" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="C104" s="8"/>
       <c r="D104" s="5"/>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B105" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="B105" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="C105" s="8"/>
       <c r="D105" s="5"/>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="B106" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="C106" s="8"/>
       <c r="D106" s="5"/>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B107" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="B107" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="C107" s="8"/>
       <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="1:4">
+      <c r="A108" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C108" s="8"/>
+      <c r="D108" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2631,7 +2643,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C102">
+  <conditionalFormatting sqref="C101">
     <cfRule type="cellIs" dxfId="0" priority="345" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -2715,6 +2727,20 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C108">
+    <cfRule type="cellIs" dxfId="0" priority="369" operator="equal">
+      <formula>"voldoet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="370" operator="equal">
+      <formula>"voldoet deels"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="371" operator="equal">
+      <formula>"voldoet niet"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="372" operator="equal">
+      <formula>"niet van toepassing"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C11">
     <cfRule type="cellIs" dxfId="0" priority="13" operator="equal">
       <formula>"voldoet"</formula>
@@ -3513,7 +3539,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C73">
+  <conditionalFormatting sqref="C72">
     <cfRule type="cellIs" dxfId="0" priority="241" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3555,7 +3581,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C77">
+  <conditionalFormatting sqref="C76">
     <cfRule type="cellIs" dxfId="0" priority="253" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3681,7 +3707,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C86">
+  <conditionalFormatting sqref="C85">
     <cfRule type="cellIs" dxfId="0" priority="285" operator="equal">
       <formula>"voldoet"</formula>
     </cfRule>
@@ -3891,7 +3917,7 @@
       <formula>"niet van toepassing"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="92">
+  <dataValidations count="93">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
@@ -4072,7 +4098,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C71">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C73">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C72">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C74">
@@ -4081,7 +4107,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C75">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C77">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C76">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C78">
@@ -4105,7 +4131,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C84">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C86">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C85">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C87">
@@ -4150,7 +4176,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C100">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C102">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C101">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C103">
@@ -4166,6 +4192,9 @@
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C107">
+      <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C108">
       <formula1>"voldoet,voldoet deels,voldoet niet,niet van toepassing"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4177,24 +4206,24 @@
     <hyperlink ref="A41" r:id="rId5" location="m04"/>
     <hyperlink ref="A42" r:id="rId6" location="m07"/>
     <hyperlink ref="A52" r:id="rId7" location="m16"/>
-    <hyperlink ref="A70" r:id="rId8" location="m08"/>
-    <hyperlink ref="A71" r:id="rId9" location="m26"/>
-    <hyperlink ref="A73" r:id="rId10" location="m14"/>
-    <hyperlink ref="A74" r:id="rId11" location="m21"/>
-    <hyperlink ref="A75" r:id="rId12" location="m23"/>
-    <hyperlink ref="A76" r:id="rId13" location="m05"/>
-    <hyperlink ref="A81" r:id="rId14" location="m35"/>
-    <hyperlink ref="A82" r:id="rId15" location="m10"/>
-    <hyperlink ref="A83" r:id="rId16" location="m28"/>
-    <hyperlink ref="A84" r:id="rId17" location="m30"/>
-    <hyperlink ref="A85" r:id="rId18" location="m34"/>
-    <hyperlink ref="A100" r:id="rId19" location="m27"/>
-    <hyperlink ref="A102" r:id="rId20" location="m29"/>
-    <hyperlink ref="A103" r:id="rId21" location="m19"/>
-    <hyperlink ref="A104" r:id="rId22" location="m18"/>
-    <hyperlink ref="A105" r:id="rId23" location="m11"/>
-    <hyperlink ref="A106" r:id="rId24" location="m12"/>
-    <hyperlink ref="A107" r:id="rId25" location="m33"/>
+    <hyperlink ref="A71" r:id="rId8" location="m08"/>
+    <hyperlink ref="A72" r:id="rId9" location="m26"/>
+    <hyperlink ref="A74" r:id="rId10" location="m14"/>
+    <hyperlink ref="A75" r:id="rId11" location="m21"/>
+    <hyperlink ref="A76" r:id="rId12" location="m23"/>
+    <hyperlink ref="A77" r:id="rId13" location="m05"/>
+    <hyperlink ref="A82" r:id="rId14" location="m35"/>
+    <hyperlink ref="A83" r:id="rId15" location="m10"/>
+    <hyperlink ref="A84" r:id="rId16" location="m28"/>
+    <hyperlink ref="A85" r:id="rId17" location="m30"/>
+    <hyperlink ref="A86" r:id="rId18" location="m34"/>
+    <hyperlink ref="A101" r:id="rId19" location="m27"/>
+    <hyperlink ref="A103" r:id="rId20" location="m29"/>
+    <hyperlink ref="A104" r:id="rId21" location="m19"/>
+    <hyperlink ref="A105" r:id="rId22" location="m18"/>
+    <hyperlink ref="A106" r:id="rId23" location="m11"/>
+    <hyperlink ref="A107" r:id="rId24" location="m12"/>
+    <hyperlink ref="A108" r:id="rId25" location="m33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId26"/>
@@ -4217,7 +4246,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -4225,10 +4254,10 @@
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Mark measure and submeasure titles in the XML
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -62,6 +62,7 @@
 Als een DPIA niet nodig is, dan is een verklaring daaromtrent vereist.
 Impact assessment mensenrechten en algoritmes
 Een impact assessment voor mensenrechten bij de inzet van algoritmes is een instrument voor discussie en besluitvorming door overheidsorganen over de ontwikkeling en/of inzet van een algoritmisch systeem. Met een dergelijke impact assessment kan een interdisciplinaire dialoog gevoerd worden tussen relevante partijen bij de afweging om wel of niet een algoritmische toepassing te gaan ontwikkelen. En het helpt om de gekozen ontwikkeling en implementatie vervolgens op een verantwoorde manier te doen. In het IAMA worden verbanden gelegd met relevante regels, instrumenten en toetskaders op het gebied van algoritmen.
+Een IAMA wordt ingezet in alle gevallen waarin een overheidsorgaan overweegt een algoritme te (laten) ontwikkelen, in te kopen, aan te passen en/of in te gaan zetten.
 Zie https://www.rijksoverheid.nl/documenten/rapporten/2021/02/25/impact-assessment-mensenrechten-en-algoritmes.
 Voor meer informatie over het gezamenlijk gebruik van IAMA en DPIA, zie https://www.cip-overheid.nl/media/av0dmahv/20230614-gezamenlijk-gebruik-iama-en-model-dpia-rijksdienst-v1-0.pdf.
 Projectstartarchitectuur en solution architectuur
@@ -226,11 +227,11 @@
 Projecten bewaken zo snel mogelijk vanaf de start de door het project en ICTU vastgestelde kwaliteitsnormen en voldoen daar zo snel en goed mogelijk aan. De kwaliteit van producten, die nog niet zijn afgerond of nog niet aan de normen voldoen, wordt door het project bewaakt. Het voldoen aan de kwaliteitsnormen is onderdeel van de Definition of Done en herstel van de kwaliteit wordt planmatig opgepakt.
 De kwaliteitsnormen voor het product zijn beschreven in de niet-functionele eisen, het informatiebeveiligingsplan, het kwaliteitsplan en deze Kwaliteitsaanpak, zie M01: Het project ontvangt en levert in elke fase vastgestelde producten en informatie.
 Om continu te bewaken dat het product aan de kwaliteitsnormen voldoet, voert het project de volgende activiteiten uit:
-1. Tijdens de voorfase: het project reviewt de deliverables periodiek.
-2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software.
-3. Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.
-4. Tijdens de realisatiefase: het project evalueert periodiek en handmatig de kwaliteitseigenschappen van de software die niet geautomatiseerd kunnen worden gemeten.
-5. Tijdens de realisatiefase: het project actualiseert en reviewt periodiek de documentatie.
+1. Tijdens de voorfase: het project reviewt de deliverables periodiek,
+2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software,
+3. Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer,
+4. Tijdens de realisatiefase: het project evalueert periodiek en handmatig de kwaliteitseigenschappen van de software die niet geautomatiseerd kunnen worden gemeten,
+5. Tijdens de realisatiefase: het project actualiseert en reviewt periodiek de documentatie,
 6. Indien nodig: de kwaliteitsmanager escaleert het langdurig niet halen van de kwaliteitsnormen.
 Daarnaast voert het project periodiek een self-assessment uit tegen de actuele versie van de Kwaliteitsaanpak, zie M28: Het project voert periodiek een self-assessment uit tegen de actuele versie van de Kwaliteitsaanpak.
 Voorfase: review documenten
@@ -487,9 +488,9 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">M23: Het project zorgt voor de aanwezigheid van kennis van en ervaring met de Kwaliteitsaanpak
-De software delivery manager zorgt ervoor dat bij nieuwe projecten wordt gestart met ten minste twee projectleden die bekend zijn met de Kwaliteitsaanpak. Projectleden die nog niet bekend zijn met de Kwaliteitsaanpak krijgen uitleg over de inhoud en achtergrond van de Kwaliteitsaanpak.
+De software delivery manager zorgt ervoor dat bij nieuwe projecten wordt gestart met ten minste twee projectleden die bekend zijn met de Kwaliteitsaanpak. Projectleden, inclusief projectleider, die nog niet bekend zijn met de Kwaliteitsaanpak krijgen uitleg over de inhoud en achtergrond van de Kwaliteitsaanpak.
 Rationale
-Het inzetten van teamleden die bekend zijn met de Kwaliteitsaanpak zorgt voor een soepeler start van een nieuw project omdat zij bekend zijn met de inhoud van de Kwaliteitsaanpak, zoals kwaliteitsnormen en tools, en omdat zij al doende nieuwe teamleden bekend kunnen maken met de Kwaliteitsaanpak.
+Het inzetten van projectleden die bekend zijn met de Kwaliteitsaanpak zorgt voor een soepeler start van een nieuw project omdat zij bekend zijn met de inhoud van de Kwaliteitsaanpak, zoals kwaliteitsnormen en tools, en omdat zij al doende nieuwe projectleden bekend kunnen maken met de Kwaliteitsaanpak.
 </t>
         </r>
       </text>
@@ -642,7 +643,7 @@
 6. De broncode heeft een beperkte mate van duplicatie (6.2),
 7. De broncode heeft een beperkte mate van complexiteit (6.3),
 8. De broncode bevat geen of een beperkt aantal niet-afgeronde werkzaamheden ("todo's") (6.4).
-9. De tests raken een voldoende groot deel van de broncode (code dekking) (7.1),
+9. De tests raken een voldoende groot deel van de broncode (7.1),
 10. De tests raken een voldoende groot deel van de functionaliteit (functionele dekking) (7.2),
 11. De onderkende productrisico's zijn gedekt (7.3),
 12. Er is een regressietest beschikbaar (7.4),
@@ -816,7 +817,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 11-04-2025.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 22-09-2025.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Vul bij maatregelen met submaatregelen alleen de status van de submaatregelen in.</t>
@@ -918,13 +919,13 @@
     <t>Het project onderzoekt de kwaliteit van over te nemen software</t>
   </si>
   <si>
-    <t>1. Een rapportage met tenminste de bevindingen, risico's voor opdrachtgevende organisatie en ICTU, en mitigerende maatregelen,</t>
-  </si>
-  <si>
-    <t>2. Een transitieplan dat de activiteiten beschrijft die nodig zijn om de software af te bouwen of te herbouwen en te onderhouden, en</t>
-  </si>
-  <si>
-    <t>3. Als er significante technische schuld aanwezig is in de bestaande software: een plan voor het aflossen van deze schuld.</t>
+    <t>1. Een rapportage met tenminste de bevindingen, risico's voor opdrachtgevende organisatie en ICTU, en mitigerende maatregelen</t>
+  </si>
+  <si>
+    <t>2. Een transitieplan dat de activiteiten beschrijft die nodig zijn om de software af te bouwen of te herbouwen en te onderhouden</t>
+  </si>
+  <si>
+    <t>3. Als er significante technische schuld aanwezig is in de bestaande software: een plan voor het aflossen van deze schuld</t>
   </si>
   <si>
     <t>M02</t>
@@ -933,22 +934,22 @@
     <t>Het project bewaakt continu dat het product aan de kwaliteitsnormen voldoet</t>
   </si>
   <si>
-    <t>1. Tijdens de voorfase: het project reviewt de deliverables periodiek.</t>
-  </si>
-  <si>
-    <t>2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software.</t>
-  </si>
-  <si>
-    <t>3. Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer.</t>
-  </si>
-  <si>
-    <t>4. Tijdens de realisatiefase: het project evalueert periodiek en handmatig de kwaliteitseigenschappen van de software die niet geautomatiseerd kunnen worden gemeten.</t>
-  </si>
-  <si>
-    <t>5. Tijdens de realisatiefase: het project actualiseert en reviewt periodiek de documentatie.</t>
-  </si>
-  <si>
-    <t>6. Indien nodig: de kwaliteitsmanager escaleert het langdurig niet halen van de kwaliteitsnormen.</t>
+    <t>1. Tijdens de voorfase: het project reviewt de deliverables periodiek</t>
+  </si>
+  <si>
+    <t>2. Tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd de kwaliteit van de software</t>
+  </si>
+  <si>
+    <t>3. Als operationeel beheer onderdeel is van de dienstverlening tijdens de realisatiefase: het project bewaakt op dagelijkse basis en geautomatiseerd het gedrag van de software in gebruik en beheer</t>
+  </si>
+  <si>
+    <t>4. Tijdens de realisatiefase: het project evalueert periodiek en handmatig de kwaliteitseigenschappen van de software die niet geautomatiseerd kunnen worden gemeten</t>
+  </si>
+  <si>
+    <t>5. Tijdens de realisatiefase: het project actualiseert en reviewt periodiek de documentatie</t>
+  </si>
+  <si>
+    <t>6. Indien nodig: de kwaliteitsmanager escaleert het langdurig niet halen van de kwaliteitsnormen</t>
   </si>
   <si>
     <t>M03</t>
@@ -969,31 +970,31 @@
     <t>Het project gebruikt een continuous delivery pipeline om het product te bouwen, testen en op te leveren</t>
   </si>
   <si>
-    <t>1. Bouw van de software,</t>
-  </si>
-  <si>
-    <t>2. Unit tests,</t>
-  </si>
-  <si>
-    <t>3. Regressietests,</t>
-  </si>
-  <si>
-    <t>4. Beveiligingstests,</t>
-  </si>
-  <si>
-    <t>5. Performancetests,</t>
-  </si>
-  <si>
-    <t>6. Toegankelijkheidstests,</t>
-  </si>
-  <si>
-    <t>7. Broncodekwaliteitscontroles,</t>
-  </si>
-  <si>
-    <t>8. Installatie van de software in test, acceptatie en/of productieomgevingen,</t>
-  </si>
-  <si>
-    <t>9. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie.</t>
+    <t>1. Bouw van de software</t>
+  </si>
+  <si>
+    <t>2. Unit tests</t>
+  </si>
+  <si>
+    <t>3. Regressietests</t>
+  </si>
+  <si>
+    <t>4. Beveiligingstests</t>
+  </si>
+  <si>
+    <t>5. Performancetests</t>
+  </si>
+  <si>
+    <t>6. Toegankelijkheidstests</t>
+  </si>
+  <si>
+    <t>7. Broncodekwaliteitscontroles</t>
+  </si>
+  <si>
+    <t>8. Installatie van de software in test, acceptatie en/of productieomgevingen</t>
+  </si>
+  <si>
+    <t>9. Oplevering van het totale product, dus inclusief alle deliverables, in de vorm zoals bruikbaar voor en afgesproken met de opdrachtgevende organisatie</t>
   </si>
   <si>
     <t>M16</t>
@@ -1092,16 +1093,16 @@
     <t>Het project hanteert een iteratief en incrementeel ontwikkelproces</t>
   </si>
   <si>
-    <t>1. Scrumteam bestaand uit product owner, ontwikkelaars (zoals programmeurs, testers en ontwerpers) en Scrummaster,</t>
-  </si>
-  <si>
-    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement,</t>
-  </si>
-  <si>
-    <t>3. Definition of Ready en Definition of Done,</t>
-  </si>
-  <si>
-    <t>4. Product backlog en sprint backlog.</t>
+    <t>1. Scrumteam bestaand uit product owner, ontwikkelaars (zoals programmeurs, testers en ontwerpers) en Scrummaster</t>
+  </si>
+  <si>
+    <t>2. Proces met daily scrum, sprints, sprint planning, sprint review, sprint retrospective en sprint refinement</t>
+  </si>
+  <si>
+    <t>3. Definition of Ready en Definition of Done</t>
+  </si>
+  <si>
+    <t>4. Product backlog en sprint backlog</t>
   </si>
   <si>
     <t>M35</t>
@@ -1134,46 +1135,46 @@
     <t>Het project draagt software beheerst over</t>
   </si>
   <si>
-    <t>1. De documentatie beschrijft de ontwikkel- en testomgeving die is toegepast (5.1),</t>
-  </si>
-  <si>
-    <t>2. De functionele documentatie beschrijft gegevensmodellen, functionele indeling, koppelingen, berichtdefinities en workflows/processen (5.2),</t>
-  </si>
-  <si>
-    <t>3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures (5.3),</t>
-  </si>
-  <si>
-    <t>4. De product backlog bevat de bekende bugs en wensen (5.4),</t>
-  </si>
-  <si>
-    <t>5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling (6.1),</t>
-  </si>
-  <si>
-    <t>6. De broncode heeft een beperkte mate van duplicatie (6.2),</t>
-  </si>
-  <si>
-    <t>7. De broncode heeft een beperkte mate van complexiteit (6.3),</t>
-  </si>
-  <si>
-    <t>8. De broncode bevat geen of een beperkt aantal niet-afgeronde werkzaamheden ("todo's") (6.4).</t>
-  </si>
-  <si>
-    <t>9. De tests raken een voldoende groot deel van de broncode (code dekking) (7.1),</t>
-  </si>
-  <si>
-    <t>10. De tests raken een voldoende groot deel van de functionaliteit (functionele dekking) (7.2),</t>
-  </si>
-  <si>
-    <t>11. De onderkende productrisico's zijn gedekt (7.3),</t>
-  </si>
-  <si>
-    <t>12. Er is een regressietest beschikbaar (7.4),</t>
-  </si>
-  <si>
-    <t>13. Er is traceerbaarheid van eisen naar testgevallen (7.5), en</t>
-  </si>
-  <si>
-    <t>14. De testset is goed opgebouwd (7.6).</t>
+    <t>1. De documentatie beschrijft de ontwikkel- en testomgeving die is toegepast</t>
+  </si>
+  <si>
+    <t>2. De functionele documentatie beschrijft gegevensmodellen, functionele indeling, koppelingen, berichtdefinities en workflows/processen</t>
+  </si>
+  <si>
+    <t>3. Als operationeel beheer onderdeel was van de dienstverlening: de operationele bedieningsinstructies beschrijven minimaal back-up/recovery, procedures bij calamiteiten, regelmatig terugkerende beheeractiviteiten en opstart- en afsluitprocedures</t>
+  </si>
+  <si>
+    <t>4. De product backlog bevat de bekende bugs en wensen</t>
+  </si>
+  <si>
+    <t>5. De broncode kent een gezonde balans tussen isolatie, cohesie en koppeling</t>
+  </si>
+  <si>
+    <t>6. De broncode heeft een beperkte mate van duplicatie</t>
+  </si>
+  <si>
+    <t>7. De broncode heeft een beperkte mate van complexiteit</t>
+  </si>
+  <si>
+    <t>8. De broncode bevat geen of een beperkt aantal niet-afgeronde werkzaamheden ("todo's")</t>
+  </si>
+  <si>
+    <t>9. De tests raken een voldoende groot deel van de broncode</t>
+  </si>
+  <si>
+    <t>10. De tests raken een voldoende groot deel van de functionaliteit (functionele dekking)</t>
+  </si>
+  <si>
+    <t>11. De onderkende productrisico's zijn gedekt</t>
+  </si>
+  <si>
+    <t>12. Er is een regressietest beschikbaar</t>
+  </si>
+  <si>
+    <t>13. Er is traceerbaarheid van eisen naar testgevallen</t>
+  </si>
+  <si>
+    <t>14. De testset is goed opgebouwd</t>
   </si>
   <si>
     <t>M27</t>

</xml_diff>

<commit_message>
Verwijder hoofdstukken "Kaders" uit templates
Closes #1033.
</commit_message>
<xml_diff>
--- a/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
+++ b/docs/wip/ICTU-Kwaliteitsaanpak-Checklist.xlsx
@@ -98,7 +98,8 @@
 - methode Grip op SDD (Secure Software Development) van het Centrum Informatiebeveiliging en Privacybescherming (CIP),
 - Algemene verordening gegevensbescherming (AVG),
 - ISO 9241-210:2019 Ergonomics of human-system interaction - Part 210: Human-centred design for interactive systems,
-- Web Content Accessibility Guidelines versie 2.2, niveau A en AA. Hiermee wordt invulling gegeven aan hoofdstuk 9 van de Europese Standaard EN 301 549 die verwijst naar WCAG versie 2.1.
+- Web Content Accessibility Guidelines versie 2.2, niveau A en AA. Hiermee wordt invulling gegeven aan hoofdstuk 9 van de Europese Standaard EN 301 549 die verwijst naar WCAG versie 2.1,
+- Indien van toepassing: NEN 7510-2:2024 Informatiebeveiliging in de zorg - Deel 2: Beheersmaatregelen.
 De beschrijving van niet-functionele eisen moet expliciet aandacht besteden aan de door de beoogd beheerder gewenste ondersteuning van beheerfuncties. Bepaalde niet-functionele eisen kunnen aanleiding zijn tot het treffen van beveiligingsmaatregelen. Door deze eisen expliciet in de voorfase te benoemen, wordt voorkomen dat de bijbehorende beveiligingsmaatregelen achteraf moeten worden toegevoegd.
 Overheidsorganisaties moeten een toegankelijkheidsverklaring op hun websites plaatsen. Indien gewenst ondersteunt ICTU bij het opstellen van de toegankelijkheidsverklaring.
 Bronnen van de opdrachtgevende organisatie zoals procesbeschrijvingen, data protection impact assessment (DPIA), beheeracceptatiecriteria, beveiligingsbeleid en projectstartarchitectuur vormen het startpunt voor de niet-functionele eisen.
@@ -817,7 +818,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="138">
   <si>
-    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 24-12-2025.</t>
+    <t>Onderstaande checklist kan gebruikt worden voor het uitvoeren van een assessment tegen de ICTU Kwaliteitsaanpak Softwareontwikkeling versie wip, 05-01-2026.</t>
   </si>
   <si>
     <t>Gebruik de 'Status' kolom om aan te geven in hoeverre een maatregel uit de Kwaliteitsaanpak is toegepast. Vul bij maatregelen met submaatregelen alleen de status van de submaatregelen in.</t>

</xml_diff>